<commit_message>
Work on codegen FMKCPU/ FMKIO + interruptLine Managed
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\fModuleCan\Doc\ConfigPrj\ExcelCfg\STM32F474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB02D3D1-91CE-4E8C-89B4-020E11ADBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8BAA3A-520C-46CA-9E61-E7A8078D0B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="341">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1044,6 +1044,24 @@
   </si>
   <si>
     <t>PA11</t>
+  </si>
+  <si>
+    <t>Interrupt line associate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purpose </t>
+  </si>
+  <si>
+    <t>Timer Purpose</t>
+  </si>
+  <si>
+    <t>PWM/IC/OC/OP</t>
+  </si>
+  <si>
+    <t>EVENT</t>
+  </si>
+  <si>
+    <t>DAC</t>
   </si>
 </sst>
 </file>
@@ -1118,17 +1136,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:K30" totalsRowShown="0">
-  <autoFilter ref="J18:K30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:M30" totalsRowShown="0">
+  <autoFilter ref="J18:M30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8EBC08AF-F674-4D3F-80D1-664693CE12C7}" name="Timer_name"/>
     <tableColumn id="2" xr3:uid="{9707AE90-9D0C-47B3-A89D-28A13CE83851}" name="Number of channels"/>
+    <tableColumn id="3" xr3:uid="{D8031831-59FD-4378-ADF9-534E59E34124}" name="Interrupt line associate"/>
+    <tableColumn id="4" xr3:uid="{F81B2123-AE73-4BAA-A2DB-915ACD9E2233}" name="Purpose "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}" name="Tableau26" displayName="Tableau26" ref="AD41:AD44" totalsRowShown="0">
+  <autoFilter ref="AD41:AD44" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{41DEADB1-B8AC-4DA1-AAC6-1E2E0AF40D54}" name="Timer Purpose"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:C17" totalsRowShown="0">
   <autoFilter ref="A6:C17" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
   <tableColumns count="3">
@@ -1140,7 +1170,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="AD5:AF14" totalsRowShown="0">
   <autoFilter ref="AD5:AF14" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="3">
@@ -1152,7 +1182,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="K6:P9" totalsRowShown="0">
   <autoFilter ref="K6:P9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="6">
@@ -1167,7 +1197,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}" name="FMKIO_InputEvnt" displayName="FMKIO_InputEvnt" ref="R5:U7" totalsRowShown="0">
   <autoFilter ref="R5:U7" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}"/>
   <tableColumns count="4">
@@ -1180,7 +1210,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="W5:AB13" totalsRowShown="0">
   <autoFilter ref="W5:AB13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="6">
@@ -1195,7 +1225,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:I16" totalsRowShown="0">
   <autoFilter ref="E6:I16" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="5">
@@ -1209,7 +1239,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}" name="Tableau17" displayName="Tableau17" ref="AJ5:AJ21" totalsRowShown="0">
   <autoFilter ref="AJ5:AJ21" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}"/>
   <tableColumns count="1">
@@ -1219,7 +1249,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}" name="Tableau18" displayName="Tableau18" ref="AL6:AL10" totalsRowShown="0">
   <autoFilter ref="AL6:AL10" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}"/>
   <tableColumns count="1">
@@ -1229,7 +1259,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}" name="Tableau1720" displayName="Tableau1720" ref="AN5:AN23" totalsRowShown="0">
   <autoFilter ref="AN5:AN23" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}"/>
   <tableColumns count="1">
@@ -1239,7 +1269,18 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="O33:P40" totalsRowShown="0">
+  <autoFilter ref="O33:P40" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3404615A-1121-4984-AE0D-5A1D34461BCA}" name="GPIO_Name"/>
+    <tableColumn id="2" xr3:uid="{37ECDCD3-2CED-4177-80B2-3A88EFA9E7C2}" name="Number of pin"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}" name="Tableau20" displayName="Tableau20" ref="A25:C28" totalsRowShown="0">
   <autoFilter ref="A25:C28" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}"/>
   <tableColumns count="3">
@@ -1251,18 +1292,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="M18:N25" totalsRowShown="0">
-  <autoFilter ref="M18:N25" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3404615A-1121-4984-AE0D-5A1D34461BCA}" name="GPIO_Name"/>
-    <tableColumn id="2" xr3:uid="{37ECDCD3-2CED-4177-80B2-3A88EFA9E7C2}" name="Number of pin"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}" name="Tableau2022" displayName="Tableau2022" ref="E27:G29" totalsRowShown="0">
   <autoFilter ref="E27:G29" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}"/>
   <tableColumns count="3">
@@ -1274,7 +1304,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}" name="Tableau202223" displayName="Tableau202223" ref="I27:K30" totalsRowShown="0">
   <autoFilter ref="I27:K30" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}"/>
   <tableColumns count="3">
@@ -1286,7 +1316,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="Tableau20222324" displayName="Tableau20222324" ref="M27:O30" totalsRowShown="0">
   <autoFilter ref="M27:O30" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
   <tableColumns count="3">
@@ -1298,7 +1328,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -1309,7 +1339,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
   <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
   <tableColumns count="4">
@@ -1322,7 +1352,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
   <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
@@ -1336,8 +1366,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="P18:Q23" totalsRowShown="0">
-  <autoFilter ref="P18:Q23" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="S36:T41" totalsRowShown="0">
+  <autoFilter ref="S36:T41" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
     <tableColumn id="2" xr3:uid="{20DF5352-4B39-416D-A6E4-D94E56AED1C9}" name="number of channel"/>
@@ -1347,8 +1377,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="S18:T19" totalsRowShown="0">
-  <autoFilter ref="S18:T19" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="V36:W37" totalsRowShown="0">
+  <autoFilter ref="V36:W37" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{73150C50-6B2A-4CD8-A7E6-62C171935AF8}" name="DAC_Name"/>
     <tableColumn id="2" xr3:uid="{EF9B5413-9A3C-4163-8063-C74DAB2D51F7}" name="number of channel"/>
@@ -1380,8 +1410,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="V18:W20" totalsRowShown="0">
-  <autoFilter ref="V18:W20" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="Y36:Z38" totalsRowShown="0">
+  <autoFilter ref="Y36:Z38" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00302DEC-D815-47CE-9380-676FE769FF43}" name="DMA_Name"/>
     <tableColumn id="2" xr3:uid="{2654BB85-F763-4BBA-9124-13A3875B62D0}" name="number of channel"/>
@@ -1391,8 +1421,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AA17:AA20" totalsRowShown="0">
-  <autoFilter ref="AA17:AA20" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AD35:AD38" totalsRowShown="0">
+  <autoFilter ref="AD35:AD38" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
   </tableColumns>
@@ -1727,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="B17:AA119"/>
+  <dimension ref="B18:AD119"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,7 +1775,7 @@
     <col min="8" max="8" width="21.44140625" customWidth="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" customWidth="1"/>
     <col min="14" max="14" width="22.77734375" customWidth="1"/>
     <col min="15" max="15" width="23.44140625" customWidth="1"/>
@@ -1754,14 +1784,10 @@
     <col min="22" max="22" width="18.77734375" customWidth="1"/>
     <col min="23" max="23" width="29.21875" customWidth="1"/>
     <col min="27" max="27" width="24" customWidth="1"/>
+    <col min="30" max="30" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="AA17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>169</v>
       </c>
@@ -1783,35 +1809,14 @@
       <c r="K18" t="s">
         <v>3</v>
       </c>
+      <c r="L18" t="s">
+        <v>335</v>
+      </c>
       <c r="M18" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>18</v>
-      </c>
-      <c r="S18" t="s">
-        <v>19</v>
-      </c>
-      <c r="T18" t="s">
-        <v>18</v>
-      </c>
-      <c r="V18" t="s">
-        <v>23</v>
-      </c>
-      <c r="W18" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>170</v>
       </c>
@@ -1830,35 +1835,14 @@
       <c r="K19">
         <v>4</v>
       </c>
+      <c r="L19" t="s">
+        <v>191</v>
+      </c>
       <c r="M19" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19">
-        <v>16</v>
-      </c>
-      <c r="P19" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19">
-        <v>18</v>
-      </c>
-      <c r="S19" t="s">
-        <v>20</v>
-      </c>
-      <c r="T19" t="s">
-        <v>20</v>
-      </c>
-      <c r="V19" t="s">
-        <v>95</v>
-      </c>
-      <c r="W19">
-        <v>8</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>277</v>
       </c>
@@ -1874,29 +1858,14 @@
       <c r="K20">
         <v>4</v>
       </c>
+      <c r="L20" t="s">
+        <v>194</v>
+      </c>
       <c r="M20" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20">
-        <v>16</v>
-      </c>
-      <c r="P20" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q20">
-        <v>18</v>
-      </c>
-      <c r="V20" t="s">
-        <v>277</v>
-      </c>
-      <c r="W20">
-        <v>8</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>281</v>
       </c>
@@ -1912,20 +1881,14 @@
       <c r="K21">
         <v>4</v>
       </c>
+      <c r="L21" t="s">
+        <v>66</v>
+      </c>
       <c r="M21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21">
-        <v>16</v>
-      </c>
-      <c r="P21" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>282</v>
       </c>
@@ -1941,20 +1904,14 @@
       <c r="K22">
         <v>4</v>
       </c>
+      <c r="L22" t="s">
+        <v>195</v>
+      </c>
       <c r="M22" t="s">
-        <v>14</v>
-      </c>
-      <c r="N22">
-        <v>16</v>
-      </c>
-      <c r="P22" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>283</v>
       </c>
@@ -1970,20 +1927,14 @@
       <c r="K23">
         <v>4</v>
       </c>
+      <c r="L23" t="s">
+        <v>211</v>
+      </c>
       <c r="M23" t="s">
-        <v>308</v>
-      </c>
-      <c r="N23">
-        <v>16</v>
-      </c>
-      <c r="P23" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q23">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>284</v>
       </c>
@@ -1999,14 +1950,14 @@
       <c r="K24">
         <v>1</v>
       </c>
+      <c r="L24" t="s">
+        <v>215</v>
+      </c>
       <c r="M24" t="s">
-        <v>15</v>
-      </c>
-      <c r="N24">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>94</v>
       </c>
@@ -2022,14 +1973,14 @@
       <c r="K25">
         <v>1</v>
       </c>
+      <c r="L25" t="s">
+        <v>216</v>
+      </c>
       <c r="M25" t="s">
-        <v>309</v>
-      </c>
-      <c r="N25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>310</v>
       </c>
@@ -2045,8 +1996,14 @@
       <c r="K26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>204</v>
+      </c>
+      <c r="M26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>93</v>
       </c>
@@ -2062,8 +2019,14 @@
       <c r="K27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>211</v>
+      </c>
+      <c r="M27" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>278</v>
       </c>
@@ -2079,8 +2042,14 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
+        <v>192</v>
+      </c>
+      <c r="M28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>279</v>
       </c>
@@ -2096,8 +2065,14 @@
       <c r="K29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>193</v>
+      </c>
+      <c r="M29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>92</v>
       </c>
@@ -2113,8 +2088,14 @@
       <c r="K30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
+        <v>238</v>
+      </c>
+      <c r="M30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>91</v>
       </c>
@@ -2125,7 +2106,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>90</v>
       </c>
@@ -2136,7 +2117,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>285</v>
       </c>
@@ -2146,8 +2127,14 @@
       <c r="H33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>286</v>
       </c>
@@ -2157,8 +2144,14 @@
       <c r="H34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>11</v>
+      </c>
+      <c r="P34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>276</v>
       </c>
@@ -2168,8 +2161,17 @@
       <c r="H35" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35">
+        <v>16</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>275</v>
       </c>
@@ -2179,8 +2181,35 @@
       <c r="H36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O36" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36">
+        <v>16</v>
+      </c>
+      <c r="S36" t="s">
+        <v>17</v>
+      </c>
+      <c r="T36" t="s">
+        <v>18</v>
+      </c>
+      <c r="V36" t="s">
+        <v>19</v>
+      </c>
+      <c r="W36" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>287</v>
       </c>
@@ -2190,8 +2219,35 @@
       <c r="H37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O37" t="s">
+        <v>14</v>
+      </c>
+      <c r="P37">
+        <v>16</v>
+      </c>
+      <c r="S37" t="s">
+        <v>16</v>
+      </c>
+      <c r="T37">
+        <v>18</v>
+      </c>
+      <c r="V37" t="s">
+        <v>20</v>
+      </c>
+      <c r="W37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z37">
+        <v>8</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>288</v>
       </c>
@@ -2201,8 +2257,29 @@
       <c r="H38" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O38" t="s">
+        <v>308</v>
+      </c>
+      <c r="P38">
+        <v>16</v>
+      </c>
+      <c r="S38" t="s">
+        <v>311</v>
+      </c>
+      <c r="T38">
+        <v>18</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>262</v>
       </c>
@@ -2212,8 +2289,20 @@
       <c r="H39" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O39" t="s">
+        <v>15</v>
+      </c>
+      <c r="P39">
+        <v>16</v>
+      </c>
+      <c r="S39" t="s">
+        <v>312</v>
+      </c>
+      <c r="T39">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>289</v>
       </c>
@@ -2223,8 +2312,20 @@
       <c r="H40" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="O40" t="s">
+        <v>309</v>
+      </c>
+      <c r="P40">
+        <v>11</v>
+      </c>
+      <c r="S40" t="s">
+        <v>313</v>
+      </c>
+      <c r="T40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>290</v>
       </c>
@@ -2234,8 +2335,17 @@
       <c r="H41" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="S41" t="s">
+        <v>314</v>
+      </c>
+      <c r="T41">
+        <v>18</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>274</v>
       </c>
@@ -2245,8 +2355,11 @@
       <c r="H42" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AD42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>82</v>
       </c>
@@ -2256,8 +2369,11 @@
       <c r="H43" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AD43" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="44" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>273</v>
       </c>
@@ -2267,8 +2383,11 @@
       <c r="H44" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AD44" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="45" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>291</v>
       </c>
@@ -2279,7 +2398,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
         <v>272</v>
       </c>
@@ -2290,7 +2409,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>271</v>
       </c>
@@ -2301,7 +2420,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>292</v>
       </c>
@@ -2972,14 +3091,17 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18:H119" xr:uid="{049086B5-6506-4A03-974B-48087CF064BC}">
-      <formula1>$AA$18:$AA$20</formula1>
+      <formula1>$AD$36:$AD$38</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M30" xr:uid="{697CB459-5495-4019-B31C-A222FA50D4B5}">
+      <formula1>$AD$42:$AD$44</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2989,6 +3111,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2997,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4049,13 +4172,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA00DA78-9682-47F8-B701-D35809CE3FB0}">
           <x14:formula1>
-            <xm:f>General_Info!$M$19:$M$24</xm:f>
+            <xm:f>General_Info!$O$34:$O$39</xm:f>
           </x14:formula1>
-          <xm:sqref>K7:K9 A7:A17 E7:E16 AD6:AD14 W6:W13 R6:R7</xm:sqref>
+          <xm:sqref>K7:K9 R6:R7 W6:W13 AD6:AD14 E7:E16 A7:A17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
           <x14:formula1>
-            <xm:f>General_Info!$P$19:$P$23</xm:f>
+            <xm:f>General_Info!$S$37:$S$41</xm:f>
           </x14:formula1>
           <xm:sqref>G6:G16</xm:sqref>
         </x14:dataValidation>
@@ -4117,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
   <dimension ref="I2:V5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4226,13 +4349,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
           <x14:formula1>
-            <xm:f>General_Info!$P$19:$P$23</xm:f>
+            <xm:f>General_Info!$S$37:$S$41</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
           <x14:formula1>
-            <xm:f>General_Info!R19</xm:f>
+            <xm:f>General_Info!U37</xm:f>
           </x14:formula1>
           <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Work On PWM for SMT32G family
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2DA139-9947-4D5E-A936-59BF18D7868C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087912D5-D1C5-485F-9A92-01F79705E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="346">
   <si>
     <t>Colonne1</t>
   </si>
@@ -989,12 +989,6 @@
     <t>GPIO_AF9_TIM15</t>
   </si>
   <si>
-    <t>PE8</t>
-  </si>
-  <si>
-    <t>PE9</t>
-  </si>
-  <si>
     <t>PF12</t>
   </si>
   <si>
@@ -1068,6 +1062,21 @@
   </si>
   <si>
     <t>UART5</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>Registre</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Max Clock Frequency (MHz)</t>
   </si>
 </sst>
 </file>
@@ -1165,6 +1174,17 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00403EF2-391D-4DDF-AB62-FECA73965F51}" name="Tableau27" displayName="Tableau27" ref="A27:B30" totalsRowShown="0">
+  <autoFilter ref="A27:B30" xr:uid="{00403EF2-391D-4DDF-AB62-FECA73965F51}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8DA9BC8A-42CE-4C30-97A8-288FDEAB51D0}" name="Registre"/>
+    <tableColumn id="2" xr3:uid="{B79EB748-2894-4CA2-AF71-1F52E1882F52}" name="Max Clock Frequency (MHz)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:C17" totalsRowShown="0">
   <autoFilter ref="A6:C17" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
   <tableColumns count="3">
@@ -1176,7 +1196,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="AD5:AF14" totalsRowShown="0">
   <autoFilter ref="AD5:AF14" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="3">
@@ -1188,7 +1208,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="K6:P9" totalsRowShown="0">
   <autoFilter ref="K6:P9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="6">
@@ -1203,7 +1223,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}" name="FMKIO_InputEvnt" displayName="FMKIO_InputEvnt" ref="R5:U7" totalsRowShown="0">
   <autoFilter ref="R5:U7" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}"/>
   <tableColumns count="4">
@@ -1216,7 +1236,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="W5:AB13" totalsRowShown="0">
   <autoFilter ref="W5:AB13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="6">
@@ -1231,7 +1251,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:I16" totalsRowShown="0">
   <autoFilter ref="E6:I16" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="5">
@@ -1245,7 +1265,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}" name="Tableau17" displayName="Tableau17" ref="AJ5:AJ21" totalsRowShown="0">
   <autoFilter ref="AJ5:AJ21" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}"/>
   <tableColumns count="1">
@@ -1255,21 +1275,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}" name="Tableau18" displayName="Tableau18" ref="AL6:AL10" totalsRowShown="0">
   <autoFilter ref="AL6:AL10" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DD976920-6FFB-4C96-8085-12D970F3A0A7}" name="Channel_Choice"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}" name="Tableau1720" displayName="Tableau1720" ref="AN5:AN23" totalsRowShown="0">
-  <autoFilter ref="AN5:AN23" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D50D0836-4115-4278-AA16-2E66D5FB62AC}" name="Adc_Channel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1287,6 +1297,16 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}" name="Tableau1720" displayName="Tableau1720" ref="AN5:AN23" totalsRowShown="0">
+  <autoFilter ref="AN5:AN23" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D50D0836-4115-4278-AA16-2E66D5FB62AC}" name="Adc_Channel"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}" name="Tableau20" displayName="Tableau20" ref="A25:C28" totalsRowShown="0">
   <autoFilter ref="A25:C28" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}"/>
   <tableColumns count="3">
@@ -1298,7 +1318,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}" name="Tableau2022" displayName="Tableau2022" ref="E27:G29" totalsRowShown="0">
   <autoFilter ref="E27:G29" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}"/>
   <tableColumns count="3">
@@ -1310,7 +1330,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}" name="Tableau202223" displayName="Tableau202223" ref="I27:K30" totalsRowShown="0">
   <autoFilter ref="I27:K30" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}"/>
   <tableColumns count="3">
@@ -1322,7 +1342,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="Tableau20222324" displayName="Tableau20222324" ref="M27:O30" totalsRowShown="0">
   <autoFilter ref="M27:O30" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
   <tableColumns count="3">
@@ -1334,7 +1354,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -1345,7 +1365,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
   <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
   <tableColumns count="4">
@@ -1358,7 +1378,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
   <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
@@ -1765,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="B16:AD119"/>
+  <dimension ref="A16:AD119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,7 +1822,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="V17" t="s">
         <v>19</v>
       </c>
@@ -1819,7 +1839,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>169</v>
       </c>
@@ -1842,10 +1862,10 @@
         <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="V18" t="s">
         <v>20</v>
@@ -1863,7 +1883,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>170</v>
       </c>
@@ -1886,7 +1906,7 @@
         <v>191</v>
       </c>
       <c r="M19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Y19" t="s">
         <v>277</v>
@@ -1898,7 +1918,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>277</v>
       </c>
@@ -1918,10 +1938,10 @@
         <v>194</v>
       </c>
       <c r="M20" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>281</v>
       </c>
@@ -1941,10 +1961,10 @@
         <v>66</v>
       </c>
       <c r="M21" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>282</v>
       </c>
@@ -1964,13 +1984,13 @@
         <v>195</v>
       </c>
       <c r="M22" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AD22" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>283</v>
       </c>
@@ -1990,13 +2010,13 @@
         <v>211</v>
       </c>
       <c r="M23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AD23" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>284</v>
       </c>
@@ -2016,13 +2036,13 @@
         <v>215</v>
       </c>
       <c r="M24" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AD24" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>94</v>
       </c>
@@ -2042,13 +2062,13 @@
         <v>216</v>
       </c>
       <c r="M25" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AD25" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>308</v>
       </c>
@@ -2068,10 +2088,16 @@
         <v>204</v>
       </c>
       <c r="M26" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" t="s">
+        <v>345</v>
+      </c>
       <c r="D27" t="s">
         <v>93</v>
       </c>
@@ -2091,10 +2117,16 @@
         <v>211</v>
       </c>
       <c r="M27" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>344</v>
+      </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
       <c r="D28" t="s">
         <v>278</v>
       </c>
@@ -2114,10 +2146,16 @@
         <v>192</v>
       </c>
       <c r="M28" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29">
+        <v>170</v>
+      </c>
       <c r="D29" t="s">
         <v>279</v>
       </c>
@@ -2137,10 +2175,10 @@
         <v>193</v>
       </c>
       <c r="M29" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>92</v>
       </c>
@@ -2160,10 +2198,10 @@
         <v>238</v>
       </c>
       <c r="M30" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>91</v>
       </c>
@@ -2174,7 +2212,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>90</v>
       </c>
@@ -2259,10 +2297,10 @@
         <v>18</v>
       </c>
       <c r="U36" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V36" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="4:22" x14ac:dyDescent="0.3">
@@ -2549,7 +2587,7 @@
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G55" t="s">
         <v>68</v>
@@ -2560,7 +2598,7 @@
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G56" t="s">
         <v>69</v>
@@ -3151,7 +3189,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="10">
+  <tableParts count="11">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3162,6 +3200,7 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3171,7 +3210,7 @@
   <dimension ref="A2:AN30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3326,22 +3365,22 @@
         <v>148</v>
       </c>
       <c r="W6" t="s">
-        <v>306</v>
+        <v>13</v>
       </c>
       <c r="X6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y6" t="s">
         <v>49</v>
       </c>
       <c r="Z6" t="s">
-        <v>305</v>
+        <v>5</v>
       </c>
       <c r="AA6" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="AB6" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="AD6" t="s">
         <v>12</v>
@@ -3397,13 +3436,13 @@
         <v>315</v>
       </c>
       <c r="N7" t="s">
-        <v>5</v>
+        <v>303</v>
       </c>
       <c r="O7" t="s">
         <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R7" t="s">
         <v>11</v>
@@ -3418,22 +3457,22 @@
         <v>75</v>
       </c>
       <c r="W7" t="s">
-        <v>306</v>
+        <v>13</v>
       </c>
       <c r="X7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Y7" t="s">
         <v>49</v>
       </c>
       <c r="Z7" t="s">
-        <v>305</v>
+        <v>5</v>
       </c>
       <c r="AA7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AB7" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="AD7" t="s">
         <v>12</v>
@@ -3462,7 +3501,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -3492,10 +3531,10 @@
         <v>5</v>
       </c>
       <c r="O8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="P8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -3513,7 +3552,7 @@
         <v>46</v>
       </c>
       <c r="AB8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD8" t="s">
         <v>13</v>
@@ -3575,7 +3614,7 @@
         <v>102</v>
       </c>
       <c r="P9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W9" t="s">
         <v>15</v>
@@ -3593,7 +3632,7 @@
         <v>47</v>
       </c>
       <c r="AB9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AD9" t="s">
         <v>13</v>
@@ -3655,7 +3694,7 @@
         <v>102</v>
       </c>
       <c r="AB10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
@@ -3717,7 +3756,7 @@
         <v>52</v>
       </c>
       <c r="AB11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AD11" t="s">
         <v>15</v>
@@ -3788,7 +3827,7 @@
         <v>40</v>
       </c>
       <c r="AF12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AJ12" t="s">
         <v>32</v>
@@ -3847,7 +3886,7 @@
         <v>35</v>
       </c>
       <c r="AF13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AJ13" t="s">
         <v>33</v>
@@ -3888,7 +3927,7 @@
         <v>36</v>
       </c>
       <c r="AF14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AJ14" t="s">
         <v>34</v>
@@ -4346,7 +4385,7 @@
         <v>159</v>
       </c>
       <c r="J4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -4358,7 +4397,7 @@
         <v>162</v>
       </c>
       <c r="T4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
@@ -4369,10 +4408,10 @@
     </row>
     <row r="5" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J5" t="s">
         <v>328</v>
-      </c>
-      <c r="J5" t="s">
-        <v>330</v>
       </c>
       <c r="K5" t="s">
         <v>312</v>

</xml_diff>

<commit_message>
PWM on sTM32G OK, use the right AF function
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087912D5-D1C5-485F-9A92-01F79705E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC66E95-EB2E-4A9F-A13C-0C4BECB00FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="349">
   <si>
     <t>Colonne1</t>
   </si>
@@ -188,9 +188,6 @@
     <t>GPIO_IRQN</t>
   </si>
   <si>
-    <t>GPIO_AF0_MCO</t>
-  </si>
-  <si>
     <t>ADC_Used</t>
   </si>
   <si>
@@ -1077,6 +1074,18 @@
   </si>
   <si>
     <t>Max Clock Frequency (MHz)</t>
+  </si>
+  <si>
+    <t>Reference to AlternateFunction Datasheet</t>
+  </si>
+  <si>
+    <t>GPIO_AF2_TIM3</t>
+  </si>
+  <si>
+    <t>GPIO_AF2_TIM20</t>
+  </si>
+  <si>
+    <t>GPIO_AF6_TIM5</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A16:AD119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1828,7 @@
   <sheetData>
     <row r="16" spans="30:30" x14ac:dyDescent="0.3">
       <c r="AD16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
@@ -1836,12 +1845,12 @@
         <v>18</v>
       </c>
       <c r="AD17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -1850,10 +1859,10 @@
         <v>21</v>
       </c>
       <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
         <v>59</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
       </c>
       <c r="J18" t="s">
         <v>2</v>
@@ -1862,10 +1871,10 @@
         <v>3</v>
       </c>
       <c r="L18" t="s">
+        <v>330</v>
+      </c>
+      <c r="M18" t="s">
         <v>331</v>
-      </c>
-      <c r="M18" t="s">
-        <v>332</v>
       </c>
       <c r="V18" t="s">
         <v>20</v>
@@ -1874,27 +1883,27 @@
         <v>20</v>
       </c>
       <c r="Y18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z18">
         <v>8</v>
       </c>
       <c r="AD18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J19" t="s">
         <v>4</v>
@@ -1903,53 +1912,53 @@
         <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Y19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z19">
         <v>8</v>
       </c>
       <c r="AD19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J21" t="s">
         <v>5</v>
@@ -1958,154 +1967,154 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K23">
         <v>4</v>
       </c>
       <c r="L23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AD24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AD25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K26">
         <v>4</v>
       </c>
       <c r="L26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J27" t="s">
         <v>6</v>
@@ -2114,27 +2123,27 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B28">
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J28" t="s">
         <v>7</v>
@@ -2143,27 +2152,27 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B29">
         <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J29" t="s">
         <v>8</v>
@@ -2172,66 +2181,66 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O33" t="s">
         <v>9</v>
@@ -2242,13 +2251,13 @@
     </row>
     <row r="34" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O34" t="s">
         <v>11</v>
@@ -2259,13 +2268,13 @@
     </row>
     <row r="35" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O35" t="s">
         <v>12</v>
@@ -2276,13 +2285,13 @@
     </row>
     <row r="36" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O36" t="s">
         <v>13</v>
@@ -2297,21 +2306,21 @@
         <v>18</v>
       </c>
       <c r="U36" t="s">
+        <v>336</v>
+      </c>
+      <c r="V36" t="s">
         <v>337</v>
-      </c>
-      <c r="V36" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="37" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O37" t="s">
         <v>14</v>
@@ -2326,50 +2335,50 @@
         <v>18</v>
       </c>
       <c r="U37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P38">
         <v>16</v>
       </c>
       <c r="S38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T38">
         <v>18</v>
       </c>
       <c r="U38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O39" t="s">
         <v>15</v>
@@ -2378,803 +2387,803 @@
         <v>16</v>
       </c>
       <c r="S39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T39">
         <v>18</v>
       </c>
       <c r="U39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="V39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O40" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P40">
         <v>11</v>
       </c>
       <c r="S40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T40">
         <v>18</v>
       </c>
       <c r="U40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="V40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S41" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T41">
         <v>18</v>
       </c>
       <c r="U41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G52" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G65" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E67" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E68" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G68" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G72" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G75" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G78" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G79" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G80" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H80" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G84" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G85" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G87" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G88" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H88" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G91" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H91" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G92" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G93" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G94" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G95" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H95" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G96" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G97" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H97" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G98" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G99" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G100" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G101" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H101" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G102" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H102" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G103" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G104" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G105" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H105" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G106" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H106" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G107" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H107" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G108" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G109" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="110" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G110" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H110" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="111" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G111" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="112" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G112" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="113" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H114" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="115" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G115" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H115" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="116" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G116" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="117" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G117" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G118" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H118" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="119" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G119" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H119" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3209,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:AN30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3224,6 +3233,7 @@
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.21875" customWidth="1"/>
     <col min="10" max="10" width="24.109375" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" customWidth="1"/>
     <col min="16" max="16" width="24.6640625" customWidth="1"/>
     <col min="18" max="18" width="14.88671875" customWidth="1"/>
@@ -3239,15 +3249,18 @@
   <sheetData>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="R4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" t="s">
         <v>57</v>
       </c>
-      <c r="W4" t="s">
-        <v>58</v>
+      <c r="Y4" t="s">
+        <v>345</v>
       </c>
       <c r="AD4" t="s">
         <v>38</v>
@@ -3255,13 +3268,16 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" t="s">
-        <v>56</v>
+      <c r="M5" t="s">
+        <v>345</v>
       </c>
       <c r="R5" t="s">
         <v>24</v>
@@ -3273,7 +3289,7 @@
         <v>48</v>
       </c>
       <c r="U5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W5" t="s">
         <v>24</v>
@@ -3291,7 +3307,7 @@
         <v>45</v>
       </c>
       <c r="AB5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD5" t="s">
         <v>24</v>
@@ -3300,13 +3316,13 @@
         <v>25</v>
       </c>
       <c r="AF5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AJ5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.3">
@@ -3317,7 +3333,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -3326,13 +3342,13 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
@@ -3350,7 +3366,7 @@
         <v>45</v>
       </c>
       <c r="P6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R6" t="s">
         <v>12</v>
@@ -3359,10 +3375,10 @@
         <v>36</v>
       </c>
       <c r="T6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W6" t="s">
         <v>13</v>
@@ -3371,7 +3387,7 @@
         <v>33</v>
       </c>
       <c r="Y6" t="s">
-        <v>49</v>
+        <v>346</v>
       </c>
       <c r="Z6" t="s">
         <v>5</v>
@@ -3380,7 +3396,7 @@
         <v>47</v>
       </c>
       <c r="AB6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AD6" t="s">
         <v>12</v>
@@ -3389,16 +3405,16 @@
         <v>39</v>
       </c>
       <c r="AF6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AJ6" t="s">
         <v>26</v>
       </c>
       <c r="AL6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN6" t="s">
         <v>103</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.3">
@@ -3409,7 +3425,7 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -3421,28 +3437,28 @@
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
       </c>
       <c r="M7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O7" t="s">
         <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R7" t="s">
         <v>11</v>
@@ -3451,10 +3467,10 @@
         <v>30</v>
       </c>
       <c r="T7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W7" t="s">
         <v>13</v>
@@ -3463,7 +3479,7 @@
         <v>32</v>
       </c>
       <c r="Y7" t="s">
-        <v>49</v>
+        <v>346</v>
       </c>
       <c r="Z7" t="s">
         <v>5</v>
@@ -3472,7 +3488,7 @@
         <v>46</v>
       </c>
       <c r="AB7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AD7" t="s">
         <v>12</v>
@@ -3481,7 +3497,7 @@
         <v>40</v>
       </c>
       <c r="AF7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AJ7" t="s">
         <v>27</v>
@@ -3490,7 +3506,7 @@
         <v>46</v>
       </c>
       <c r="AN7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.3">
@@ -3501,7 +3517,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -3513,28 +3529,28 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L8" t="s">
         <v>29</v>
       </c>
       <c r="M8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N8" t="s">
         <v>5</v>
       </c>
       <c r="O8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -3543,16 +3559,16 @@
         <v>39</v>
       </c>
       <c r="Y8" t="s">
-        <v>49</v>
+        <v>347</v>
       </c>
       <c r="Z8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA8" t="s">
         <v>46</v>
       </c>
       <c r="AB8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD8" t="s">
         <v>13</v>
@@ -3561,7 +3577,7 @@
         <v>30</v>
       </c>
       <c r="AF8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AJ8" t="s">
         <v>28</v>
@@ -3570,7 +3586,7 @@
         <v>47</v>
       </c>
       <c r="AN8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.3">
@@ -3581,7 +3597,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -3593,28 +3609,28 @@
         <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L9" t="s">
         <v>30</v>
       </c>
       <c r="M9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N9" t="s">
         <v>5</v>
       </c>
       <c r="O9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="W9" t="s">
         <v>15</v>
@@ -3623,16 +3639,16 @@
         <v>40</v>
       </c>
       <c r="Y9" t="s">
-        <v>49</v>
+        <v>347</v>
       </c>
       <c r="Z9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA9" t="s">
         <v>47</v>
       </c>
       <c r="AB9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD9" t="s">
         <v>13</v>
@@ -3641,16 +3657,16 @@
         <v>31</v>
       </c>
       <c r="AF9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ9" t="s">
         <v>29</v>
       </c>
       <c r="AL9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AN9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
@@ -3661,7 +3677,7 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -3673,10 +3689,10 @@
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="W10" t="s">
         <v>15</v>
@@ -3685,16 +3701,16 @@
         <v>41</v>
       </c>
       <c r="Y10" t="s">
-        <v>49</v>
+        <v>347</v>
       </c>
       <c r="Z10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
@@ -3703,16 +3719,16 @@
         <v>40</v>
       </c>
       <c r="AF10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ10" t="s">
         <v>30</v>
       </c>
       <c r="AL10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AN10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.3">
@@ -3723,7 +3739,7 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -3732,13 +3748,13 @@
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W11" t="s">
         <v>15</v>
@@ -3747,16 +3763,16 @@
         <v>42</v>
       </c>
       <c r="Y11" t="s">
-        <v>49</v>
+        <v>347</v>
       </c>
       <c r="Z11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AD11" t="s">
         <v>15</v>
@@ -3765,13 +3781,13 @@
         <v>30</v>
       </c>
       <c r="AF11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AJ11" t="s">
         <v>31</v>
       </c>
       <c r="AN11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.3">
@@ -3782,7 +3798,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -3791,16 +3807,16 @@
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W12" t="s">
         <v>15</v>
@@ -3809,16 +3825,16 @@
         <v>32</v>
       </c>
       <c r="Y12" t="s">
-        <v>49</v>
+        <v>348</v>
       </c>
       <c r="Z12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AA12" t="s">
         <v>46</v>
       </c>
       <c r="AB12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD12" t="s">
         <v>14</v>
@@ -3827,13 +3843,13 @@
         <v>40</v>
       </c>
       <c r="AF12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AJ12" t="s">
         <v>32</v>
       </c>
       <c r="AN12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.3">
@@ -3844,7 +3860,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -3856,10 +3872,10 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W13" t="s">
         <v>15</v>
@@ -3868,16 +3884,16 @@
         <v>33</v>
       </c>
       <c r="Y13" t="s">
-        <v>49</v>
+        <v>348</v>
       </c>
       <c r="Z13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AA13" t="s">
         <v>47</v>
       </c>
       <c r="AB13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AD13" t="s">
         <v>14</v>
@@ -3886,13 +3902,13 @@
         <v>35</v>
       </c>
       <c r="AF13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AJ13" t="s">
         <v>33</v>
       </c>
       <c r="AN13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.3">
@@ -3903,7 +3919,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -3915,10 +3931,10 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AD14" t="s">
         <v>14</v>
@@ -3927,13 +3943,13 @@
         <v>36</v>
       </c>
       <c r="AF14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AJ14" t="s">
         <v>34</v>
       </c>
       <c r="AN14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.3">
@@ -3944,7 +3960,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -3956,16 +3972,16 @@
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ15" t="s">
         <v>35</v>
       </c>
       <c r="AN15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.3">
@@ -3976,7 +3992,7 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -3988,16 +4004,16 @@
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AJ16" t="s">
         <v>36</v>
       </c>
       <c r="AN16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
@@ -4008,13 +4024,13 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AJ17" t="s">
         <v>37</v>
       </c>
       <c r="AN17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
@@ -4022,7 +4038,7 @@
         <v>39</v>
       </c>
       <c r="AN18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -4030,7 +4046,7 @@
         <v>40</v>
       </c>
       <c r="AN19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.3">
@@ -4038,7 +4054,7 @@
         <v>41</v>
       </c>
       <c r="AN20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.3">
@@ -4046,22 +4062,22 @@
         <v>42</v>
       </c>
       <c r="AN21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AN22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AN23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.3">
@@ -4072,7 +4088,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.3">
@@ -4083,16 +4099,16 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M26" t="s">
         <v>137</v>
-      </c>
-      <c r="M26" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.3">
@@ -4103,7 +4119,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
@@ -4112,7 +4128,7 @@
         <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I27" t="s">
         <v>24</v>
@@ -4121,7 +4137,7 @@
         <v>25</v>
       </c>
       <c r="K27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M27" t="s">
         <v>24</v>
@@ -4130,7 +4146,7 @@
         <v>25</v>
       </c>
       <c r="O27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
@@ -4141,7 +4157,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -4150,7 +4166,7 @@
         <v>32</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I28" t="s">
         <v>13</v>
@@ -4159,7 +4175,7 @@
         <v>36</v>
       </c>
       <c r="K28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M28" t="s">
         <v>11</v>
@@ -4168,7 +4184,7 @@
         <v>26</v>
       </c>
       <c r="O28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.3">
@@ -4179,7 +4195,7 @@
         <v>33</v>
       </c>
       <c r="G29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
@@ -4188,7 +4204,7 @@
         <v>37</v>
       </c>
       <c r="K29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M29" t="s">
         <v>11</v>
@@ -4197,7 +4213,7 @@
         <v>41</v>
       </c>
       <c r="O29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.3">
@@ -4208,7 +4224,7 @@
         <v>39</v>
       </c>
       <c r="K30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M30" t="s">
         <v>11</v>
@@ -4217,12 +4233,12 @@
         <v>42</v>
       </c>
       <c r="O30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ22 L7:L9 S6:S7 X6:X13 AE6:AE14 F7:F16 B7:B17" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
       <formula1>$AJ$6:$AJ$21</formula1>
     </dataValidation>
@@ -4252,7 +4268,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C3D18C3-7241-4088-8034-07AAE0EB53A9}">
           <x14:formula1>
             <xm:f>General_Info!$J$19:$J$30</xm:f>
@@ -4289,7 +4305,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -4348,76 +4364,76 @@
   <sheetData>
     <row r="2" spans="9:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" t="s">
+        <v>165</v>
+      </c>
+      <c r="S3" t="s">
+        <v>162</v>
+      </c>
+      <c r="T3" t="s">
         <v>167</v>
       </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
+        <v>164</v>
+      </c>
+      <c r="V3" t="s">
         <v>165</v>
-      </c>
-      <c r="L3" t="s">
-        <v>166</v>
-      </c>
-      <c r="S3" t="s">
-        <v>163</v>
-      </c>
-      <c r="T3" t="s">
-        <v>168</v>
-      </c>
-      <c r="U3" t="s">
-        <v>165</v>
-      </c>
-      <c r="V3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="4" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
       </c>
       <c r="V4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on SysClock Configuration, impact on PWM
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD53EE3-632F-4A65-84EA-AC08F74732BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903DDFA1-DA53-48E1-B07F-B153D0106613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="317">
   <si>
     <t>Colonne1</t>
   </si>
@@ -978,6 +978,18 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Clock Src</t>
+  </si>
+  <si>
+    <t>APB1</t>
+  </si>
+  <si>
+    <t>APB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock Source </t>
   </si>
 </sst>
 </file>
@@ -1053,21 +1065,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:M30" totalsRowShown="0">
-  <autoFilter ref="J18:M30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:N30" totalsRowShown="0">
+  <autoFilter ref="J18:N30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8EBC08AF-F674-4D3F-80D1-664693CE12C7}" name="Timer_name"/>
     <tableColumn id="2" xr3:uid="{9707AE90-9D0C-47B3-A89D-28A13CE83851}" name="Number of channels"/>
     <tableColumn id="3" xr3:uid="{D8031831-59FD-4378-ADF9-534E59E34124}" name="Interrupt line associate"/>
     <tableColumn id="4" xr3:uid="{F81B2123-AE73-4BAA-A2DB-915ACD9E2233}" name="Purpose "/>
+    <tableColumn id="5" xr3:uid="{90409EC9-D84F-4040-AB7C-7CFE8D3ABB81}" name="Clock Source "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}" name="Tableau26" displayName="Tableau26" ref="AD22:AD25" totalsRowShown="0">
-  <autoFilter ref="AD22:AD25" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}" name="Tableau26" displayName="Tableau26" ref="AE46:AE49" totalsRowShown="0">
+  <autoFilter ref="AE46:AE49" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{41DEADB1-B8AC-4DA1-AAC6-1E2E0AF40D54}" name="Timer Purpose"/>
   </tableColumns>
@@ -1087,6 +1100,16 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}" name="Tableau28" displayName="Tableau28" ref="AE52:AE54" totalsRowShown="0">
+  <autoFilter ref="AE52:AE54" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{23F99948-81BD-4C18-8B63-7CCABA76B6A0}" name="Clock Src"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:B15" totalsRowShown="0">
   <autoFilter ref="A6:B15" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
   <tableColumns count="2">
@@ -1097,7 +1120,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="Z7:AA16" totalsRowShown="0">
   <autoFilter ref="Z7:AA16" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="2">
@@ -1108,7 +1131,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="J6:N9" totalsRowShown="0">
   <autoFilter ref="J6:N9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="5">
@@ -1122,7 +1145,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}" name="FMKIO_InputEvnt" displayName="FMKIO_InputEvnt" ref="V6:X8" totalsRowShown="0">
   <autoFilter ref="V6:X8" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}"/>
   <tableColumns count="3">
@@ -1134,7 +1157,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="P6:T14" totalsRowShown="0">
   <autoFilter ref="P6:T14" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="5">
@@ -1148,7 +1171,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:H16" totalsRowShown="0">
   <autoFilter ref="E6:H16" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="4">
@@ -1161,21 +1184,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}" name="Tableau17" displayName="Tableau17" ref="AW29:AW45" totalsRowShown="0">
   <autoFilter ref="AW29:AW45" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{01BF5210-733A-4DB1-A72E-FC1B749F7F18}" name="Pin_Choice"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}" name="Tableau18" displayName="Tableau18" ref="AY30:AY34" totalsRowShown="0">
-  <autoFilter ref="AY30:AY34" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DD976920-6FFB-4C96-8085-12D970F3A0A7}" name="Channel_Choice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1193,6 +1206,16 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}" name="Tableau18" displayName="Tableau18" ref="AY30:AY34" totalsRowShown="0">
+  <autoFilter ref="AY30:AY34" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DD976920-6FFB-4C96-8085-12D970F3A0A7}" name="Channel_Choice"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}" name="Tableau1720" displayName="Tableau1720" ref="BA29:BA47" totalsRowShown="0">
   <autoFilter ref="BA29:BA47" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}"/>
   <tableColumns count="1">
@@ -1202,7 +1225,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}" name="Tableau20" displayName="Tableau20" ref="K74:L77" totalsRowShown="0">
   <autoFilter ref="K74:L77" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}"/>
   <tableColumns count="2">
@@ -1213,7 +1236,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}" name="Tableau2022" displayName="Tableau2022" ref="O78:Q80" totalsRowShown="0">
   <autoFilter ref="O78:Q80" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}"/>
   <tableColumns count="3">
@@ -1225,7 +1248,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}" name="Tableau202223" displayName="Tableau202223" ref="S78:U81" totalsRowShown="0">
   <autoFilter ref="S78:U81" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}"/>
   <tableColumns count="3">
@@ -1237,7 +1260,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="FMKIO_CanCfg" displayName="FMKIO_CanCfg" ref="C29:H32" totalsRowShown="0">
   <autoFilter ref="C29:H32" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
   <tableColumns count="6">
@@ -1252,7 +1275,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -1263,7 +1286,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
   <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
   <tableColumns count="4">
@@ -1276,7 +1299,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
   <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
@@ -1303,8 +1326,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="V17:W18" totalsRowShown="0">
-  <autoFilter ref="V17:W18" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="X36:Y37" totalsRowShown="0">
+  <autoFilter ref="X36:Y37" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{73150C50-6B2A-4CD8-A7E6-62C171935AF8}" name="DAC_Name"/>
     <tableColumn id="2" xr3:uid="{EF9B5413-9A3C-4163-8063-C74DAB2D51F7}" name="number of channel"/>
@@ -1336,8 +1359,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="Y17:Z19" totalsRowShown="0">
-  <autoFilter ref="Y17:Z19" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="AA36:AB38" totalsRowShown="0">
+  <autoFilter ref="AA36:AB38" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00302DEC-D815-47CE-9380-676FE769FF43}" name="DMA_Name"/>
     <tableColumn id="2" xr3:uid="{2654BB85-F763-4BBA-9124-13A3875B62D0}" name="number of channel"/>
@@ -1347,8 +1370,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AD16:AD19" totalsRowShown="0">
-  <autoFilter ref="AD16:AD19" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AE40:AE43" totalsRowShown="0">
+  <autoFilter ref="AE40:AE43" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
   </tableColumns>
@@ -1683,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="A16:AD119"/>
+  <dimension ref="A18:AE119"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,29 +1738,7 @@
     <col min="30" max="30" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="30:30" x14ac:dyDescent="0.3">
-      <c r="AD16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="V17" t="s">
-        <v>19</v>
-      </c>
-      <c r="W17" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>133</v>
       </c>
@@ -1765,23 +1766,11 @@
       <c r="M18" t="s">
         <v>285</v>
       </c>
-      <c r="V18" t="s">
-        <v>20</v>
-      </c>
-      <c r="W18" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z18">
-        <v>8</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>134</v>
       </c>
@@ -1806,17 +1795,11 @@
       <c r="M19" t="s">
         <v>287</v>
       </c>
-      <c r="Y19" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z19">
-        <v>8</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>241</v>
       </c>
@@ -1838,8 +1821,11 @@
       <c r="M20" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>245</v>
       </c>
@@ -1861,8 +1847,11 @@
       <c r="M21" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>246</v>
       </c>
@@ -1884,11 +1873,11 @@
       <c r="M22" t="s">
         <v>287</v>
       </c>
-      <c r="AD22" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>247</v>
       </c>
@@ -1910,11 +1899,11 @@
       <c r="M23" t="s">
         <v>287</v>
       </c>
-      <c r="AD23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>248</v>
       </c>
@@ -1936,11 +1925,11 @@
       <c r="M24" t="s">
         <v>289</v>
       </c>
-      <c r="AD24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>85</v>
       </c>
@@ -1962,11 +1951,11 @@
       <c r="M25" t="s">
         <v>289</v>
       </c>
-      <c r="AD25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>272</v>
       </c>
@@ -1988,8 +1977,11 @@
       <c r="M26" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>294</v>
       </c>
@@ -2017,8 +2009,11 @@
       <c r="M27" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>295</v>
       </c>
@@ -2046,8 +2041,11 @@
       <c r="M28" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>258</v>
       </c>
@@ -2075,8 +2073,11 @@
       <c r="M29" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>83</v>
       </c>
@@ -2098,8 +2099,11 @@
       <c r="M30" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>82</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>81</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>249</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>250</v>
       </c>
@@ -2155,7 +2159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>240</v>
       </c>
@@ -2172,7 +2176,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>239</v>
       </c>
@@ -2200,8 +2204,20 @@
       <c r="V36" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="37" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="X36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>251</v>
       </c>
@@ -2229,8 +2245,20 @@
       <c r="V37" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="X37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>252</v>
       </c>
@@ -2258,8 +2286,14 @@
       <c r="V38" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AA38" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>226</v>
       </c>
@@ -2288,7 +2322,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>253</v>
       </c>
@@ -2316,8 +2350,11 @@
       <c r="V40" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="41" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>254</v>
       </c>
@@ -2339,8 +2376,11 @@
       <c r="V41" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="42" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>238</v>
       </c>
@@ -2350,8 +2390,11 @@
       <c r="H42" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>73</v>
       </c>
@@ -2361,8 +2404,11 @@
       <c r="H43" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>237</v>
       </c>
@@ -2373,7 +2419,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>255</v>
       </c>
@@ -2384,7 +2430,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
         <v>236</v>
       </c>
@@ -2394,8 +2440,11 @@
       <c r="H46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE46" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="47" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>235</v>
       </c>
@@ -2405,8 +2454,11 @@
       <c r="H47" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="48" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AE47" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="48" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>256</v>
       </c>
@@ -2416,8 +2468,11 @@
       <c r="H48" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AE48" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>257</v>
       </c>
@@ -2427,8 +2482,11 @@
       <c r="H49" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AE49" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="50" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>87</v>
       </c>
@@ -2439,7 +2497,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2508,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>231</v>
       </c>
@@ -2460,8 +2518,11 @@
       <c r="H52" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AE52" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="53" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>80</v>
       </c>
@@ -2471,8 +2532,11 @@
       <c r="H53" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AE53" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="54" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>230</v>
       </c>
@@ -2482,8 +2546,11 @@
       <c r="H54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="AE54" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="55" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>292</v>
       </c>
@@ -2494,7 +2561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>293</v>
       </c>
@@ -2505,7 +2572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>229</v>
       </c>
@@ -2516,7 +2583,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>227</v>
       </c>
@@ -2527,7 +2594,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>258</v>
       </c>
@@ -2538,7 +2605,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>88</v>
       </c>
@@ -2549,7 +2616,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>228</v>
       </c>
@@ -2560,7 +2627,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>232</v>
       </c>
@@ -2571,7 +2638,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>259</v>
       </c>
@@ -2582,7 +2649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>71</v>
       </c>
@@ -3077,17 +3144,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18:H119" xr:uid="{049086B5-6506-4A03-974B-48087CF064BC}">
-      <formula1>$AD$17:$AD$19</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18:H119" xr:uid="{3E8F037A-5A22-4138-A36A-F90B67434DDA}">
+      <formula1>$AE$41:$AE$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M30" xr:uid="{697CB459-5495-4019-B31C-A222FA50D4B5}">
-      <formula1>$AD$23:$AD$25</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M30" xr:uid="{17DBAA90-8141-4522-B025-71F13961596F}">
+      <formula1>$AE$47:$AE$49</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N30" xr:uid="{C93913E9-44DA-490C-8435-4DAABE3AC990}">
+      <formula1>$AE$53:$AE$54</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="11">
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3099,6 +3169,7 @@
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3107,7 +3178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Start SysTem Clock Code Gen Configuration
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903DDFA1-DA53-48E1-B07F-B153D0106613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF7CB50-3613-4995-B6C5-F36E175A7A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="324">
   <si>
     <t>Colonne1</t>
   </si>
@@ -104,9 +104,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>RCC_ClockName</t>
   </si>
   <si>
@@ -773,9 +770,6 @@
     <t>GPIOD</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>DMAMUX1</t>
   </si>
   <si>
@@ -990,6 +984,33 @@
   </si>
   <si>
     <t xml:space="preserve">Clock Source </t>
+  </si>
+  <si>
+    <t>Clock Soure</t>
+  </si>
+  <si>
+    <t>HSE</t>
+  </si>
+  <si>
+    <t>HSI</t>
+  </si>
+  <si>
+    <t>SYSTEM</t>
+  </si>
+  <si>
+    <t>HCLK1</t>
+  </si>
+  <si>
+    <t>PLLQ</t>
+  </si>
+  <si>
+    <t>PLLP</t>
+  </si>
+  <si>
+    <t>AHB1</t>
+  </si>
+  <si>
+    <t>AHB2</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1121,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}" name="Tableau28" displayName="Tableau28" ref="AE52:AE54" totalsRowShown="0">
-  <autoFilter ref="AE52:AE54" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}" name="GI_OSCILLATOR" displayName="GI_OSCILLATOR" ref="AE52:AE62" totalsRowShown="0">
+  <autoFilter ref="AE52:AE62" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{23F99948-81BD-4C18-8B63-7CCABA76B6A0}" name="Clock Src"/>
   </tableColumns>
@@ -1352,7 +1373,7 @@
   <autoFilter ref="D18:E75" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{402A3AD5-0AFA-40A5-A5A4-0D9CB2EED72D}" name="RCC_ClockName"/>
-    <tableColumn id="2" xr3:uid="{05025EF0-98DC-4B06-8DD6-ABD9D73D50B7}" name="Description"/>
+    <tableColumn id="2" xr3:uid="{05025EF0-98DC-4B06-8DD6-ABD9D73D50B7}" name="Clock Soure"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1708,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="N25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,8 +1738,8 @@
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="81" customWidth="1"/>
-    <col min="5" max="5" width="85.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
     <col min="6" max="6" width="33.109375" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" customWidth="1"/>
     <col min="8" max="8" width="21.44140625" customWidth="1"/>
@@ -1740,19 +1761,19 @@
   <sheetData>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>315</v>
       </c>
       <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
         <v>58</v>
-      </c>
-      <c r="H18" t="s">
-        <v>59</v>
       </c>
       <c r="J18" t="s">
         <v>2</v>
@@ -1761,27 +1782,30 @@
         <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>322</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J19" t="s">
         <v>4</v>
@@ -1790,50 +1814,56 @@
         <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="E20" t="s">
+        <v>322</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N20" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="E21" t="s">
+        <v>322</v>
       </c>
       <c r="G21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J21" t="s">
         <v>5</v>
@@ -1842,160 +1872,178 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+      <c r="E22" t="s">
+        <v>322</v>
       </c>
       <c r="G22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>247</v>
+        <v>245</v>
+      </c>
+      <c r="E23" t="s">
+        <v>322</v>
       </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K23">
         <v>4</v>
       </c>
       <c r="L23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>248</v>
+        <v>246</v>
+      </c>
+      <c r="E24" t="s">
+        <v>322</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>322</v>
       </c>
       <c r="G25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J25" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>272</v>
+        <v>270</v>
+      </c>
+      <c r="E26" t="s">
+        <v>323</v>
       </c>
       <c r="G26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K26">
         <v>4</v>
       </c>
       <c r="L26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>292</v>
+      </c>
+      <c r="B27" t="s">
         <v>294</v>
       </c>
-      <c r="B27" t="s">
-        <v>296</v>
-      </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>323</v>
       </c>
       <c r="G27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J27" t="s">
         <v>6</v>
@@ -2004,30 +2052,33 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M27" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B28">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>242</v>
+        <v>241</v>
+      </c>
+      <c r="E28" t="s">
+        <v>323</v>
       </c>
       <c r="G28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J28" t="s">
         <v>7</v>
@@ -2036,30 +2087,33 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B29">
         <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+      <c r="E29" t="s">
+        <v>323</v>
       </c>
       <c r="G29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J29" t="s">
         <v>8</v>
@@ -2068,72 +2122,84 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N29" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>323</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M30" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N30" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>323</v>
       </c>
       <c r="G31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>323</v>
       </c>
       <c r="G32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>249</v>
+        <v>247</v>
+      </c>
+      <c r="E33" t="s">
+        <v>321</v>
       </c>
       <c r="G33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O33" t="s">
         <v>9</v>
@@ -2144,13 +2210,16 @@
     </row>
     <row r="34" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="E34" t="s">
+        <v>321</v>
       </c>
       <c r="G34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O34" t="s">
         <v>11</v>
@@ -2161,13 +2230,16 @@
     </row>
     <row r="35" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+      <c r="E35" t="s">
+        <v>313</v>
       </c>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O35" t="s">
         <v>12</v>
@@ -2178,13 +2250,16 @@
     </row>
     <row r="36" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="E36" t="s">
+        <v>313</v>
       </c>
       <c r="G36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O36" t="s">
         <v>13</v>
@@ -2199,10 +2274,10 @@
         <v>18</v>
       </c>
       <c r="U36" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="V36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="X36" t="s">
         <v>19</v>
@@ -2211,7 +2286,7 @@
         <v>18</v>
       </c>
       <c r="AA36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB36" t="s">
         <v>18</v>
@@ -2219,13 +2294,16 @@
     </row>
     <row r="37" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>251</v>
+        <v>249</v>
+      </c>
+      <c r="E37" t="s">
+        <v>313</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O37" t="s">
         <v>14</v>
@@ -2240,10 +2318,10 @@
         <v>18</v>
       </c>
       <c r="U37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="X37" t="s">
         <v>20</v>
@@ -2252,7 +2330,7 @@
         <v>20</v>
       </c>
       <c r="AA37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB37">
         <v>8</v>
@@ -2260,34 +2338,37 @@
     </row>
     <row r="38" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>252</v>
+        <v>250</v>
+      </c>
+      <c r="E38" t="s">
+        <v>313</v>
       </c>
       <c r="G38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P38">
         <v>16</v>
       </c>
       <c r="S38" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="T38">
         <v>18</v>
       </c>
       <c r="U38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AB38">
         <v>8</v>
@@ -2295,13 +2376,16 @@
     </row>
     <row r="39" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="E39" t="s">
+        <v>323</v>
       </c>
       <c r="G39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O39" t="s">
         <v>15</v>
@@ -2310,836 +2394,959 @@
         <v>16</v>
       </c>
       <c r="S39" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="T39">
         <v>18</v>
       </c>
       <c r="U39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V39" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>253</v>
+        <v>251</v>
+      </c>
+      <c r="E40" t="s">
+        <v>323</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P40">
         <v>11</v>
       </c>
       <c r="S40" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="T40">
         <v>18</v>
       </c>
       <c r="U40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AE40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>254</v>
+        <v>252</v>
+      </c>
+      <c r="E41" t="s">
+        <v>320</v>
       </c>
       <c r="G41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S41" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T41">
         <v>18</v>
       </c>
       <c r="U41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V41" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AE41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="E42" t="s">
+        <v>312</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="E43" t="s">
+        <v>312</v>
       </c>
       <c r="G43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="E44" t="s">
+        <v>312</v>
       </c>
       <c r="G44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="E45" t="s">
+        <v>312</v>
       </c>
       <c r="G45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>236</v>
+        <v>235</v>
+      </c>
+      <c r="E46" t="s">
+        <v>312</v>
       </c>
       <c r="G46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="E47" t="s">
+        <v>312</v>
       </c>
       <c r="G47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>256</v>
+        <v>254</v>
+      </c>
+      <c r="E48" t="s">
+        <v>312</v>
       </c>
       <c r="G48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE48" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>257</v>
+        <v>255</v>
+      </c>
+      <c r="E49" t="s">
+        <v>312</v>
       </c>
       <c r="G49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE49" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="E50" t="s">
+        <v>312</v>
       </c>
       <c r="G50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>312</v>
       </c>
       <c r="G51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="E52" t="s">
+        <v>312</v>
       </c>
       <c r="G52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE52" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="53" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E53" t="s">
+        <v>312</v>
       </c>
       <c r="G53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE53" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="E54" t="s">
+        <v>312</v>
       </c>
       <c r="G54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE54" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>292</v>
+        <v>290</v>
+      </c>
+      <c r="E55" t="s">
+        <v>312</v>
       </c>
       <c r="G55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H55" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="E56" t="s">
+        <v>312</v>
       </c>
       <c r="G56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H56" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="E57" t="s">
+        <v>312</v>
       </c>
       <c r="G57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H57" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
+        <v>312</v>
       </c>
       <c r="G58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H58" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>258</v>
+        <v>256</v>
+      </c>
+      <c r="E59" t="s">
+        <v>320</v>
       </c>
       <c r="G59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H59" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="E60" t="s">
+        <v>312</v>
       </c>
       <c r="G60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H60" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="61" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+      <c r="E61" t="s">
+        <v>312</v>
       </c>
       <c r="G61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H61" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="E62" t="s">
+        <v>312</v>
       </c>
       <c r="G62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H62" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="E63" t="s">
+        <v>312</v>
       </c>
       <c r="G63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E64" t="s">
+        <v>313</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="E65" t="s">
+        <v>313</v>
       </c>
       <c r="G65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="E66" t="s">
+        <v>313</v>
       </c>
       <c r="G66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="G67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="G68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E69" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="G69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>313</v>
       </c>
       <c r="G70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="E71" t="s">
+        <v>313</v>
       </c>
       <c r="G71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="E72" t="s">
+        <v>313</v>
       </c>
       <c r="G72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>233</v>
+        <v>232</v>
+      </c>
+      <c r="E73" t="s">
+        <v>313</v>
       </c>
       <c r="G73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>261</v>
+        <v>259</v>
+      </c>
+      <c r="E74" t="s">
+        <v>313</v>
       </c>
       <c r="G74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>262</v>
+        <v>260</v>
+      </c>
+      <c r="E75" t="s">
+        <v>313</v>
       </c>
       <c r="G75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G79" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.3">
       <c r="G80" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G85" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H87" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G90" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G91" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H92" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G100" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G101" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G102" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H102" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G103" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G104" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H104" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G106" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H106" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H107" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G108" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H108" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G109" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H109" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G110" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H110" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G111" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H111" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G112" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H112" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="113" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G113" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H113" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="114" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G114" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H114" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="115" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G115" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H115" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="116" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G116" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H116" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G117" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H117" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G118" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H118" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G119" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H119" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3151,8 +3358,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M30" xr:uid="{17DBAA90-8141-4522-B025-71F13961596F}">
       <formula1>$AE$47:$AE$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N30" xr:uid="{C93913E9-44DA-490C-8435-4DAABE3AC990}">
-      <formula1>$AE$53:$AE$54</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N30 E19:E75" xr:uid="{C93913E9-44DA-490C-8435-4DAABE3AC990}">
+      <formula1>$AE$53:$AE$62</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3213,92 +3420,92 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
+        <v>295</v>
+      </c>
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" t="s">
+        <v>295</v>
+      </c>
+      <c r="V5" t="s">
         <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>297</v>
-      </c>
-      <c r="P5" t="s">
-        <v>57</v>
-      </c>
-      <c r="R5" t="s">
-        <v>297</v>
-      </c>
-      <c r="V5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
       <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
       <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
       <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>44</v>
       </c>
-      <c r="N6" t="s">
-        <v>45</v>
-      </c>
       <c r="P6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" t="s">
-        <v>25</v>
-      </c>
       <c r="R6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" t="s">
         <v>43</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>44</v>
       </c>
-      <c r="T6" t="s">
-        <v>45</v>
-      </c>
       <c r="V6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W6" t="s">
         <v>24</v>
       </c>
-      <c r="W6" t="s">
-        <v>25</v>
-      </c>
       <c r="X6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Z6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
@@ -3306,64 +3513,64 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
       </c>
       <c r="Q7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="S7" t="s">
         <v>5</v>
       </c>
       <c r="T7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V7" t="s">
         <v>12</v>
       </c>
       <c r="W7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" t="s">
         <v>24</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
@@ -3371,64 +3578,64 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
       </c>
       <c r="N8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" t="s">
         <v>13</v>
       </c>
       <c r="Q8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="S8" t="s">
         <v>5</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V8" t="s">
         <v>11</v>
       </c>
       <c r="W8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z8" t="s">
         <v>12</v>
       </c>
       <c r="AA8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
@@ -3436,55 +3643,55 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
         <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P9" t="s">
         <v>15</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Z9" t="s">
         <v>12</v>
       </c>
       <c r="AA9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
@@ -3492,40 +3699,40 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P10" t="s">
         <v>15</v>
       </c>
       <c r="Q10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z10" t="s">
         <v>13</v>
       </c>
       <c r="AA10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
@@ -3533,40 +3740,40 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P11" t="s">
         <v>15</v>
       </c>
       <c r="Q11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z11" t="s">
         <v>13</v>
       </c>
       <c r="AA11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
@@ -3574,40 +3781,40 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P12" t="s">
         <v>15</v>
       </c>
       <c r="Q12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z12" t="s">
         <v>13</v>
       </c>
       <c r="AA12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
@@ -3615,40 +3822,40 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P13" t="s">
         <v>15</v>
       </c>
       <c r="Q13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Z13" t="s">
         <v>15</v>
       </c>
       <c r="AA13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
@@ -3656,40 +3863,40 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P14" t="s">
         <v>15</v>
       </c>
       <c r="Q14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z14" t="s">
         <v>14</v>
       </c>
       <c r="AA14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
@@ -3697,25 +3904,25 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z15" t="s">
         <v>14</v>
       </c>
       <c r="AA15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
@@ -3723,19 +3930,19 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z16" t="s">
         <v>14</v>
       </c>
       <c r="AA16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="3:53" x14ac:dyDescent="0.3">
@@ -3743,38 +3950,38 @@
     </row>
     <row r="23" spans="3:53" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="3:53" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="3:53" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
+        <v>302</v>
+      </c>
+      <c r="D29" t="s">
+        <v>303</v>
+      </c>
+      <c r="E29" t="s">
         <v>304</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>305</v>
       </c>
-      <c r="E29" t="s">
-        <v>306</v>
-      </c>
-      <c r="F29" t="s">
-        <v>307</v>
-      </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AW29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BA29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="3:53" x14ac:dyDescent="0.3">
@@ -3782,224 +3989,224 @@
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AW30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AY30" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA30" t="s">
         <v>94</v>
-      </c>
-      <c r="BA30" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" spans="3:53" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>269</v>
+      </c>
+      <c r="F31" t="s">
         <v>41</v>
       </c>
-      <c r="E31" t="s">
-        <v>271</v>
-      </c>
-      <c r="F31" t="s">
-        <v>42</v>
-      </c>
       <c r="G31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H31" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AW31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AY31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BA31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="3:53" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H32" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AW32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AY32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="BA32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AY33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BA33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AY34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BA34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BA35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="BA36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BA37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BA38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BA39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BA40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BA41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="BA42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BA43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BA44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="49:53" x14ac:dyDescent="0.3">
       <c r="AW45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="49:53" x14ac:dyDescent="0.3">
       <c r="BA46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="49:53" x14ac:dyDescent="0.3">
       <c r="BA47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="36:36" x14ac:dyDescent="0.3">
       <c r="AJ57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="11:21" x14ac:dyDescent="0.3">
       <c r="K73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="11:21" x14ac:dyDescent="0.3">
       <c r="K74" t="s">
+        <v>23</v>
+      </c>
+      <c r="L74" t="s">
         <v>24</v>
-      </c>
-      <c r="L74" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="75" spans="11:21" x14ac:dyDescent="0.3">
@@ -4007,7 +4214,7 @@
         <v>11</v>
       </c>
       <c r="L75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="11:21" x14ac:dyDescent="0.3">
@@ -4015,7 +4222,7 @@
         <v>11</v>
       </c>
       <c r="L76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="11:21" x14ac:dyDescent="0.3">
@@ -4023,33 +4230,33 @@
         <v>11</v>
       </c>
       <c r="L77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R77" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" spans="11:21" x14ac:dyDescent="0.3">
       <c r="O78" t="s">
+        <v>23</v>
+      </c>
+      <c r="P78" t="s">
         <v>24</v>
       </c>
-      <c r="P78" t="s">
-        <v>25</v>
-      </c>
       <c r="Q78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S78" t="s">
+        <v>23</v>
+      </c>
+      <c r="T78" t="s">
         <v>24</v>
       </c>
-      <c r="T78" t="s">
-        <v>25</v>
-      </c>
       <c r="U78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="11:21" x14ac:dyDescent="0.3">
@@ -4057,19 +4264,19 @@
         <v>12</v>
       </c>
       <c r="P79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S79" t="s">
         <v>13</v>
       </c>
       <c r="T79" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="11:21" x14ac:dyDescent="0.3">
@@ -4077,19 +4284,19 @@
         <v>12</v>
       </c>
       <c r="P80" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q80" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S80" t="s">
         <v>13</v>
       </c>
       <c r="T80" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="19:21" x14ac:dyDescent="0.3">
@@ -4097,10 +4304,10 @@
         <v>13</v>
       </c>
       <c r="T81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4172,7 +4379,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -4188,7 +4395,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -4196,7 +4403,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -4231,76 +4438,76 @@
   <sheetData>
     <row r="2" spans="9:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" t="s">
+        <v>129</v>
+      </c>
+      <c r="S3" t="s">
+        <v>126</v>
+      </c>
+      <c r="T3" t="s">
         <v>131</v>
       </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
+        <v>128</v>
+      </c>
+      <c r="V3" t="s">
         <v>129</v>
-      </c>
-      <c r="L3" t="s">
-        <v>130</v>
-      </c>
-      <c r="S3" t="s">
-        <v>127</v>
-      </c>
-      <c r="T3" t="s">
-        <v>132</v>
-      </c>
-      <c r="U3" t="s">
-        <v>129</v>
-      </c>
-      <c r="V3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
       </c>
       <c r="V4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
+        <v>278</v>
+      </c>
+      <c r="J5" t="s">
         <v>280</v>
       </c>
-      <c r="J5" t="s">
-        <v>282</v>
-      </c>
       <c r="K5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work On COde GEn FMKMAC
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\Stm32PrjTpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDB8D5E-08AE-4916-8A3B-F287C114C457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617EBBA9-AEAB-4607-ACC3-E95714D18908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
     <sheet name="FMK_IO" sheetId="2" r:id="rId2"/>
     <sheet name="FMK_CPU" sheetId="3" r:id="rId3"/>
     <sheet name="FMK_CDA" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1" sheetId="5" r:id="rId5"/>
+    <sheet name="FMKMAC" sheetId="6" r:id="rId5"/>
+    <sheet name="Feuil1" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="364">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1087,6 +1088,51 @@
   </si>
   <si>
     <t>FrequenceeTheo</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>DMA_1</t>
+  </si>
+  <si>
+    <t>DMA_2</t>
+  </si>
+  <si>
+    <t>RqstDmaType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMA </t>
+  </si>
+  <si>
+    <t>CHANNEL</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>CHANNEL_5</t>
+  </si>
+  <si>
+    <t>UART4_RX</t>
+  </si>
+  <si>
+    <t>UART4_TX</t>
+  </si>
+  <si>
+    <t>USART1_RX</t>
+  </si>
+  <si>
+    <t>CHANNEL_6</t>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+  </si>
+  <si>
+    <t>CHANNEL_7</t>
+  </si>
+  <si>
+    <t>SERIAL CONFIGURATION</t>
   </si>
 </sst>
 </file>
@@ -3669,8 +3715,8 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="FMKIO_CanCfg" displayName="FMKIO_CanCfg" ref="C29:H32" totalsRowShown="0">
-  <autoFilter ref="C29:H32" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="FMKIO_CanCfg" displayName="FMKIO_CanCfg" ref="A25:F28" totalsRowShown="0">
+  <autoFilter ref="A25:F28" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{95762CE8-B06D-493C-B844-88501CD65909}" name="Rx_GPIO_name"/>
     <tableColumn id="4" xr3:uid="{A74F40FB-56BA-4761-B2D5-1E61012674DB}" name="RxPin_name"/>
@@ -3684,6 +3730,21 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}" name="FMKIO_CanCfg31" displayName="FMKIO_CanCfg31" ref="A34:F37" totalsRowShown="0">
+  <autoFilter ref="A34:F37" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{24FCFF33-29FB-4C97-8C6A-E82227514712}" name="Rx_GPIO_name"/>
+    <tableColumn id="4" xr3:uid="{12CA2E7A-25CB-4594-B099-0C3300125F20}" name="RxPin_name"/>
+    <tableColumn id="6" xr3:uid="{D003CF17-D1FC-4925-A150-971DDF359F41}" name="Tx_Gpio_Name"/>
+    <tableColumn id="5" xr3:uid="{14396C2C-537A-4355-B49A-DC2EB4D94AF0}" name="Tx_Pin_Name"/>
+    <tableColumn id="2" xr3:uid="{EBD561D8-5769-44A2-9D68-D1A8F057FDD0}" name="alternate function timer"/>
+    <tableColumn id="7" xr3:uid="{9DFBCFF1-0113-4C17-8011-2570BD8C9102}" name="FDCAnx"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -3694,7 +3755,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
   <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
   <tableColumns count="4">
@@ -3707,7 +3768,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
   <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
@@ -3721,13 +3782,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="S36:V41" totalsRowShown="0">
-  <autoFilter ref="S36:V41" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="S20:V25" totalsRowShown="0">
+  <autoFilter ref="S20:V25" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
     <tableColumn id="2" xr3:uid="{20DF5352-4B39-416D-A6E4-D94E56AED1C9}" name="number of channel"/>
     <tableColumn id="3" xr3:uid="{9F9316C2-2066-47BF-B84E-436D4C41B07C}" name="IRQN assoiated"/>
     <tableColumn id="4" xr3:uid="{CC116C4D-98B0-46BC-A882-0B90828FFD68}" name="Clock Associated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}" name="FMKMAC_Cfg" displayName="FMKMAC_Cfg" ref="B2:E9" totalsRowShown="0">
+  <autoFilter ref="B2:E9" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{9B6EDCAA-F526-412C-A8EC-AC6897A0EB04}" name="RqstDmaType"/>
+    <tableColumn id="2" xr3:uid="{ED583461-6D2B-456F-A394-15F76B273D8C}" name="DMA "/>
+    <tableColumn id="3" xr3:uid="{7F10CEC2-41BD-45B5-9EDB-D20E18825436}" name="CHANNEL"/>
+    <tableColumn id="4" xr3:uid="{EFAF749E-49CF-4544-A2E6-D7B17CF25518}" name="Priority"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3767,11 +3841,12 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="AA36:AB38" totalsRowShown="0">
-  <autoFilter ref="AA36:AB38" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="AA20:AC22" totalsRowShown="0">
+  <autoFilter ref="AA20:AC22" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00302DEC-D815-47CE-9380-676FE769FF43}" name="DMA_Name"/>
     <tableColumn id="2" xr3:uid="{2654BB85-F763-4BBA-9124-13A3875B62D0}" name="number of channel"/>
+    <tableColumn id="3" xr3:uid="{8630D7D5-DAE5-4E6D-9958-F1FC2A620F7A}" name="Clock Associated"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4116,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AE119"/>
   <sheetViews>
-    <sheetView topLeftCell="G14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27:L27"/>
+    <sheetView topLeftCell="U16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4146,7 +4221,7 @@
     <col min="30" max="30" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>132</v>
       </c>
@@ -4178,7 +4253,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>133</v>
       </c>
@@ -4210,7 +4285,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>240</v>
       </c>
@@ -4238,8 +4313,29 @@
       <c r="N20" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>17</v>
+      </c>
+      <c r="T20" t="s">
+        <v>18</v>
+      </c>
+      <c r="U20" t="s">
+        <v>288</v>
+      </c>
+      <c r="V20" t="s">
+        <v>289</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>243</v>
       </c>
@@ -4267,8 +4363,29 @@
       <c r="N21" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
+        <v>16</v>
+      </c>
+      <c r="T21">
+        <v>18</v>
+      </c>
+      <c r="U21" t="s">
+        <v>148</v>
+      </c>
+      <c r="V21" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB21">
+        <v>8</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>244</v>
       </c>
@@ -4296,8 +4413,29 @@
       <c r="N22" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S22" t="s">
+        <v>271</v>
+      </c>
+      <c r="T22">
+        <v>18</v>
+      </c>
+      <c r="U22" t="s">
+        <v>148</v>
+      </c>
+      <c r="V22" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB22">
+        <v>8</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>245</v>
       </c>
@@ -4325,8 +4463,20 @@
       <c r="N23" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S23" t="s">
+        <v>272</v>
+      </c>
+      <c r="T23">
+        <v>18</v>
+      </c>
+      <c r="U23" t="s">
+        <v>171</v>
+      </c>
+      <c r="V23" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>246</v>
       </c>
@@ -4354,8 +4504,20 @@
       <c r="N24" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S24" t="s">
+        <v>273</v>
+      </c>
+      <c r="T24">
+        <v>18</v>
+      </c>
+      <c r="U24" t="s">
+        <v>185</v>
+      </c>
+      <c r="V24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>84</v>
       </c>
@@ -4383,8 +4545,20 @@
       <c r="N25" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S25" t="s">
+        <v>274</v>
+      </c>
+      <c r="T25">
+        <v>18</v>
+      </c>
+      <c r="U25" t="s">
+        <v>186</v>
+      </c>
+      <c r="V25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>270</v>
       </c>
@@ -4413,7 +4587,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>292</v>
       </c>
@@ -4448,7 +4622,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>293</v>
       </c>
@@ -4483,7 +4657,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>256</v>
       </c>
@@ -4518,7 +4692,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>82</v>
       </c>
@@ -4547,7 +4721,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>81</v>
       </c>
@@ -4561,7 +4735,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>80</v>
       </c>
@@ -4654,28 +4828,10 @@
       <c r="P36">
         <v>16</v>
       </c>
-      <c r="S36" t="s">
-        <v>17</v>
-      </c>
-      <c r="T36" t="s">
-        <v>18</v>
-      </c>
-      <c r="U36" t="s">
-        <v>288</v>
-      </c>
-      <c r="V36" t="s">
-        <v>289</v>
-      </c>
       <c r="X36" t="s">
         <v>19</v>
       </c>
       <c r="Y36" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB36" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4698,29 +4854,11 @@
       <c r="P37">
         <v>16</v>
       </c>
-      <c r="S37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T37">
-        <v>18</v>
-      </c>
-      <c r="U37" t="s">
-        <v>148</v>
-      </c>
-      <c r="V37" t="s">
-        <v>247</v>
-      </c>
       <c r="X37" t="s">
         <v>20</v>
       </c>
       <c r="Y37" t="s">
         <v>20</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB37">
-        <v>8</v>
       </c>
     </row>
     <row r="38" spans="4:31" x14ac:dyDescent="0.3">
@@ -4742,24 +4880,6 @@
       <c r="P38">
         <v>16</v>
       </c>
-      <c r="S38" t="s">
-        <v>271</v>
-      </c>
-      <c r="T38">
-        <v>18</v>
-      </c>
-      <c r="U38" t="s">
-        <v>148</v>
-      </c>
-      <c r="V38" t="s">
-        <v>247</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>240</v>
-      </c>
-      <c r="AB38">
-        <v>8</v>
-      </c>
     </row>
     <row r="39" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
@@ -4780,18 +4900,6 @@
       <c r="P39">
         <v>16</v>
       </c>
-      <c r="S39" t="s">
-        <v>272</v>
-      </c>
-      <c r="T39">
-        <v>18</v>
-      </c>
-      <c r="U39" t="s">
-        <v>171</v>
-      </c>
-      <c r="V39" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="40" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
@@ -4812,18 +4920,6 @@
       <c r="P40">
         <v>11</v>
       </c>
-      <c r="S40" t="s">
-        <v>273</v>
-      </c>
-      <c r="T40">
-        <v>18</v>
-      </c>
-      <c r="U40" t="s">
-        <v>185</v>
-      </c>
-      <c r="V40" t="s">
-        <v>248</v>
-      </c>
       <c r="AE40" t="s">
         <v>88</v>
       </c>
@@ -4840,18 +4936,6 @@
       </c>
       <c r="H41" t="s">
         <v>90</v>
-      </c>
-      <c r="S41" t="s">
-        <v>274</v>
-      </c>
-      <c r="T41">
-        <v>18</v>
-      </c>
-      <c r="U41" t="s">
-        <v>186</v>
-      </c>
-      <c r="V41" t="s">
-        <v>248</v>
       </c>
       <c r="AE41" t="s">
         <v>89</v>
@@ -5772,8 +5856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6332,38 +6416,100 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="3:53" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
       <c r="Q18" s="4"/>
     </row>
-    <row r="23" spans="3:53" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="3:53" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" t="s">
+        <v>303</v>
+      </c>
+      <c r="C25" t="s">
+        <v>304</v>
+      </c>
+      <c r="D25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>301</v>
+      </c>
+      <c r="F26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>269</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>301</v>
+      </c>
+      <c r="F27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
       <c r="C28" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="29" spans="3:53" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>302</v>
-      </c>
-      <c r="D29" t="s">
-        <v>303</v>
-      </c>
-      <c r="E29" t="s">
-        <v>304</v>
-      </c>
-      <c r="F29" t="s">
-        <v>305</v>
-      </c>
-      <c r="G29" t="s">
-        <v>42</v>
-      </c>
-      <c r="H29" t="s">
-        <v>309</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>301</v>
+      </c>
+      <c r="F28" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW29" t="s">
         <v>91</v>
       </c>
@@ -6371,25 +6517,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="3:53" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" t="s">
-        <v>301</v>
-      </c>
-      <c r="H30" t="s">
-        <v>306</v>
-      </c>
+    <row r="30" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW30" t="s">
         <v>25</v>
       </c>
@@ -6400,25 +6528,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="3:53" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>269</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" t="s">
-        <v>269</v>
-      </c>
-      <c r="F31" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" t="s">
-        <v>301</v>
-      </c>
-      <c r="H31" t="s">
-        <v>308</v>
-      </c>
+    <row r="31" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW31" t="s">
         <v>26</v>
       </c>
@@ -6429,25 +6539,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="3:53" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>269</v>
-      </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" t="s">
-        <v>269</v>
-      </c>
-      <c r="F32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" t="s">
-        <v>301</v>
-      </c>
-      <c r="H32" t="s">
-        <v>307</v>
-      </c>
+    <row r="32" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW32" t="s">
         <v>27</v>
       </c>
@@ -6458,7 +6550,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>363</v>
+      </c>
       <c r="AW33" t="s">
         <v>28</v>
       </c>
@@ -6469,7 +6564,25 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B34" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34" t="s">
+        <v>304</v>
+      </c>
+      <c r="D34" t="s">
+        <v>305</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" t="s">
+        <v>309</v>
+      </c>
       <c r="AW34" t="s">
         <v>29</v>
       </c>
@@ -6480,7 +6593,25 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>301</v>
+      </c>
+      <c r="F35" t="s">
+        <v>306</v>
+      </c>
       <c r="AW35" t="s">
         <v>30</v>
       </c>
@@ -6488,7 +6619,25 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>269</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>301</v>
+      </c>
+      <c r="F36" t="s">
+        <v>308</v>
+      </c>
       <c r="AW36" t="s">
         <v>31</v>
       </c>
@@ -6496,7 +6645,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>269</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>301</v>
+      </c>
+      <c r="F37" t="s">
+        <v>307</v>
+      </c>
       <c r="AW37" t="s">
         <v>32</v>
       </c>
@@ -6504,7 +6671,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW38" t="s">
         <v>33</v>
       </c>
@@ -6512,7 +6679,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW39" t="s">
         <v>34</v>
       </c>
@@ -6520,7 +6687,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW40" t="s">
         <v>35</v>
       </c>
@@ -6528,7 +6695,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW41" t="s">
         <v>36</v>
       </c>
@@ -6536,7 +6703,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW42" t="s">
         <v>38</v>
       </c>
@@ -6544,7 +6711,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW43" t="s">
         <v>39</v>
       </c>
@@ -6552,7 +6719,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW44" t="s">
         <v>40</v>
       </c>
@@ -6560,7 +6727,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW45" t="s">
         <v>41</v>
       </c>
@@ -6568,12 +6735,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:53" x14ac:dyDescent="0.3">
       <c r="BA46" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="49:53" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.3">
       <c r="BA47" t="s">
         <v>111</v>
       </c>
@@ -6712,7 +6879,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="13">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -6726,6 +6893,7 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -6744,7 +6912,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
           <x14:formula1>
-            <xm:f>General_Info!$S$37:$S$41</xm:f>
+            <xm:f>General_Info!$S$21:$S$25</xm:f>
           </x14:formula1>
           <xm:sqref>G6:G16</xm:sqref>
         </x14:dataValidation>
@@ -6759,7 +6927,7 @@
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6907,17 +7075,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
-          <x14:formula1>
-            <xm:f>General_Info!$S$37:$S$41</xm:f>
-          </x14:formula1>
-          <xm:sqref>K4:K5</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AB0981D-B484-49AA-81E2-46EA728857EF}">
           <x14:formula1>
             <xm:f>FMK_IO!$BA$30:$BA$47</xm:f>
           </x14:formula1>
           <xm:sqref>V4 L4:L5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
+          <x14:formula1>
+            <xm:f>General_Info!$S$21:$S$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4:K5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
           <x14:formula1>
@@ -6932,10 +7100,145 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E18236-E25D-41B3-8B1E-0194276152B3}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860CCB6B-9BC8-4B28-B4AE-B22F38F81573}">
   <dimension ref="B1:P254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Code Gen IO for Serila, Done, FMK_SRL.c To be tested
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617EBBA9-AEAB-4607-ACC3-E95714D18908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18C936F-9CA9-4431-970A-9E6B2A6C9999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="367">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1133,6 +1133,15 @@
   </si>
   <si>
     <t>SERIAL CONFIGURATION</t>
+  </si>
+  <si>
+    <t>GPIO_AF7_USART2</t>
+  </si>
+  <si>
+    <t>GPIO_AF5_UART4</t>
+  </si>
+  <si>
+    <t>UART/USART REF</t>
   </si>
 </sst>
 </file>
@@ -3730,15 +3739,15 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}" name="FMKIO_CanCfg31" displayName="FMKIO_CanCfg31" ref="A34:F37" totalsRowShown="0">
-  <autoFilter ref="A34:F37" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}" name="FMKIO_SerialCfg" displayName="FMKIO_SerialCfg" ref="A34:F36" totalsRowShown="0">
+  <autoFilter ref="A34:F36" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{24FCFF33-29FB-4C97-8C6A-E82227514712}" name="Rx_GPIO_name"/>
     <tableColumn id="4" xr3:uid="{12CA2E7A-25CB-4594-B099-0C3300125F20}" name="RxPin_name"/>
     <tableColumn id="6" xr3:uid="{D003CF17-D1FC-4925-A150-971DDF359F41}" name="Tx_Gpio_Name"/>
     <tableColumn id="5" xr3:uid="{14396C2C-537A-4355-B49A-DC2EB4D94AF0}" name="Tx_Pin_Name"/>
     <tableColumn id="2" xr3:uid="{EBD561D8-5769-44A2-9D68-D1A8F057FDD0}" name="alternate function timer"/>
-    <tableColumn id="7" xr3:uid="{9DFBCFF1-0113-4C17-8011-2570BD8C9102}" name="FDCAnx"/>
+    <tableColumn id="7" xr3:uid="{9DFBCFF1-0113-4C17-8011-2570BD8C9102}" name="UART/USART REF"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5856,8 +5865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6378,7 +6387,7 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -6398,7 +6407,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
         <v>28</v>
@@ -6581,7 +6590,7 @@
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -6598,19 +6607,19 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>301</v>
+        <v>364</v>
       </c>
       <c r="F35" t="s">
-        <v>306</v>
+        <v>79</v>
       </c>
       <c r="AW35" t="s">
         <v>30</v>
@@ -6621,22 +6630,22 @@
     </row>
     <row r="36" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>301</v>
+        <v>365</v>
       </c>
       <c r="F36" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="AW36" t="s">
         <v>31</v>
@@ -6646,24 +6655,6 @@
       </c>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>269</v>
-      </c>
-      <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" t="s">
-        <v>269</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" t="s">
-        <v>301</v>
-      </c>
-      <c r="F37" t="s">
-        <v>307</v>
-      </c>
       <c r="AW37" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Serial Mode Polling Working
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18C936F-9CA9-4431-970A-9E6B2A6C9999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5833EA-70C0-4B7A-B819-F4E31DA08974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="FMK_CPU" sheetId="3" r:id="rId3"/>
     <sheet name="FMK_CDA" sheetId="4" r:id="rId4"/>
     <sheet name="FMKMAC" sheetId="6" r:id="rId5"/>
-    <sheet name="Feuil1" sheetId="5" r:id="rId6"/>
+    <sheet name="FMKCAN" sheetId="7" r:id="rId6"/>
+    <sheet name="FMKSRL" sheetId="8" r:id="rId7"/>
+    <sheet name="Feuil1" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="423">
   <si>
     <t>Colonne1</t>
   </si>
@@ -973,9 +975,6 @@
     <t>FDCAnx</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>Clock Src</t>
   </si>
   <si>
@@ -1142,6 +1141,177 @@
   </si>
   <si>
     <t>UART/USART REF</t>
+  </si>
+  <si>
+    <t>TIM1_BRK_TIM15_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM1_UP_TIM16_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM1_TRG_COM_TIM17_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM1_CC_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM2_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM3_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM4_IRQHandler</t>
+  </si>
+  <si>
+    <t>List IRQN_Handler</t>
+  </si>
+  <si>
+    <t>TIM6_DAC_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM7_DAC_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM20_BRK_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM20_UP_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM20_TRG_COM_IRQHandler</t>
+  </si>
+  <si>
+    <t>TIM20_CC_IRQHandler</t>
+  </si>
+  <si>
+    <t>check startup_stm32XYYY</t>
+  </si>
+  <si>
+    <t>EXTI0_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI1_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI2_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI3_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI4_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI9_5_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI15_10_IRQHandler</t>
+  </si>
+  <si>
+    <t>ADC1_2_IRQHandler</t>
+  </si>
+  <si>
+    <t>ADC3_IRQHandler</t>
+  </si>
+  <si>
+    <t>ADC4_IRQHandler</t>
+  </si>
+  <si>
+    <t>ADC5_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel1_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel2_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel3_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel4_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel5_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel1_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel2_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel3_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel4_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel5_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel6_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA1_Channel7_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel6_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel7_IRQHandler</t>
+  </si>
+  <si>
+    <t>DMA2_Channel8_IRQHandler</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>FDCAN2_IT0_IRQHandler</t>
+  </si>
+  <si>
+    <t>FDCAN2_IT1_IRQHandler</t>
+  </si>
+  <si>
+    <t>FDCAN3_IT0_IRQHandler</t>
+  </si>
+  <si>
+    <t>FDCAN3_IT1_IRQHandler</t>
+  </si>
+  <si>
+    <t>FDCAN1_IT0_IRQHandler</t>
+  </si>
+  <si>
+    <t>FDCAN1_IT1_IRQHandler</t>
+  </si>
+  <si>
+    <t>Timer Associated</t>
+  </si>
+  <si>
+    <t>Adc, Dac associated</t>
+  </si>
+  <si>
+    <t>ADC1,ADC2</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>ADC4</t>
+  </si>
+  <si>
+    <t>ADC5</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Request Periph Cfg</t>
   </si>
 </sst>
 </file>
@@ -3528,8 +3698,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:N30" totalsRowShown="0">
-  <autoFilter ref="J18:N30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="K18:O30" totalsRowShown="0">
+  <autoFilter ref="K18:O30" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8EBC08AF-F674-4D3F-80D1-664693CE12C7}" name="Timer_name"/>
     <tableColumn id="2" xr3:uid="{9707AE90-9D0C-47B3-A89D-28A13CE83851}" name="Number of channels"/>
@@ -3542,8 +3712,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}" name="Tableau26" displayName="Tableau26" ref="AE46:AE49" totalsRowShown="0">
-  <autoFilter ref="AE46:AE49" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}" name="Tableau26" displayName="Tableau26" ref="AF46:AF49" totalsRowShown="0">
+  <autoFilter ref="AF46:AF49" xr:uid="{7B17A539-E635-4152-9412-9ADCB0D5ADE1}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{41DEADB1-B8AC-4DA1-AAC6-1E2E0AF40D54}" name="Timer Purpose"/>
   </tableColumns>
@@ -3563,8 +3733,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}" name="GI_OSCILLATOR" displayName="GI_OSCILLATOR" ref="AE52:AE62" totalsRowShown="0">
-  <autoFilter ref="AE52:AE62" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}" name="GI_OSCILLATOR" displayName="GI_OSCILLATOR" ref="AF52:AF62" totalsRowShown="0">
+  <autoFilter ref="AF52:AF62" xr:uid="{93312290-37F4-462E-A13D-1DDA737E97BF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{23F99948-81BD-4C18-8B63-7CCABA76B6A0}" name="Clock Src"/>
   </tableColumns>
@@ -3658,8 +3828,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="O33:P40" totalsRowShown="0">
-  <autoFilter ref="O33:P40" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="P33:Q40" totalsRowShown="0">
+  <autoFilter ref="P33:Q40" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3404615A-1121-4984-AE0D-5A1D34461BCA}" name="GPIO_Name"/>
     <tableColumn id="2" xr3:uid="{37ECDCD3-2CED-4177-80B2-3A88EFA9E7C2}" name="Number of pin"/>
@@ -3754,6 +3924,16 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}" name="FMKIO_IRQNHandler" displayName="FMKIO_IRQNHandler" ref="L21:L28" totalsRowShown="0">
+  <autoFilter ref="L21:L28" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{435A2CB3-E527-4D4E-9A3C-7D2BA856E09C}" name="List IRQN_Handler"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -3764,7 +3944,31 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}" name="FMKCPU_IRQNHandler" displayName="FMKCPU_IRQNHandler" ref="F4:G17" totalsRowShown="0">
+  <autoFilter ref="F4:G17" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C0EA827E-D0A1-4F96-9D94-60107C8F02D0}" name="List IRQN_Handler"/>
+    <tableColumn id="2" xr3:uid="{B344E14A-A089-45F4-9C1B-D978E362DC5A}" name="Timer Associated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="T20:W25" totalsRowShown="0">
+  <autoFilter ref="T20:W25" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
+    <tableColumn id="2" xr3:uid="{20DF5352-4B39-416D-A6E4-D94E56AED1C9}" name="number of channel"/>
+    <tableColumn id="3" xr3:uid="{9F9316C2-2066-47BF-B84E-436D4C41B07C}" name="IRQN assoiated"/>
+    <tableColumn id="4" xr3:uid="{CC116C4D-98B0-46BC-A882-0B90828FFD68}" name="Clock Associated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
   <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
   <tableColumns count="4">
@@ -3777,7 +3981,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
   <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
@@ -3790,20 +3994,18 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="S20:V25" totalsRowShown="0">
-  <autoFilter ref="S20:V25" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
-    <tableColumn id="2" xr3:uid="{20DF5352-4B39-416D-A6E4-D94E56AED1C9}" name="number of channel"/>
-    <tableColumn id="3" xr3:uid="{9F9316C2-2066-47BF-B84E-436D4C41B07C}" name="IRQN assoiated"/>
-    <tableColumn id="4" xr3:uid="{CC116C4D-98B0-46BC-A882-0B90828FFD68}" name="Clock Associated"/>
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}" name="FMKCDA_IRQNHandler" displayName="FMKCDA_IRQNHandler" ref="E8:F12" totalsRowShown="0">
+  <autoFilter ref="E8:F12" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CD80BAAD-36DA-496C-9F7C-D80D4296914C}" name="List IRQN_Handler"/>
+    <tableColumn id="2" xr3:uid="{9F8B466B-BFC7-4900-8330-976222B1008D}" name="Adc, Dac associated"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}" name="FMKMAC_Cfg" displayName="FMKMAC_Cfg" ref="B2:E9" totalsRowShown="0">
   <autoFilter ref="B2:E9" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}"/>
   <tableColumns count="4">
@@ -3816,9 +4018,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}" name="Tableau34" displayName="Tableau34" ref="J3:J18" totalsRowShown="0">
+  <autoFilter ref="J3:J18" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{7FC5E369-C5C5-44CD-98EF-8136D5348789}" name="List IRQN_Handler"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}" name="Tableau35" displayName="Tableau35" ref="B5:B11" totalsRowShown="0">
+  <autoFilter ref="B5:B11" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{61C0BDFB-C4E4-44F5-AA25-0ECEC1F95FDC}" name="List IRQN_Handler"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="X36:Y37" totalsRowShown="0">
-  <autoFilter ref="X36:Y37" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="Y36:Z37" totalsRowShown="0">
+  <autoFilter ref="Y36:Z37" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{73150C50-6B2A-4CD8-A7E6-62C171935AF8}" name="DAC_Name"/>
     <tableColumn id="2" xr3:uid="{EF9B5413-9A3C-4163-8063-C74DAB2D51F7}" name="number of channel"/>
@@ -3828,8 +4050,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}" name="GI_IRQN" displayName="GI_IRQN" ref="G18:H119" totalsRowShown="0">
-  <autoFilter ref="G18:H119" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}" name="GI_IRQN" displayName="GI_IRQN" ref="H18:I119" totalsRowShown="0">
+  <autoFilter ref="H18:I119" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{95486269-8ABF-444C-A7FD-956C784AC88B}" name="IRQN_name"/>
     <tableColumn id="2" xr3:uid="{72C5AB1D-5859-4FB9-812E-7971E444E4B8}" name="Interrupt Prioirty "/>
@@ -3839,19 +4061,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}" name="GI_RCC_CLOCK" displayName="GI_RCC_CLOCK" ref="D18:E75" totalsRowShown="0">
-  <autoFilter ref="D18:E75" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}" name="GI_RCC_CLOCK" displayName="GI_RCC_CLOCK" ref="D18:F75" totalsRowShown="0">
+  <autoFilter ref="D18:F75" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{402A3AD5-0AFA-40A5-A5A4-0D9CB2EED72D}" name="RCC_ClockName"/>
     <tableColumn id="2" xr3:uid="{05025EF0-98DC-4B06-8DD6-ABD9D73D50B7}" name="Clock Soure"/>
+    <tableColumn id="3" xr3:uid="{A98345EB-D57F-464A-8549-42B6B6F4ED23}" name="Request Periph Cfg"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="AA20:AC22" totalsRowShown="0">
-  <autoFilter ref="AA20:AC22" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="AB20:AD22" totalsRowShown="0">
+  <autoFilter ref="AB20:AD22" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00302DEC-D815-47CE-9380-676FE769FF43}" name="DMA_Name"/>
     <tableColumn id="2" xr3:uid="{2654BB85-F763-4BBA-9124-13A3875B62D0}" name="number of channel"/>
@@ -3862,8 +4085,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AE40:AE43" totalsRowShown="0">
-  <autoFilter ref="AE40:AE43" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AF40:AF43" totalsRowShown="0">
+  <autoFilter ref="AF40:AF43" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
   </tableColumns>
@@ -4198,10 +4421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="A18:AE119"/>
+  <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="U16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4210,27 +4433,27 @@
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" customWidth="1"/>
-    <col min="14" max="14" width="22.77734375" customWidth="1"/>
-    <col min="15" max="15" width="23.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" customWidth="1"/>
-    <col min="20" max="20" width="21.21875" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" customWidth="1"/>
-    <col min="22" max="22" width="18.77734375" customWidth="1"/>
-    <col min="23" max="23" width="29.21875" customWidth="1"/>
-    <col min="27" max="27" width="24" customWidth="1"/>
-    <col min="30" max="30" width="17.77734375" customWidth="1"/>
+    <col min="5" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="22.77734375" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" customWidth="1"/>
+    <col min="21" max="21" width="21.21875" customWidth="1"/>
+    <col min="22" max="22" width="19.109375" customWidth="1"/>
+    <col min="23" max="23" width="18.77734375" customWidth="1"/>
+    <col min="24" max="24" width="29.21875" customWidth="1"/>
+    <col min="28" max="28" width="24" customWidth="1"/>
+    <col min="31" max="31" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>132</v>
       </c>
@@ -4238,31 +4461,34 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>315</v>
-      </c>
-      <c r="G18" t="s">
+        <v>314</v>
+      </c>
+      <c r="F18" t="s">
+        <v>422</v>
+      </c>
+      <c r="H18" t="s">
         <v>57</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>58</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>2</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>3</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>282</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>283</v>
       </c>
-      <c r="N18" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>133</v>
       </c>
@@ -4270,333 +4496,357 @@
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>322</v>
-      </c>
-      <c r="G19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F19" t="s">
+        <v>420</v>
+      </c>
+      <c r="H19" t="s">
         <v>59</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>69</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>4</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>4</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>154</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>285</v>
       </c>
-      <c r="N19" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>240</v>
       </c>
       <c r="E20" t="s">
-        <v>322</v>
-      </c>
-      <c r="G20" t="s">
+        <v>321</v>
+      </c>
+      <c r="F20" t="s">
+        <v>420</v>
+      </c>
+      <c r="H20" t="s">
         <v>134</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>69</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>261</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>4</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>157</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>285</v>
       </c>
-      <c r="N20" t="s">
-        <v>312</v>
-      </c>
-      <c r="S20" t="s">
+      <c r="O20" t="s">
+        <v>311</v>
+      </c>
+      <c r="T20" t="s">
         <v>17</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>18</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>288</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>289</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AB20" t="s">
         <v>22</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>18</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>243</v>
       </c>
       <c r="E21" t="s">
-        <v>322</v>
-      </c>
-      <c r="G21" t="s">
+        <v>321</v>
+      </c>
+      <c r="F21" t="s">
+        <v>420</v>
+      </c>
+      <c r="H21" t="s">
         <v>135</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>69</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>5</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>4</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>64</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>285</v>
       </c>
-      <c r="N21" t="s">
-        <v>312</v>
-      </c>
-      <c r="S21" t="s">
+      <c r="O21" t="s">
+        <v>311</v>
+      </c>
+      <c r="T21" t="s">
         <v>16</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>18</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>148</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>247</v>
       </c>
-      <c r="AA21" t="s">
-        <v>350</v>
-      </c>
-      <c r="AB21">
+      <c r="AB21" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC21">
         <v>8</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>244</v>
       </c>
       <c r="E22" t="s">
-        <v>322</v>
-      </c>
-      <c r="G22" t="s">
+        <v>321</v>
+      </c>
+      <c r="F22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" t="s">
         <v>136</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>69</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>262</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>4</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>158</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>285</v>
       </c>
-      <c r="N22" t="s">
-        <v>312</v>
-      </c>
-      <c r="S22" t="s">
+      <c r="O22" t="s">
+        <v>311</v>
+      </c>
+      <c r="T22" t="s">
         <v>271</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>18</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>148</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
         <v>247</v>
       </c>
-      <c r="AA22" t="s">
-        <v>351</v>
-      </c>
-      <c r="AB22">
+      <c r="AB22" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC22">
         <v>8</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>245</v>
       </c>
       <c r="E23" t="s">
-        <v>322</v>
-      </c>
-      <c r="G23" t="s">
+        <v>321</v>
+      </c>
+      <c r="F23" t="s">
+        <v>420</v>
+      </c>
+      <c r="H23" t="s">
         <v>60</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>267</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>4</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>174</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>285</v>
       </c>
-      <c r="N23" t="s">
-        <v>312</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="O23" t="s">
+        <v>311</v>
+      </c>
+      <c r="T23" t="s">
         <v>272</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>18</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>171</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>246</v>
       </c>
       <c r="E24" t="s">
-        <v>322</v>
-      </c>
-      <c r="G24" t="s">
+        <v>321</v>
+      </c>
+      <c r="F24" t="s">
+        <v>420</v>
+      </c>
+      <c r="H24" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>69</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>263</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>178</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>287</v>
       </c>
-      <c r="N24" t="s">
-        <v>312</v>
-      </c>
-      <c r="S24" t="s">
+      <c r="O24" t="s">
+        <v>311</v>
+      </c>
+      <c r="T24" t="s">
         <v>273</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>18</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>185</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>322</v>
-      </c>
-      <c r="G25" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" t="s">
+        <v>420</v>
+      </c>
+      <c r="H25" t="s">
         <v>137</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>69</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>264</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>1</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>179</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>287</v>
       </c>
-      <c r="N25" t="s">
-        <v>313</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="O25" t="s">
+        <v>312</v>
+      </c>
+      <c r="T25" t="s">
         <v>274</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>18</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>186</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>270</v>
       </c>
       <c r="E26" t="s">
-        <v>323</v>
-      </c>
-      <c r="G26" t="s">
+        <v>322</v>
+      </c>
+      <c r="F26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H26" t="s">
         <v>138</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>69</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>265</v>
       </c>
-      <c r="K26">
-        <v>4</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="L26">
+        <v>6</v>
+      </c>
+      <c r="M26" t="s">
         <v>167</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>285</v>
       </c>
-      <c r="N26" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>292</v>
       </c>
@@ -4607,31 +4857,34 @@
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>323</v>
-      </c>
-      <c r="G27" t="s">
+        <v>322</v>
+      </c>
+      <c r="F27" t="s">
+        <v>420</v>
+      </c>
+      <c r="H27" t="s">
         <v>139</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>69</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>6</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>2</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>154</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>286</v>
       </c>
-      <c r="N27" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>293</v>
       </c>
@@ -4642,31 +4895,34 @@
         <v>241</v>
       </c>
       <c r="E28" t="s">
-        <v>323</v>
-      </c>
-      <c r="G28" t="s">
+        <v>322</v>
+      </c>
+      <c r="F28" t="s">
+        <v>420</v>
+      </c>
+      <c r="H28" t="s">
         <v>140</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>69</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>7</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>1</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>155</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>286</v>
       </c>
-      <c r="N28" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>256</v>
       </c>
@@ -4677,1169 +4933,1313 @@
         <v>242</v>
       </c>
       <c r="E29" t="s">
-        <v>323</v>
-      </c>
-      <c r="G29" t="s">
+        <v>322</v>
+      </c>
+      <c r="F29" t="s">
+        <v>420</v>
+      </c>
+      <c r="H29" t="s">
         <v>141</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>69</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>8</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>1</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>156</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>286</v>
       </c>
-      <c r="N29" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>323</v>
-      </c>
-      <c r="G30" t="s">
+        <v>322</v>
+      </c>
+      <c r="F30" t="s">
+        <v>420</v>
+      </c>
+      <c r="H30" t="s">
         <v>62</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>69</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>266</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>4</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>201</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>285</v>
       </c>
-      <c r="N30" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>323</v>
-      </c>
-      <c r="G31" t="s">
+        <v>322</v>
+      </c>
+      <c r="F31" t="s">
+        <v>420</v>
+      </c>
+      <c r="H31" t="s">
         <v>142</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>323</v>
-      </c>
-      <c r="G32" t="s">
+        <v>322</v>
+      </c>
+      <c r="F32" t="s">
+        <v>420</v>
+      </c>
+      <c r="H32" t="s">
         <v>143</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>247</v>
       </c>
       <c r="E33" t="s">
-        <v>321</v>
-      </c>
-      <c r="G33" t="s">
+        <v>320</v>
+      </c>
+      <c r="F33" t="s">
+        <v>421</v>
+      </c>
+      <c r="H33" t="s">
         <v>144</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>69</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>9</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>248</v>
       </c>
       <c r="E34" t="s">
-        <v>321</v>
-      </c>
-      <c r="G34" t="s">
+        <v>320</v>
+      </c>
+      <c r="F34" t="s">
+        <v>421</v>
+      </c>
+      <c r="H34" t="s">
         <v>145</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>69</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>11</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>239</v>
       </c>
       <c r="E35" t="s">
-        <v>313</v>
-      </c>
-      <c r="G35" t="s">
+        <v>312</v>
+      </c>
+      <c r="F35" t="s">
+        <v>420</v>
+      </c>
+      <c r="H35" t="s">
         <v>146</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>69</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>12</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>238</v>
       </c>
       <c r="E36" t="s">
-        <v>313</v>
-      </c>
-      <c r="G36" t="s">
+        <v>312</v>
+      </c>
+      <c r="F36" t="s">
+        <v>420</v>
+      </c>
+      <c r="H36" t="s">
         <v>147</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>69</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>13</v>
       </c>
-      <c r="P36">
+      <c r="Q36">
         <v>16</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>19</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>249</v>
       </c>
       <c r="E37" t="s">
-        <v>313</v>
-      </c>
-      <c r="G37" t="s">
+        <v>312</v>
+      </c>
+      <c r="F37" t="s">
+        <v>420</v>
+      </c>
+      <c r="H37" t="s">
         <v>148</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>69</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>14</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>16</v>
-      </c>
-      <c r="X37" t="s">
-        <v>20</v>
       </c>
       <c r="Y37" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="Z37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>250</v>
       </c>
       <c r="E38" t="s">
-        <v>313</v>
-      </c>
-      <c r="G38" t="s">
+        <v>312</v>
+      </c>
+      <c r="F38" t="s">
+        <v>420</v>
+      </c>
+      <c r="H38" t="s">
         <v>149</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>69</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>268</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>225</v>
       </c>
       <c r="E39" t="s">
-        <v>323</v>
-      </c>
-      <c r="G39" t="s">
+        <v>322</v>
+      </c>
+      <c r="F39" t="s">
+        <v>420</v>
+      </c>
+      <c r="H39" t="s">
         <v>150</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>69</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>15</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>251</v>
       </c>
       <c r="E40" t="s">
-        <v>323</v>
-      </c>
-      <c r="G40" t="s">
+        <v>322</v>
+      </c>
+      <c r="F40" t="s">
+        <v>420</v>
+      </c>
+      <c r="H40" t="s">
         <v>151</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>90</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>269</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
         <v>11</v>
       </c>
-      <c r="AE40" t="s">
+      <c r="AF40" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>252</v>
       </c>
       <c r="E41" t="s">
-        <v>320</v>
-      </c>
-      <c r="G41" t="s">
+        <v>319</v>
+      </c>
+      <c r="F41" t="s">
+        <v>421</v>
+      </c>
+      <c r="H41" t="s">
         <v>152</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>90</v>
       </c>
-      <c r="AE41" t="s">
+      <c r="AF41" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>237</v>
       </c>
       <c r="E42" t="s">
-        <v>312</v>
-      </c>
-      <c r="G42" t="s">
+        <v>311</v>
+      </c>
+      <c r="F42" t="s">
+        <v>420</v>
+      </c>
+      <c r="H42" t="s">
         <v>153</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>69</v>
       </c>
-      <c r="AE42" t="s">
+      <c r="AF42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>312</v>
-      </c>
-      <c r="G43" t="s">
+        <v>311</v>
+      </c>
+      <c r="F43" t="s">
+        <v>420</v>
+      </c>
+      <c r="H43" t="s">
         <v>154</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>69</v>
       </c>
-      <c r="AE43" t="s">
+      <c r="AF43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>236</v>
       </c>
       <c r="E44" t="s">
-        <v>312</v>
-      </c>
-      <c r="G44" t="s">
+        <v>311</v>
+      </c>
+      <c r="F44" t="s">
+        <v>420</v>
+      </c>
+      <c r="H44" t="s">
         <v>155</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>253</v>
       </c>
       <c r="E45" t="s">
-        <v>312</v>
-      </c>
-      <c r="G45" t="s">
+        <v>311</v>
+      </c>
+      <c r="F45" t="s">
+        <v>420</v>
+      </c>
+      <c r="H45" t="s">
         <v>156</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
         <v>235</v>
       </c>
       <c r="E46" t="s">
-        <v>312</v>
-      </c>
-      <c r="G46" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" t="s">
+        <v>420</v>
+      </c>
+      <c r="H46" t="s">
         <v>63</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>69</v>
       </c>
-      <c r="AE46" t="s">
+      <c r="AF46" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="47" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>234</v>
       </c>
       <c r="E47" t="s">
-        <v>312</v>
-      </c>
-      <c r="G47" t="s">
+        <v>311</v>
+      </c>
+      <c r="F47" t="s">
+        <v>420</v>
+      </c>
+      <c r="H47" t="s">
         <v>157</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>69</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AF47" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="48" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>254</v>
       </c>
       <c r="E48" t="s">
-        <v>312</v>
-      </c>
-      <c r="G48" t="s">
+        <v>311</v>
+      </c>
+      <c r="F48" t="s">
+        <v>420</v>
+      </c>
+      <c r="H48" t="s">
         <v>64</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>69</v>
       </c>
-      <c r="AE48" t="s">
+      <c r="AF48" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="49" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>255</v>
       </c>
       <c r="E49" t="s">
-        <v>312</v>
-      </c>
-      <c r="G49" t="s">
+        <v>311</v>
+      </c>
+      <c r="F49" t="s">
+        <v>420</v>
+      </c>
+      <c r="H49" t="s">
         <v>158</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>69</v>
       </c>
-      <c r="AE49" t="s">
+      <c r="AF49" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="50" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>312</v>
-      </c>
-      <c r="G50" t="s">
+        <v>311</v>
+      </c>
+      <c r="F50" t="s">
+        <v>420</v>
+      </c>
+      <c r="H50" t="s">
         <v>159</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>312</v>
-      </c>
-      <c r="G51" t="s">
+        <v>311</v>
+      </c>
+      <c r="F51" t="s">
+        <v>420</v>
+      </c>
+      <c r="H51" t="s">
         <v>160</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>230</v>
       </c>
       <c r="E52" t="s">
-        <v>312</v>
-      </c>
-      <c r="G52" t="s">
+        <v>311</v>
+      </c>
+      <c r="F52" t="s">
+        <v>420</v>
+      </c>
+      <c r="H52" t="s">
         <v>161</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>69</v>
       </c>
-      <c r="AE52" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="53" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF52" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>312</v>
-      </c>
-      <c r="G53" t="s">
+        <v>311</v>
+      </c>
+      <c r="F53" t="s">
+        <v>421</v>
+      </c>
+      <c r="H53" t="s">
         <v>162</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>69</v>
       </c>
-      <c r="AE53" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="54" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF53" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="54" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>229</v>
       </c>
       <c r="E54" t="s">
-        <v>312</v>
-      </c>
-      <c r="G54" t="s">
+        <v>311</v>
+      </c>
+      <c r="F54" t="s">
+        <v>421</v>
+      </c>
+      <c r="H54" t="s">
         <v>65</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>69</v>
       </c>
-      <c r="AE54" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="55" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF54" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="55" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>290</v>
       </c>
       <c r="E55" t="s">
-        <v>312</v>
-      </c>
-      <c r="G55" t="s">
+        <v>311</v>
+      </c>
+      <c r="F55" t="s">
+        <v>421</v>
+      </c>
+      <c r="H55" t="s">
         <v>66</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>69</v>
       </c>
-      <c r="AE55" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="56" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF55" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="56" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>291</v>
       </c>
       <c r="E56" t="s">
-        <v>312</v>
-      </c>
-      <c r="G56" t="s">
+        <v>311</v>
+      </c>
+      <c r="F56" t="s">
+        <v>421</v>
+      </c>
+      <c r="H56" t="s">
         <v>67</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>69</v>
       </c>
-      <c r="AE56" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="57" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF56" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="57" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>228</v>
       </c>
       <c r="E57" t="s">
-        <v>312</v>
-      </c>
-      <c r="G57" t="s">
+        <v>311</v>
+      </c>
+      <c r="F57" t="s">
+        <v>420</v>
+      </c>
+      <c r="H57" t="s">
         <v>68</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>69</v>
       </c>
-      <c r="AE57" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="58" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF57" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="58" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>226</v>
       </c>
       <c r="E58" t="s">
-        <v>312</v>
-      </c>
-      <c r="G58" t="s">
+        <v>311</v>
+      </c>
+      <c r="F58" t="s">
+        <v>420</v>
+      </c>
+      <c r="H58" t="s">
         <v>163</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>69</v>
       </c>
-      <c r="AE58" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="59" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF58" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="59" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>256</v>
       </c>
       <c r="E59" t="s">
-        <v>320</v>
-      </c>
-      <c r="G59" t="s">
+        <v>319</v>
+      </c>
+      <c r="F59" t="s">
+        <v>421</v>
+      </c>
+      <c r="H59" t="s">
         <v>164</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>69</v>
       </c>
-      <c r="AE59" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="60" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF59" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="60" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>87</v>
       </c>
       <c r="E60" t="s">
+        <v>311</v>
+      </c>
+      <c r="F60" t="s">
+        <v>420</v>
+      </c>
+      <c r="H60" t="s">
+        <v>165</v>
+      </c>
+      <c r="I60" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF60" t="s">
         <v>312</v>
       </c>
-      <c r="G60" t="s">
-        <v>165</v>
-      </c>
-      <c r="H60" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE60" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="61" spans="4:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>227</v>
       </c>
       <c r="E61" t="s">
-        <v>312</v>
-      </c>
-      <c r="G61" t="s">
+        <v>311</v>
+      </c>
+      <c r="F61" t="s">
+        <v>421</v>
+      </c>
+      <c r="H61" t="s">
         <v>166</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>69</v>
       </c>
-      <c r="AE61" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="62" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF61" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>231</v>
       </c>
       <c r="E62" t="s">
-        <v>312</v>
-      </c>
-      <c r="G62" t="s">
+        <v>311</v>
+      </c>
+      <c r="F62" t="s">
+        <v>420</v>
+      </c>
+      <c r="H62" t="s">
         <v>167</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>69</v>
       </c>
-      <c r="AE62" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="63" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="AF62" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="63" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>257</v>
       </c>
       <c r="E63" t="s">
-        <v>312</v>
-      </c>
-      <c r="G63" t="s">
+        <v>311</v>
+      </c>
+      <c r="F63" t="s">
+        <v>420</v>
+      </c>
+      <c r="H63" t="s">
         <v>168</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>313</v>
-      </c>
-      <c r="G64" t="s">
+        <v>312</v>
+      </c>
+      <c r="F64" t="s">
+        <v>420</v>
+      </c>
+      <c r="H64" t="s">
         <v>169</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>313</v>
-      </c>
-      <c r="G65" t="s">
+        <v>312</v>
+      </c>
+      <c r="F65" t="s">
+        <v>420</v>
+      </c>
+      <c r="H65" t="s">
         <v>170</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>313</v>
-      </c>
-      <c r="G66" t="s">
+        <v>312</v>
+      </c>
+      <c r="F66" t="s">
+        <v>420</v>
+      </c>
+      <c r="H66" t="s">
         <v>171</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>313</v>
-      </c>
-      <c r="G67" t="s">
+        <v>312</v>
+      </c>
+      <c r="F67" t="s">
+        <v>420</v>
+      </c>
+      <c r="H67" t="s">
         <v>172</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>313</v>
-      </c>
-      <c r="G68" t="s">
+        <v>312</v>
+      </c>
+      <c r="F68" t="s">
+        <v>421</v>
+      </c>
+      <c r="H68" t="s">
         <v>173</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
         <v>258</v>
       </c>
       <c r="E69" t="s">
-        <v>313</v>
-      </c>
-      <c r="G69" t="s">
+        <v>312</v>
+      </c>
+      <c r="F69" t="s">
+        <v>420</v>
+      </c>
+      <c r="H69" t="s">
         <v>174</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>313</v>
-      </c>
-      <c r="G70" t="s">
+        <v>312</v>
+      </c>
+      <c r="F70" t="s">
+        <v>420</v>
+      </c>
+      <c r="H70" t="s">
         <v>175</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
         <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>313</v>
-      </c>
-      <c r="G71" t="s">
+        <v>312</v>
+      </c>
+      <c r="F71" t="s">
+        <v>420</v>
+      </c>
+      <c r="H71" t="s">
         <v>176</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>313</v>
-      </c>
-      <c r="G72" t="s">
+        <v>312</v>
+      </c>
+      <c r="F72" t="s">
+        <v>420</v>
+      </c>
+      <c r="H72" t="s">
         <v>177</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
         <v>232</v>
       </c>
       <c r="E73" t="s">
-        <v>313</v>
-      </c>
-      <c r="G73" t="s">
+        <v>312</v>
+      </c>
+      <c r="F73" t="s">
+        <v>420</v>
+      </c>
+      <c r="H73" t="s">
         <v>178</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
         <v>259</v>
       </c>
       <c r="E74" t="s">
-        <v>313</v>
-      </c>
-      <c r="G74" t="s">
+        <v>312</v>
+      </c>
+      <c r="F74" t="s">
+        <v>420</v>
+      </c>
+      <c r="H74" t="s">
         <v>179</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>260</v>
       </c>
       <c r="E75" t="s">
-        <v>313</v>
-      </c>
-      <c r="G75" t="s">
+        <v>312</v>
+      </c>
+      <c r="F75" t="s">
+        <v>420</v>
+      </c>
+      <c r="H75" t="s">
         <v>180</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G76" t="s">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H76" t="s">
         <v>181</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G77" t="s">
+    <row r="77" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H77" t="s">
         <v>182</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G78" t="s">
+    <row r="78" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H78" t="s">
         <v>183</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G79" t="s">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H79" t="s">
         <v>184</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G80" t="s">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H80" t="s">
         <v>185</v>
       </c>
-      <c r="H80" t="s">
+      <c r="I80" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G81" t="s">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
         <v>186</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G82" t="s">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H82" t="s">
         <v>187</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G83" t="s">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H83" t="s">
         <v>188</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G84" t="s">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H84" t="s">
         <v>189</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G85" t="s">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H85" t="s">
         <v>190</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G86" t="s">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H86" t="s">
         <v>191</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G87" t="s">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H87" t="s">
         <v>192</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G88" t="s">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H88" t="s">
         <v>193</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G89" t="s">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H89" t="s">
         <v>194</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G90" t="s">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H90" t="s">
         <v>195</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G91" t="s">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H91" t="s">
         <v>196</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G92" t="s">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H92" t="s">
         <v>197</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G93" t="s">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H93" t="s">
         <v>198</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G94" t="s">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H94" t="s">
         <v>199</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G95" t="s">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H95" t="s">
         <v>200</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G96" t="s">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H96" t="s">
         <v>201</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G97" t="s">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H97" t="s">
         <v>202</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G98" t="s">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H98" t="s">
         <v>203</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G99" t="s">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H99" t="s">
         <v>204</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G100" t="s">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H100" t="s">
         <v>205</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G101" t="s">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H101" t="s">
         <v>206</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G102" t="s">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H102" t="s">
         <v>207</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G103" t="s">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H103" t="s">
         <v>208</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G104" t="s">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H104" t="s">
         <v>209</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G105" t="s">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H105" t="s">
         <v>210</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G106" t="s">
+    <row r="106" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H106" t="s">
         <v>211</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G107" t="s">
+    <row r="107" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H107" t="s">
         <v>212</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G108" t="s">
+    <row r="108" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H108" t="s">
         <v>213</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G109" t="s">
+    <row r="109" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H109" t="s">
         <v>214</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G110" t="s">
+    <row r="110" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H110" t="s">
         <v>215</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G111" t="s">
+    <row r="111" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H111" t="s">
         <v>216</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G112" t="s">
+    <row r="112" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H112" t="s">
         <v>217</v>
       </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G113" t="s">
+    <row r="113" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H113" t="s">
         <v>218</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G114" t="s">
+    <row r="114" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H114" t="s">
         <v>219</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G115" t="s">
+    <row r="115" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H115" t="s">
         <v>220</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G116" t="s">
+    <row r="116" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H116" t="s">
         <v>221</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G117" t="s">
+    <row r="117" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H117" t="s">
         <v>222</v>
       </c>
-      <c r="H117" t="s">
+      <c r="I117" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G118" t="s">
+    <row r="118" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H118" t="s">
         <v>223</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G119" t="s">
+    <row r="119" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H119" t="s">
         <v>224</v>
       </c>
-      <c r="H119" t="s">
+      <c r="I119" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18:H119" xr:uid="{3E8F037A-5A22-4138-A36A-F90B67434DDA}">
-      <formula1>$AE$41:$AE$43</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I18:I119" xr:uid="{AAB57854-EE21-4648-A1CB-0F7D2F2AF990}">
+      <formula1>$AF$41:$AF$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M30" xr:uid="{17DBAA90-8141-4522-B025-71F13961596F}">
-      <formula1>$AE$47:$AE$49</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N30" xr:uid="{FCBABE9C-10FE-40A4-8AA4-1BAED7C63E26}">
+      <formula1>$AF$47:$AF$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N30 E19:E75" xr:uid="{C93913E9-44DA-490C-8435-4DAABE3AC990}">
-      <formula1>$AE$53:$AE$62</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O19:O30 E19:E75" xr:uid="{FB123359-30B9-419B-AE41-551AB7BB7CAB}">
+      <formula1>$AF$53:$AF$62</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19:F75" xr:uid="{FBAC43ED-7412-4717-84C1-361BAB253D8D}">
+      <formula1>"No,Yes"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5865,8 +6265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6428,15 +6828,33 @@
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
       <c r="Q18" s="4"/>
     </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>381</v>
+      </c>
+    </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>310</v>
+      <c r="L23" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>300</v>
       </c>
+      <c r="L24" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -6457,6 +6875,9 @@
       <c r="F25" t="s">
         <v>309</v>
       </c>
+      <c r="L25" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -6477,6 +6898,9 @@
       <c r="F26" t="s">
         <v>306</v>
       </c>
+      <c r="L26" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -6497,6 +6921,9 @@
       <c r="F27" t="s">
         <v>308</v>
       </c>
+      <c r="L27" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -6517,6 +6944,9 @@
       <c r="F28" t="s">
         <v>307</v>
       </c>
+      <c r="L28" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AW29" t="s">
@@ -6561,7 +6991,7 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AW33" t="s">
         <v>28</v>
@@ -6590,7 +7020,7 @@
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -6616,7 +7046,7 @@
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
@@ -6642,7 +7072,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F36" t="s">
         <v>290</v>
@@ -6857,7 +7287,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 B7:B15 F7:F16 AA8:AA16 Q7:Q14 W7:W8 K7:K9" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
       <formula1>$AW$30:$AW$45</formula1>
     </dataValidation>
@@ -6870,7 +7300,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="14">
+  <tableParts count="15">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -6885,25 +7315,26 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C3D18C3-7241-4088-8034-07AAE0EB53A9}">
           <x14:formula1>
-            <xm:f>General_Info!$J$19:$J$30</xm:f>
+            <xm:f>General_Info!$K$19:$K$30</xm:f>
           </x14:formula1>
           <xm:sqref>S7:S14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA00DA78-9682-47F8-B701-D35809CE3FB0}">
           <x14:formula1>
-            <xm:f>General_Info!$O$34:$O$39</xm:f>
+            <xm:f>General_Info!$P$34:$P$39</xm:f>
           </x14:formula1>
-          <xm:sqref>J7:J9 V7:V8 P7:P14 Z8:Z16 E7:E16 A7:A15</xm:sqref>
+          <xm:sqref>J7:J9 A7:A15 E7:E16 Z8:Z16 P7:P14 V7:V8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
           <x14:formula1>
-            <xm:f>General_Info!$S$21:$S$25</xm:f>
+            <xm:f>General_Info!$T$21:$T$25</xm:f>
           </x14:formula1>
           <xm:sqref>G6:G16</xm:sqref>
         </x14:dataValidation>
@@ -6915,62 +7346,178 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E52BA6-3E0A-4F7C-9391-164B38476F25}">
-  <dimension ref="B3:C6"/>
+  <dimension ref="B3:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>373</v>
+      </c>
+      <c r="G4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>368</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>369</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>370</v>
+      </c>
+      <c r="G9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>371</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>372</v>
+      </c>
+      <c r="G11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>374</v>
+      </c>
+      <c r="G12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>375</v>
+      </c>
+      <c r="G13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>377</v>
+      </c>
+      <c r="G15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>378</v>
+      </c>
+      <c r="G16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>379</v>
+      </c>
+      <c r="G17" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
-  <dimension ref="I2:V5"/>
+  <dimension ref="E2:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
     <col min="9" max="9" width="43.88671875" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" customWidth="1"/>
@@ -6982,7 +7529,7 @@
     <col min="22" max="22" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
         <v>127</v>
       </c>
@@ -6990,7 +7537,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="9:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
         <v>123</v>
       </c>
@@ -7016,7 +7563,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="9:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>122</v>
       </c>
@@ -7042,7 +7589,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="9:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
         <v>278</v>
       </c>
@@ -7054,18 +7601,64 @@
       </c>
       <c r="L5" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>388</v>
+      </c>
+      <c r="F9" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="10" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>389</v>
+      </c>
+      <c r="F10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>390</v>
+      </c>
+      <c r="F11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>391</v>
+      </c>
+      <c r="F12" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AB0981D-B484-49AA-81E2-46EA728857EF}">
           <x14:formula1>
             <xm:f>FMK_IO!$BA$30:$BA$47</xm:f>
@@ -7074,13 +7667,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
           <x14:formula1>
-            <xm:f>General_Info!$S$21:$S$25</xm:f>
+            <xm:f>General_Info!$T$21:$T$25</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
           <x14:formula1>
-            <xm:f>General_Info!W37</xm:f>
+            <xm:f>General_Info!X37</xm:f>
           </x14:formula1>
           <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>
@@ -7092,10 +7685,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E18236-E25D-41B3-8B1E-0194276152B3}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J2" sqref="J2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7103,42 +7696,49 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" t="s">
         <v>352</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>353</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>354</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D3" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D3" t="s">
-        <v>356</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -7146,13 +7746,16 @@
       <c r="E4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D5" t="s">
         <v>92</v>
@@ -7160,13 +7763,16 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7174,13 +7780,16 @@
       <c r="E6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7188,33 +7797,151 @@
       <c r="E7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D8" t="s">
         <v>359</v>
-      </c>
-      <c r="C8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D8" t="s">
-        <v>360</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D9" t="s">
         <v>361</v>
-      </c>
-      <c r="C9" t="s">
-        <v>350</v>
-      </c>
-      <c r="D9" t="s">
-        <v>362</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D1D4C8-FD0D-4DBE-B311-5297C41CC83F}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -7225,7 +7952,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85D06B3-E762-495B-BF06-A6CD7E704A4C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860CCB6B-9BC8-4B28-B4AE-B22F38F81573}">
   <dimension ref="B1:P254"/>
   <sheetViews>
@@ -7245,7 +7984,7 @@
   <sheetData>
     <row r="1" spans="3:14" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D1" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
@@ -7255,10 +7994,10 @@
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -7271,19 +8010,19 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>326</v>
+      </c>
+      <c r="E7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" t="s">
+        <v>323</v>
+      </c>
+      <c r="G7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J7" t="s">
         <v>327</v>
-      </c>
-      <c r="E7" t="s">
-        <v>326</v>
-      </c>
-      <c r="F7" t="s">
-        <v>324</v>
-      </c>
-      <c r="G7" t="s">
-        <v>325</v>
-      </c>
-      <c r="J7" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -7305,7 +8044,7 @@
         <v>2519.6453599155921</v>
       </c>
       <c r="M8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -7316,12 +8055,12 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L13">
         <v>63997</v>
@@ -7349,10 +8088,10 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -7387,15 +8126,15 @@
     </row>
     <row r="27" spans="2:16" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D27" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -7407,39 +8146,39 @@
         <v>0.5</v>
       </c>
       <c r="M29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
+        <v>337</v>
+      </c>
+      <c r="E30" t="s">
         <v>338</v>
       </c>
-      <c r="E30" t="s">
-        <v>339</v>
-      </c>
       <c r="F30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I30" t="s">
+        <v>344</v>
+      </c>
+      <c r="J30" t="s">
+        <v>342</v>
+      </c>
+      <c r="K30" t="s">
         <v>345</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
+        <v>346</v>
+      </c>
+      <c r="M30" t="s">
         <v>343</v>
       </c>
-      <c r="K30" t="s">
-        <v>346</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>347</v>
-      </c>
-      <c r="M30" t="s">
-        <v>344</v>
-      </c>
-      <c r="O30" t="s">
-        <v>348</v>
       </c>
       <c r="P30" t="e">
         <f>2^#REF!</f>

</xml_diff>

<commit_message>
Update Code Gen FMKMAC and the module associated
Update Config SPecific for all module
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5833EA-70C0-4B7A-B819-F4E31DA08974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F50AF80-7BBA-4846-B338-6866A16FA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="429">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1312,6 +1312,24 @@
   </si>
   <si>
     <t>Request Periph Cfg</t>
+  </si>
+  <si>
+    <t>USART2_RX</t>
+  </si>
+  <si>
+    <t>USART2_TX</t>
+  </si>
+  <si>
+    <t>RqstType Associated</t>
+  </si>
+  <si>
+    <t>put ',' if two channel in one IRQN Handler</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>DMAMUX List</t>
   </si>
 </sst>
 </file>
@@ -4006,8 +4024,8 @@
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}" name="FMKMAC_Cfg" displayName="FMKMAC_Cfg" ref="B2:E9" totalsRowShown="0">
-  <autoFilter ref="B2:E9" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}" name="FMKMAC_Cfg" displayName="FMKMAC_Cfg" ref="B2:E11" totalsRowShown="0">
+  <autoFilter ref="B2:E11" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9B6EDCAA-F526-412C-A8EC-AC6897A0EB04}" name="RqstDmaType"/>
     <tableColumn id="2" xr3:uid="{ED583461-6D2B-456F-A394-15F76B273D8C}" name="DMA "/>
@@ -4019,16 +4037,27 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}" name="Tableau34" displayName="Tableau34" ref="J3:J18" totalsRowShown="0">
-  <autoFilter ref="J3:J18" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}" name="FMKMAC_IRQN" displayName="FMKMAC_IRQN" ref="J3:K18" totalsRowShown="0">
+  <autoFilter ref="J3:K18" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7FC5E369-C5C5-44CD-98EF-8136D5348789}" name="List IRQN_Handler"/>
+    <tableColumn id="2" xr3:uid="{0FFD83C8-633F-48FF-B94F-239B6386B204}" name="RqstType Associated"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{9E75F4B3-8C66-44CB-A927-82E8A09563A2}" name="FMKMAC_DMAMUX" displayName="FMKMAC_DMAMUX" ref="P3:P4" totalsRowShown="0">
+  <autoFilter ref="P3:P4" xr:uid="{9E75F4B3-8C66-44CB-A927-82E8A09563A2}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{230DEE15-D20F-429D-B4EB-51FB3C57F9A9}" name="DMAMUX List"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}" name="Tableau35" displayName="Tableau35" ref="B5:B11" totalsRowShown="0">
   <autoFilter ref="B5:B11" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}"/>
   <tableColumns count="1">
@@ -4423,8 +4452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView topLeftCell="M7" zoomScale="45" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD49" sqref="AD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7685,10 +7714,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E18236-E25D-41B3-8B1E-0194276152B3}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7697,9 +7726,11 @@
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>351</v>
       </c>
@@ -7716,7 +7747,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>348</v>
       </c>
@@ -7732,10 +7763,16 @@
       <c r="J3" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>425</v>
+      </c>
+      <c r="P3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>427</v>
       </c>
       <c r="C4" t="s">
         <v>349</v>
@@ -7749,10 +7786,19 @@
       <c r="J4" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>348</v>
+      </c>
+      <c r="L4" t="s">
+        <v>426</v>
+      </c>
+      <c r="P4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>417</v>
       </c>
       <c r="C5" t="s">
         <v>349</v>
@@ -7766,13 +7812,16 @@
       <c r="J5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7783,13 +7832,16 @@
       <c r="J6" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>357</v>
       </c>
       <c r="C7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7800,8 +7852,11 @@
       <c r="J7" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>358</v>
       </c>
@@ -7817,8 +7872,11 @@
       <c r="J8" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>360</v>
       </c>
@@ -7834,38 +7892,74 @@
       <c r="J9" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>423</v>
+      </c>
+      <c r="C10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
       <c r="J10" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
       <c r="J11" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
         <v>404</v>
       </c>
@@ -7882,9 +7976,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7968,7 +8063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860CCB6B-9BC8-4B28-B4AE-B22F38F81573}">
   <dimension ref="B1:P254"/>
   <sheetViews>
-    <sheetView topLeftCell="E27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A205" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Transmit with DMA working, error was DMa Init Periph To Memory for Rx but Memory to Periph for Tx
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F50AF80-7BBA-4846-B338-6866A16FA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D5DBA9-C898-48EF-8C64-B35A615FB15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -945,9 +945,6 @@
     <t xml:space="preserve">Others USART configuration </t>
   </si>
   <si>
-    <t>OthersCAN configuration</t>
-  </si>
-  <si>
     <t>GPIO_AF9_FDCAN1</t>
   </si>
   <si>
@@ -1330,6 +1327,9 @@
   </si>
   <si>
     <t>DMAMUX List</t>
+  </si>
+  <si>
+    <t>CAN configuration</t>
   </si>
 </sst>
 </file>
@@ -4452,7 +4452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="M7" zoomScale="45" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="O9" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AD49" sqref="AD49"/>
     </sheetView>
   </sheetViews>
@@ -4490,10 +4490,10 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -4514,7 +4514,7 @@
         <v>283</v>
       </c>
       <c r="O18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
@@ -4525,10 +4525,10 @@
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -4549,7 +4549,7 @@
         <v>285</v>
       </c>
       <c r="O19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
@@ -4557,10 +4557,10 @@
         <v>240</v>
       </c>
       <c r="E20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H20" t="s">
         <v>134</v>
@@ -4581,7 +4581,7 @@
         <v>285</v>
       </c>
       <c r="O20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T20" t="s">
         <v>17</v>
@@ -4610,10 +4610,10 @@
         <v>243</v>
       </c>
       <c r="E21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H21" t="s">
         <v>135</v>
@@ -4634,7 +4634,7 @@
         <v>285</v>
       </c>
       <c r="O21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T21" t="s">
         <v>16</v>
@@ -4649,7 +4649,7 @@
         <v>247</v>
       </c>
       <c r="AB21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AC21">
         <v>8</v>
@@ -4663,10 +4663,10 @@
         <v>244</v>
       </c>
       <c r="E22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H22" t="s">
         <v>136</v>
@@ -4687,7 +4687,7 @@
         <v>285</v>
       </c>
       <c r="O22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T22" t="s">
         <v>271</v>
@@ -4702,7 +4702,7 @@
         <v>247</v>
       </c>
       <c r="AB22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC22">
         <v>8</v>
@@ -4716,10 +4716,10 @@
         <v>245</v>
       </c>
       <c r="E23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
@@ -4740,7 +4740,7 @@
         <v>285</v>
       </c>
       <c r="O23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T23" t="s">
         <v>272</v>
@@ -4760,10 +4760,10 @@
         <v>246</v>
       </c>
       <c r="E24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H24" t="s">
         <v>61</v>
@@ -4784,7 +4784,7 @@
         <v>287</v>
       </c>
       <c r="O24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T24" t="s">
         <v>273</v>
@@ -4804,10 +4804,10 @@
         <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H25" t="s">
         <v>137</v>
@@ -4828,7 +4828,7 @@
         <v>287</v>
       </c>
       <c r="O25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T25" t="s">
         <v>274</v>
@@ -4848,10 +4848,10 @@
         <v>270</v>
       </c>
       <c r="E26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H26" t="s">
         <v>138</v>
@@ -4872,7 +4872,7 @@
         <v>285</v>
       </c>
       <c r="O26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
@@ -4886,10 +4886,10 @@
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H27" t="s">
         <v>139</v>
@@ -4910,7 +4910,7 @@
         <v>286</v>
       </c>
       <c r="O27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -4924,10 +4924,10 @@
         <v>241</v>
       </c>
       <c r="E28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H28" t="s">
         <v>140</v>
@@ -4948,7 +4948,7 @@
         <v>286</v>
       </c>
       <c r="O28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -4962,10 +4962,10 @@
         <v>242</v>
       </c>
       <c r="E29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H29" t="s">
         <v>141</v>
@@ -4986,7 +4986,7 @@
         <v>286</v>
       </c>
       <c r="O29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -4994,10 +4994,10 @@
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -5018,7 +5018,7 @@
         <v>285</v>
       </c>
       <c r="O30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -5026,10 +5026,10 @@
         <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F31" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H31" t="s">
         <v>142</v>
@@ -5043,10 +5043,10 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H32" t="s">
         <v>143</v>
@@ -5060,10 +5060,10 @@
         <v>247</v>
       </c>
       <c r="E33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F33" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H33" t="s">
         <v>144</v>
@@ -5083,10 +5083,10 @@
         <v>248</v>
       </c>
       <c r="E34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H34" t="s">
         <v>145</v>
@@ -5106,10 +5106,10 @@
         <v>239</v>
       </c>
       <c r="E35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H35" t="s">
         <v>146</v>
@@ -5129,10 +5129,10 @@
         <v>238</v>
       </c>
       <c r="E36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F36" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H36" t="s">
         <v>147</v>
@@ -5158,10 +5158,10 @@
         <v>249</v>
       </c>
       <c r="E37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H37" t="s">
         <v>148</v>
@@ -5187,10 +5187,10 @@
         <v>250</v>
       </c>
       <c r="E38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H38" t="s">
         <v>149</v>
@@ -5210,10 +5210,10 @@
         <v>225</v>
       </c>
       <c r="E39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F39" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H39" t="s">
         <v>150</v>
@@ -5233,10 +5233,10 @@
         <v>251</v>
       </c>
       <c r="E40" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F40" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H40" t="s">
         <v>151</v>
@@ -5259,10 +5259,10 @@
         <v>252</v>
       </c>
       <c r="E41" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F41" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H41" t="s">
         <v>152</v>
@@ -5279,10 +5279,10 @@
         <v>237</v>
       </c>
       <c r="E42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H42" t="s">
         <v>153</v>
@@ -5299,10 +5299,10 @@
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F43" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H43" t="s">
         <v>154</v>
@@ -5319,10 +5319,10 @@
         <v>236</v>
       </c>
       <c r="E44" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H44" t="s">
         <v>155</v>
@@ -5336,10 +5336,10 @@
         <v>253</v>
       </c>
       <c r="E45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H45" t="s">
         <v>156</v>
@@ -5353,10 +5353,10 @@
         <v>235</v>
       </c>
       <c r="E46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -5373,10 +5373,10 @@
         <v>234</v>
       </c>
       <c r="E47" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F47" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H47" t="s">
         <v>157</v>
@@ -5393,10 +5393,10 @@
         <v>254</v>
       </c>
       <c r="E48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H48" t="s">
         <v>64</v>
@@ -5413,10 +5413,10 @@
         <v>255</v>
       </c>
       <c r="E49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F49" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H49" t="s">
         <v>158</v>
@@ -5433,10 +5433,10 @@
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F50" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H50" t="s">
         <v>159</v>
@@ -5450,10 +5450,10 @@
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F51" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H51" t="s">
         <v>160</v>
@@ -5467,10 +5467,10 @@
         <v>230</v>
       </c>
       <c r="E52" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F52" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H52" t="s">
         <v>161</v>
@@ -5479,7 +5479,7 @@
         <v>69</v>
       </c>
       <c r="AF52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="4:32" x14ac:dyDescent="0.3">
@@ -5487,10 +5487,10 @@
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F53" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H53" t="s">
         <v>162</v>
@@ -5499,7 +5499,7 @@
         <v>69</v>
       </c>
       <c r="AF53" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="54" spans="4:32" x14ac:dyDescent="0.3">
@@ -5507,10 +5507,10 @@
         <v>229</v>
       </c>
       <c r="E54" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F54" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H54" t="s">
         <v>65</v>
@@ -5519,7 +5519,7 @@
         <v>69</v>
       </c>
       <c r="AF54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="4:32" x14ac:dyDescent="0.3">
@@ -5527,10 +5527,10 @@
         <v>290</v>
       </c>
       <c r="E55" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F55" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H55" t="s">
         <v>66</v>
@@ -5539,7 +5539,7 @@
         <v>69</v>
       </c>
       <c r="AF55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="4:32" x14ac:dyDescent="0.3">
@@ -5547,10 +5547,10 @@
         <v>291</v>
       </c>
       <c r="E56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F56" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H56" t="s">
         <v>67</v>
@@ -5559,7 +5559,7 @@
         <v>69</v>
       </c>
       <c r="AF56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="4:32" x14ac:dyDescent="0.3">
@@ -5567,10 +5567,10 @@
         <v>228</v>
       </c>
       <c r="E57" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F57" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H57" t="s">
         <v>68</v>
@@ -5579,7 +5579,7 @@
         <v>69</v>
       </c>
       <c r="AF57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.3">
@@ -5587,10 +5587,10 @@
         <v>226</v>
       </c>
       <c r="E58" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F58" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H58" t="s">
         <v>163</v>
@@ -5599,7 +5599,7 @@
         <v>69</v>
       </c>
       <c r="AF58" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.3">
@@ -5607,10 +5607,10 @@
         <v>256</v>
       </c>
       <c r="E59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F59" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H59" t="s">
         <v>164</v>
@@ -5619,7 +5619,7 @@
         <v>69</v>
       </c>
       <c r="AF59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="60" spans="4:32" x14ac:dyDescent="0.3">
@@ -5627,10 +5627,10 @@
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F60" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H60" t="s">
         <v>165</v>
@@ -5639,7 +5639,7 @@
         <v>69</v>
       </c>
       <c r="AF60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" spans="4:32" x14ac:dyDescent="0.3">
@@ -5647,10 +5647,10 @@
         <v>227</v>
       </c>
       <c r="E61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F61" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H61" t="s">
         <v>166</v>
@@ -5659,7 +5659,7 @@
         <v>69</v>
       </c>
       <c r="AF61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62" spans="4:32" x14ac:dyDescent="0.3">
@@ -5667,10 +5667,10 @@
         <v>231</v>
       </c>
       <c r="E62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F62" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H62" t="s">
         <v>167</v>
@@ -5679,7 +5679,7 @@
         <v>69</v>
       </c>
       <c r="AF62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="4:32" x14ac:dyDescent="0.3">
@@ -5687,10 +5687,10 @@
         <v>257</v>
       </c>
       <c r="E63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F63" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H63" t="s">
         <v>168</v>
@@ -5704,10 +5704,10 @@
         <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F64" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H64" t="s">
         <v>169</v>
@@ -5721,10 +5721,10 @@
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F65" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H65" t="s">
         <v>170</v>
@@ -5738,10 +5738,10 @@
         <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F66" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H66" t="s">
         <v>171</v>
@@ -5755,10 +5755,10 @@
         <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F67" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H67" t="s">
         <v>172</v>
@@ -5772,10 +5772,10 @@
         <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F68" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H68" t="s">
         <v>173</v>
@@ -5789,10 +5789,10 @@
         <v>258</v>
       </c>
       <c r="E69" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F69" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H69" t="s">
         <v>174</v>
@@ -5806,10 +5806,10 @@
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F70" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H70" t="s">
         <v>175</v>
@@ -5823,10 +5823,10 @@
         <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F71" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H71" t="s">
         <v>176</v>
@@ -5840,10 +5840,10 @@
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F72" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H72" t="s">
         <v>177</v>
@@ -5857,10 +5857,10 @@
         <v>232</v>
       </c>
       <c r="E73" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F73" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H73" t="s">
         <v>178</v>
@@ -5874,10 +5874,10 @@
         <v>259</v>
       </c>
       <c r="E74" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F74" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H74" t="s">
         <v>179</v>
@@ -5891,10 +5891,10 @@
         <v>260</v>
       </c>
       <c r="E75" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H75" t="s">
         <v>180</v>
@@ -6294,8 +6294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6859,53 +6859,53 @@
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>428</v>
       </c>
       <c r="L24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25" t="s">
         <v>302</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>303</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>304</v>
-      </c>
-      <c r="D25" t="s">
-        <v>305</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.3">
@@ -6922,13 +6922,13 @@
         <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
@@ -6945,13 +6945,13 @@
         <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
@@ -6968,13 +6968,13 @@
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
@@ -7020,7 +7020,7 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AW33" t="s">
         <v>28</v>
@@ -7034,22 +7034,22 @@
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>301</v>
+      </c>
+      <c r="B34" t="s">
         <v>302</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>303</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>304</v>
-      </c>
-      <c r="D34" t="s">
-        <v>305</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -7075,7 +7075,7 @@
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
@@ -7101,7 +7101,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F36" t="s">
         <v>290</v>
@@ -7392,7 +7392,7 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -7403,10 +7403,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -7417,7 +7417,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -7431,7 +7431,7 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -7439,7 +7439,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -7447,7 +7447,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -7455,7 +7455,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G9" t="s">
         <v>261</v>
@@ -7463,7 +7463,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -7471,7 +7471,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G11" t="s">
         <v>262</v>
@@ -7479,7 +7479,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G12" t="s">
         <v>263</v>
@@ -7487,7 +7487,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G13" t="s">
         <v>264</v>
@@ -7495,7 +7495,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G14" t="s">
         <v>266</v>
@@ -7503,7 +7503,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G15" t="s">
         <v>266</v>
@@ -7511,7 +7511,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G16" t="s">
         <v>266</v>
@@ -7519,7 +7519,7 @@
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G17" t="s">
         <v>266</v>
@@ -7634,47 +7634,47 @@
     </row>
     <row r="7" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -7716,7 +7716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E18236-E25D-41B3-8B1E-0194276152B3}">
   <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -7732,50 +7732,50 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" t="s">
         <v>351</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>352</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>353</v>
       </c>
-      <c r="E2" t="s">
-        <v>354</v>
-      </c>
       <c r="J2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" t="s">
         <v>348</v>
       </c>
-      <c r="C3" t="s">
-        <v>349</v>
-      </c>
       <c r="D3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -7784,13 +7784,13 @@
         <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P4" t="s">
         <v>243</v>
@@ -7798,10 +7798,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D5" t="s">
         <v>92</v>
@@ -7810,18 +7810,18 @@
         <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7830,18 +7830,18 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7850,58 +7850,58 @@
         <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D8" t="s">
         <v>358</v>
-      </c>
-      <c r="C8" t="s">
-        <v>349</v>
-      </c>
-      <c r="D8" t="s">
-        <v>359</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>359</v>
+      </c>
+      <c r="C9" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" t="s">
         <v>360</v>
-      </c>
-      <c r="C9" t="s">
-        <v>349</v>
-      </c>
-      <c r="D9" t="s">
-        <v>361</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -7910,18 +7910,18 @@
         <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -7930,48 +7930,48 @@
         <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -7996,47 +7996,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -8079,7 +8079,7 @@
   <sheetData>
     <row r="1" spans="3:14" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D1" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
@@ -8089,10 +8089,10 @@
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -8105,19 +8105,19 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>325</v>
+      </c>
+      <c r="E7" t="s">
+        <v>324</v>
+      </c>
+      <c r="F7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G7" t="s">
+        <v>323</v>
+      </c>
+      <c r="J7" t="s">
         <v>326</v>
-      </c>
-      <c r="E7" t="s">
-        <v>325</v>
-      </c>
-      <c r="F7" t="s">
-        <v>323</v>
-      </c>
-      <c r="G7" t="s">
-        <v>324</v>
-      </c>
-      <c r="J7" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -8139,7 +8139,7 @@
         <v>2519.6453599155921</v>
       </c>
       <c r="M8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -8150,12 +8150,12 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L13">
         <v>63997</v>
@@ -8183,10 +8183,10 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -8221,15 +8221,15 @@
     </row>
     <row r="27" spans="2:16" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D27" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -8241,39 +8241,39 @@
         <v>0.5</v>
       </c>
       <c r="M29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
+        <v>336</v>
+      </c>
+      <c r="E30" t="s">
         <v>337</v>
       </c>
-      <c r="E30" t="s">
-        <v>338</v>
-      </c>
       <c r="F30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I30" t="s">
+        <v>343</v>
+      </c>
+      <c r="J30" t="s">
+        <v>341</v>
+      </c>
+      <c r="K30" t="s">
         <v>344</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
+        <v>345</v>
+      </c>
+      <c r="M30" t="s">
         <v>342</v>
       </c>
-      <c r="K30" t="s">
-        <v>345</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>346</v>
-      </c>
-      <c r="M30" t="s">
-        <v>343</v>
-      </c>
-      <c r="O30" t="s">
-        <v>347</v>
       </c>
       <c r="P30" t="e">
         <f>2^#REF!</f>

</xml_diff>

<commit_message>
Code Generation for FMKSRL, [to be tested]
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D5DBA9-C898-48EF-8C64-B35A615FB15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A3135-3098-4DE5-8AC9-98CFF3AE8BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="438">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1330,6 +1330,33 @@
   </si>
   <si>
     <t>CAN configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRQN_Handler </t>
+  </si>
+  <si>
+    <t>List USART/UART</t>
+  </si>
+  <si>
+    <t>USART1_IRQHandler</t>
+  </si>
+  <si>
+    <t>USART2_IRQHandler</t>
+  </si>
+  <si>
+    <t>USART3_IRQHandler</t>
+  </si>
+  <si>
+    <t>UART4_IRQHandler</t>
+  </si>
+  <si>
+    <t>UART5_IRQHandler</t>
+  </si>
+  <si>
+    <t>Rx Buffer Size</t>
+  </si>
+  <si>
+    <t>Tx Buffer Size</t>
   </si>
 </sst>
 </file>
@@ -4067,6 +4094,19 @@
 </table>
 </file>
 
+<file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}" name="FMKSRL_INFO" displayName="FMKSRL_INFO" ref="E2:H7" totalsRowShown="0">
+  <autoFilter ref="E2:H7" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{12502774-1323-464D-ABF1-A64EAE0742C0}" name="List USART/UART"/>
+    <tableColumn id="2" xr3:uid="{73C1FD75-5549-419D-8E5F-A6563E10AE3C}" name="IRQN_Handler "/>
+    <tableColumn id="3" xr3:uid="{51FF6EA1-88DA-48AF-B204-9E7E41DF7DE2}" name="Rx Buffer Size"/>
+    <tableColumn id="4" xr3:uid="{0B3BF550-8B6E-4A05-8D50-A860E7703D9A}" name="Tx Buffer Size"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="Y36:Z37" totalsRowShown="0">
   <autoFilter ref="Y36:Z37" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
@@ -4452,7 +4492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="O9" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AD49" sqref="AD49"/>
     </sheetView>
   </sheetViews>
@@ -6294,7 +6334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -8049,13 +8089,102 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85D06B3-E762-495B-BF06-A6CD7E704A4C}">
-  <dimension ref="A1"/>
+  <dimension ref="E2:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F2" t="s">
+        <v>429</v>
+      </c>
+      <c r="G2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>431</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G4">
+        <v>256</v>
+      </c>
+      <c r="H4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>290</v>
+      </c>
+      <c r="F6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G6">
+        <v>256</v>
+      </c>
+      <c r="H6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" t="s">
+        <v>435</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Work ON ADC And Documentation
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A3135-3098-4DE5-8AC9-98CFF3AE8BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81AD52-11C9-4CF5-8A02-184D02DA2F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="442">
   <si>
     <t>Colonne1</t>
   </si>
@@ -420,9 +420,6 @@
     <t>Put in this array the name and address for calibration for reference tension Vref for each adc</t>
   </si>
   <si>
-    <t>VREFINT_CAL</t>
-  </si>
-  <si>
     <t>Vref Calib</t>
   </si>
   <si>
@@ -1357,6 +1354,21 @@
   </si>
   <si>
     <t>Tx Buffer Size</t>
+  </si>
+  <si>
+    <t>VREFINT_CAL_1</t>
+  </si>
+  <si>
+    <t>VREFINT_CAL_2</t>
+  </si>
+  <si>
+    <t>VREFINT_CAL_3</t>
+  </si>
+  <si>
+    <t>VREFINT_CAL_4</t>
+  </si>
+  <si>
+    <t>VREFINT_CAL_5</t>
   </si>
 </sst>
 </file>
@@ -4027,8 +4039,8 @@
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
-  <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V8" totalsRowShown="0">
+  <autoFilter ref="S3:V8" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0BCC2BC4-7FF0-4C14-809D-9D95A3225151}" name="Vref Calib"/>
     <tableColumn id="2" xr3:uid="{0E78A6D4-DF9E-4966-A80E-64FE5BD9F1E2}" name="address  hexacecimal"/>
@@ -4492,7 +4504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="N15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AD49" sqref="AD49"/>
     </sheetView>
   </sheetViews>
@@ -4524,16 +4536,16 @@
   <sheetData>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -4548,27 +4560,27 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
+        <v>281</v>
+      </c>
+      <c r="N18" t="s">
         <v>282</v>
       </c>
-      <c r="N18" t="s">
-        <v>283</v>
-      </c>
       <c r="O18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s">
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F19" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -4583,45 +4595,45 @@
         <v>4</v>
       </c>
       <c r="M19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I20" t="s">
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L20">
         <v>4</v>
       </c>
       <c r="M20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T20" t="s">
         <v>17</v>
@@ -4630,10 +4642,10 @@
         <v>18</v>
       </c>
       <c r="V20" t="s">
+        <v>287</v>
+      </c>
+      <c r="W20" t="s">
         <v>288</v>
-      </c>
-      <c r="W20" t="s">
-        <v>289</v>
       </c>
       <c r="AB20" t="s">
         <v>22</v>
@@ -4642,21 +4654,21 @@
         <v>18</v>
       </c>
       <c r="AD20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I21" t="s">
         <v>69</v>
@@ -4671,10 +4683,10 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T21" t="s">
         <v>16</v>
@@ -4683,13 +4695,13 @@
         <v>18</v>
       </c>
       <c r="V21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AB21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AC21">
         <v>8</v>
@@ -4700,66 +4712,66 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I22" t="s">
         <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L22">
         <v>4</v>
       </c>
       <c r="M22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U22">
         <v>18</v>
       </c>
       <c r="V22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AB22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AC22">
         <v>8</v>
       </c>
       <c r="AD22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
@@ -4768,42 +4780,42 @@
         <v>69</v>
       </c>
       <c r="K23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L23">
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U23">
         <v>18</v>
       </c>
       <c r="V23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H24" t="s">
         <v>61</v>
@@ -4812,31 +4824,31 @@
         <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U24">
         <v>18</v>
       </c>
       <c r="V24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
@@ -4844,95 +4856,95 @@
         <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
         <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U25">
         <v>18</v>
       </c>
       <c r="V25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I26" t="s">
         <v>69</v>
       </c>
       <c r="K26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L26">
         <v>6</v>
       </c>
       <c r="M26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I27" t="s">
         <v>69</v>
@@ -4944,33 +4956,33 @@
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B28">
         <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I28" t="s">
         <v>69</v>
@@ -4982,33 +4994,33 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B29">
         <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I29" t="s">
         <v>69</v>
@@ -5020,13 +5032,13 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -5034,10 +5046,10 @@
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -5046,19 +5058,19 @@
         <v>69</v>
       </c>
       <c r="K30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L30">
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -5066,13 +5078,13 @@
         <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I31" t="s">
         <v>69</v>
@@ -5083,13 +5095,13 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I32" t="s">
         <v>69</v>
@@ -5097,16 +5109,16 @@
     </row>
     <row r="33" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I33" t="s">
         <v>69</v>
@@ -5120,16 +5132,16 @@
     </row>
     <row r="34" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I34" t="s">
         <v>69</v>
@@ -5143,16 +5155,16 @@
     </row>
     <row r="35" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E35" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I35" t="s">
         <v>69</v>
@@ -5166,16 +5178,16 @@
     </row>
     <row r="36" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I36" t="s">
         <v>69</v>
@@ -5195,16 +5207,16 @@
     </row>
     <row r="37" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E37" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I37" t="s">
         <v>69</v>
@@ -5224,22 +5236,22 @@
     </row>
     <row r="38" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I38" t="s">
         <v>69</v>
       </c>
       <c r="P38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q38">
         <v>16</v>
@@ -5247,16 +5259,16 @@
     </row>
     <row r="39" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F39" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I39" t="s">
         <v>69</v>
@@ -5270,22 +5282,22 @@
     </row>
     <row r="40" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F40" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I40" t="s">
         <v>90</v>
       </c>
       <c r="P40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q40">
         <v>11</v>
@@ -5296,16 +5308,16 @@
     </row>
     <row r="41" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F41" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I41" t="s">
         <v>90</v>
@@ -5316,16 +5328,16 @@
     </row>
     <row r="42" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I42" t="s">
         <v>69</v>
@@ -5339,13 +5351,13 @@
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F43" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I43" t="s">
         <v>69</v>
@@ -5356,16 +5368,16 @@
     </row>
     <row r="44" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I44" t="s">
         <v>69</v>
@@ -5373,16 +5385,16 @@
     </row>
     <row r="45" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I45" t="s">
         <v>69</v>
@@ -5390,13 +5402,13 @@
     </row>
     <row r="46" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F46" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -5405,38 +5417,38 @@
         <v>69</v>
       </c>
       <c r="AF46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I47" t="s">
         <v>69</v>
       </c>
       <c r="AF47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H48" t="s">
         <v>64</v>
@@ -5445,27 +5457,27 @@
         <v>69</v>
       </c>
       <c r="AF48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F49" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I49" t="s">
         <v>69</v>
       </c>
       <c r="AF49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="4:32" x14ac:dyDescent="0.3">
@@ -5473,13 +5485,13 @@
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I50" t="s">
         <v>69</v>
@@ -5490,13 +5502,13 @@
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F51" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I51" t="s">
         <v>69</v>
@@ -5504,22 +5516,22 @@
     </row>
     <row r="52" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F52" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I52" t="s">
         <v>69</v>
       </c>
       <c r="AF52" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="4:32" x14ac:dyDescent="0.3">
@@ -5527,30 +5539,30 @@
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F53" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I53" t="s">
         <v>69</v>
       </c>
       <c r="AF53" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F54" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H54" t="s">
         <v>65</v>
@@ -5559,18 +5571,18 @@
         <v>69</v>
       </c>
       <c r="AF54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="55" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E55" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F55" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H55" t="s">
         <v>66</v>
@@ -5579,18 +5591,18 @@
         <v>69</v>
       </c>
       <c r="AF55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E56" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H56" t="s">
         <v>67</v>
@@ -5599,18 +5611,18 @@
         <v>69</v>
       </c>
       <c r="AF56" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E57" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F57" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H57" t="s">
         <v>68</v>
@@ -5619,47 +5631,47 @@
         <v>69</v>
       </c>
       <c r="AF57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F58" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I58" t="s">
         <v>69</v>
       </c>
       <c r="AF58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F59" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I59" t="s">
         <v>69</v>
       </c>
       <c r="AF59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="4:32" x14ac:dyDescent="0.3">
@@ -5667,73 +5679,73 @@
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F60" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I60" t="s">
         <v>69</v>
       </c>
       <c r="AF60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F61" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I61" t="s">
         <v>69</v>
       </c>
       <c r="AF61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="62" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H62" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I62" t="s">
         <v>69</v>
       </c>
       <c r="AF62" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="63" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F63" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I63" t="s">
         <v>69</v>
@@ -5744,13 +5756,13 @@
         <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F64" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I64" t="s">
         <v>69</v>
@@ -5761,13 +5773,13 @@
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F65" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I65" t="s">
         <v>69</v>
@@ -5778,13 +5790,13 @@
         <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F66" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H66" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I66" t="s">
         <v>69</v>
@@ -5792,16 +5804,16 @@
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F67" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I67" t="s">
         <v>69</v>
@@ -5812,13 +5824,13 @@
         <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F68" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H68" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I68" t="s">
         <v>69</v>
@@ -5826,16 +5838,16 @@
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I69" t="s">
         <v>69</v>
@@ -5846,13 +5858,13 @@
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F70" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I70" t="s">
         <v>69</v>
@@ -5863,13 +5875,13 @@
         <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F71" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I71" t="s">
         <v>69</v>
@@ -5880,13 +5892,13 @@
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H72" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I72" t="s">
         <v>69</v>
@@ -5894,16 +5906,16 @@
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E73" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F73" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I73" t="s">
         <v>69</v>
@@ -5911,16 +5923,16 @@
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E74" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F74" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I74" t="s">
         <v>69</v>
@@ -5928,16 +5940,16 @@
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I75" t="s">
         <v>69</v>
@@ -5945,7 +5957,7 @@
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I76" t="s">
         <v>69</v>
@@ -5953,7 +5965,7 @@
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H77" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I77" t="s">
         <v>69</v>
@@ -5961,7 +5973,7 @@
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I78" t="s">
         <v>69</v>
@@ -5969,7 +5981,7 @@
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I79" t="s">
         <v>69</v>
@@ -5977,7 +5989,7 @@
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I80" t="s">
         <v>69</v>
@@ -5985,7 +5997,7 @@
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I81" t="s">
         <v>69</v>
@@ -5993,7 +6005,7 @@
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I82" t="s">
         <v>69</v>
@@ -6001,7 +6013,7 @@
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I83" t="s">
         <v>69</v>
@@ -6009,7 +6021,7 @@
     </row>
     <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I84" t="s">
         <v>69</v>
@@ -6017,7 +6029,7 @@
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I85" t="s">
         <v>69</v>
@@ -6025,7 +6037,7 @@
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I86" t="s">
         <v>69</v>
@@ -6033,7 +6045,7 @@
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I87" t="s">
         <v>69</v>
@@ -6041,7 +6053,7 @@
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I88" t="s">
         <v>69</v>
@@ -6049,7 +6061,7 @@
     </row>
     <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I89" t="s">
         <v>69</v>
@@ -6057,7 +6069,7 @@
     </row>
     <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I90" t="s">
         <v>69</v>
@@ -6065,7 +6077,7 @@
     </row>
     <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I91" t="s">
         <v>69</v>
@@ -6073,7 +6085,7 @@
     </row>
     <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H92" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I92" t="s">
         <v>69</v>
@@ -6081,7 +6093,7 @@
     </row>
     <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H93" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I93" t="s">
         <v>69</v>
@@ -6089,7 +6101,7 @@
     </row>
     <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H94" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I94" t="s">
         <v>69</v>
@@ -6097,7 +6109,7 @@
     </row>
     <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H95" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I95" t="s">
         <v>69</v>
@@ -6105,7 +6117,7 @@
     </row>
     <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I96" t="s">
         <v>69</v>
@@ -6113,7 +6125,7 @@
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H97" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I97" t="s">
         <v>69</v>
@@ -6121,7 +6133,7 @@
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H98" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I98" t="s">
         <v>69</v>
@@ -6129,7 +6141,7 @@
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I99" t="s">
         <v>69</v>
@@ -6137,7 +6149,7 @@
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H100" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I100" t="s">
         <v>69</v>
@@ -6145,7 +6157,7 @@
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H101" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I101" t="s">
         <v>69</v>
@@ -6153,7 +6165,7 @@
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H102" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I102" t="s">
         <v>69</v>
@@ -6161,7 +6173,7 @@
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H103" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I103" t="s">
         <v>69</v>
@@ -6169,7 +6181,7 @@
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H104" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I104" t="s">
         <v>90</v>
@@ -6177,7 +6189,7 @@
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H105" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I105" t="s">
         <v>90</v>
@@ -6185,7 +6197,7 @@
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H106" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I106" t="s">
         <v>90</v>
@@ -6193,7 +6205,7 @@
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H107" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I107" t="s">
         <v>90</v>
@@ -6201,7 +6213,7 @@
     </row>
     <row r="108" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H108" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I108" t="s">
         <v>69</v>
@@ -6209,7 +6221,7 @@
     </row>
     <row r="109" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H109" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I109" t="s">
         <v>69</v>
@@ -6217,7 +6229,7 @@
     </row>
     <row r="110" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H110" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I110" t="s">
         <v>69</v>
@@ -6225,7 +6237,7 @@
     </row>
     <row r="111" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I111" t="s">
         <v>69</v>
@@ -6233,7 +6245,7 @@
     </row>
     <row r="112" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H112" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I112" t="s">
         <v>69</v>
@@ -6241,7 +6253,7 @@
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H113" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I113" t="s">
         <v>69</v>
@@ -6249,7 +6261,7 @@
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H114" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I114" t="s">
         <v>69</v>
@@ -6257,7 +6269,7 @@
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H115" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I115" t="s">
         <v>69</v>
@@ -6265,7 +6277,7 @@
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H116" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I116" t="s">
         <v>69</v>
@@ -6273,7 +6285,7 @@
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H117" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I117" t="s">
         <v>69</v>
@@ -6281,7 +6293,7 @@
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H118" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I118" t="s">
         <v>69</v>
@@ -6289,7 +6301,7 @@
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H119" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I119" t="s">
         <v>69</v>
@@ -6334,8 +6346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A9" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6383,13 +6395,13 @@
         <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P5" t="s">
         <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="V5" t="s">
         <v>55</v>
@@ -6477,16 +6489,16 @@
         <v>100</v>
       </c>
       <c r="J7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K7" t="s">
         <v>27</v>
       </c>
       <c r="L7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N7" t="s">
         <v>45</v>
@@ -6498,7 +6510,7 @@
         <v>32</v>
       </c>
       <c r="R7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S7" t="s">
         <v>5</v>
@@ -6513,7 +6525,7 @@
         <v>35</v>
       </c>
       <c r="X7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z7" t="s">
         <v>23</v>
@@ -6542,13 +6554,13 @@
         <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K8" t="s">
         <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
@@ -6563,7 +6575,7 @@
         <v>31</v>
       </c>
       <c r="R8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S8" t="s">
         <v>5</v>
@@ -6578,7 +6590,7 @@
         <v>29</v>
       </c>
       <c r="X8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z8" t="s">
         <v>12</v>
@@ -6607,13 +6619,13 @@
         <v>102</v>
       </c>
       <c r="J9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K9" t="s">
         <v>29</v>
       </c>
       <c r="L9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
@@ -6628,10 +6640,10 @@
         <v>38</v>
       </c>
       <c r="R9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="S9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T9" t="s">
         <v>45</v>
@@ -6669,10 +6681,10 @@
         <v>39</v>
       </c>
       <c r="R10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="S10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T10" t="s">
         <v>46</v>
@@ -6698,7 +6710,7 @@
         <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H11" t="s">
         <v>97</v>
@@ -6710,10 +6722,10 @@
         <v>40</v>
       </c>
       <c r="R11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="S11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T11" t="s">
         <v>92</v>
@@ -6739,7 +6751,7 @@
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H12" t="s">
         <v>98</v>
@@ -6751,10 +6763,10 @@
         <v>41</v>
       </c>
       <c r="R12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="S12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T12" t="s">
         <v>50</v>
@@ -6792,10 +6804,10 @@
         <v>31</v>
       </c>
       <c r="R13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="S13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T13" t="s">
         <v>45</v>
@@ -6833,10 +6845,10 @@
         <v>32</v>
       </c>
       <c r="R14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="S14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T14" t="s">
         <v>46</v>
@@ -6899,53 +6911,53 @@
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>300</v>
+      </c>
+      <c r="B25" t="s">
         <v>301</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>302</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>303</v>
-      </c>
-      <c r="D25" t="s">
-        <v>304</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.3">
@@ -6962,59 +6974,59 @@
         <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
@@ -7060,7 +7072,7 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AW33" t="s">
         <v>28</v>
@@ -7074,22 +7086,22 @@
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>300</v>
+      </c>
+      <c r="B34" t="s">
         <v>301</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>302</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>303</v>
-      </c>
-      <c r="D34" t="s">
-        <v>304</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -7115,7 +7127,7 @@
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
@@ -7141,10 +7153,10 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AW36" t="s">
         <v>31</v>
@@ -7280,7 +7292,7 @@
         <v>115</v>
       </c>
       <c r="R77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="11:21" x14ac:dyDescent="0.3">
@@ -7417,7 +7429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E52BA6-3E0A-4F7C-9391-164B38476F25}">
   <dimension ref="B3:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -7432,7 +7444,7 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -7443,10 +7455,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -7457,7 +7469,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -7471,7 +7483,7 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -7479,7 +7491,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -7487,7 +7499,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -7495,15 +7507,15 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -7511,58 +7523,58 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -7579,8 +7591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
   <dimension ref="E2:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7600,7 +7612,7 @@
   <sheetData>
     <row r="2" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>124</v>
@@ -7611,25 +7623,25 @@
         <v>123</v>
       </c>
       <c r="J3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>128</v>
+      </c>
+      <c r="S3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" t="s">
         <v>130</v>
       </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" t="s">
         <v>128</v>
-      </c>
-      <c r="L3" t="s">
-        <v>129</v>
-      </c>
-      <c r="S3" t="s">
-        <v>126</v>
-      </c>
-      <c r="T3" t="s">
-        <v>131</v>
-      </c>
-      <c r="U3" t="s">
-        <v>128</v>
-      </c>
-      <c r="V3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="5:22" x14ac:dyDescent="0.3">
@@ -7637,7 +7649,7 @@
         <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -7646,10 +7658,10 @@
         <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>125</v>
+        <v>437</v>
       </c>
       <c r="T4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
@@ -7660,61 +7672,111 @@
     </row>
     <row r="5" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L5" t="s">
         <v>98</v>
       </c>
+      <c r="S5" t="s">
+        <v>438</v>
+      </c>
+      <c r="T5" t="s">
+        <v>280</v>
+      </c>
+      <c r="U5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="S6" t="s">
+        <v>439</v>
+      </c>
+      <c r="T6" t="s">
+        <v>280</v>
+      </c>
+      <c r="U6" t="s">
+        <v>271</v>
+      </c>
+      <c r="V6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="7" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>379</v>
+        <v>378</v>
+      </c>
+      <c r="S7" t="s">
+        <v>440</v>
+      </c>
+      <c r="T7" t="s">
+        <v>280</v>
+      </c>
+      <c r="U7" t="s">
+        <v>272</v>
+      </c>
+      <c r="V7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F8" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="S8" t="s">
+        <v>441</v>
+      </c>
+      <c r="T8" t="s">
+        <v>280</v>
+      </c>
+      <c r="U8" t="s">
+        <v>273</v>
+      </c>
+      <c r="V8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -7727,24 +7789,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AB0981D-B484-49AA-81E2-46EA728857EF}">
           <x14:formula1>
             <xm:f>FMK_IO!$BA$30:$BA$47</xm:f>
           </x14:formula1>
-          <xm:sqref>V4 L4:L5</xm:sqref>
+          <xm:sqref>L4:L5 V4:V8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
           <x14:formula1>
             <xm:f>General_Info!$T$21:$T$25</xm:f>
           </x14:formula1>
-          <xm:sqref>K4:K5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
-          <x14:formula1>
-            <xm:f>General_Info!X37</xm:f>
-          </x14:formula1>
-          <xm:sqref>U4</xm:sqref>
+          <xm:sqref>K4:K5 U4:U8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7757,7 +7813,7 @@
   <dimension ref="B2:P18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7772,50 +7828,50 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
         <v>350</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>351</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>352</v>
       </c>
-      <c r="E2" t="s">
-        <v>353</v>
-      </c>
       <c r="J2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" t="s">
         <v>347</v>
       </c>
-      <c r="C3" t="s">
-        <v>348</v>
-      </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -7824,24 +7880,24 @@
         <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D5" t="s">
         <v>92</v>
@@ -7850,18 +7906,18 @@
         <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7870,18 +7926,18 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7890,58 +7946,58 @@
         <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D8" t="s">
         <v>357</v>
-      </c>
-      <c r="C8" t="s">
-        <v>348</v>
-      </c>
-      <c r="D8" t="s">
-        <v>358</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" t="s">
         <v>359</v>
-      </c>
-      <c r="C9" t="s">
-        <v>348</v>
-      </c>
-      <c r="D9" t="s">
-        <v>360</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -7950,18 +8006,18 @@
         <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -7970,48 +8026,48 @@
         <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -8036,47 +8092,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -8091,8 +8147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85D06B3-E762-495B-BF06-A6CD7E704A4C}">
   <dimension ref="E2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8100,20 +8156,22 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H2" t="s">
         <v>436</v>
-      </c>
-      <c r="H2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="3" spans="5:8" x14ac:dyDescent="0.3">
@@ -8121,7 +8179,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -8135,7 +8193,7 @@
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G4">
         <v>256</v>
@@ -8146,18 +8204,18 @@
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G6">
         <v>256</v>
@@ -8168,10 +8226,10 @@
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -8208,7 +8266,7 @@
   <sheetData>
     <row r="1" spans="3:14" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
@@ -8218,10 +8276,10 @@
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -8234,19 +8292,19 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G7" t="s">
+        <v>322</v>
+      </c>
+      <c r="J7" t="s">
         <v>325</v>
-      </c>
-      <c r="E7" t="s">
-        <v>324</v>
-      </c>
-      <c r="F7" t="s">
-        <v>322</v>
-      </c>
-      <c r="G7" t="s">
-        <v>323</v>
-      </c>
-      <c r="J7" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -8268,7 +8326,7 @@
         <v>2519.6453599155921</v>
       </c>
       <c r="M8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -8279,12 +8337,12 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L13">
         <v>63997</v>
@@ -8312,10 +8370,10 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -8350,15 +8408,15 @@
     </row>
     <row r="27" spans="2:16" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D27" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -8370,39 +8428,39 @@
         <v>0.5</v>
       </c>
       <c r="M29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
+        <v>335</v>
+      </c>
+      <c r="E30" t="s">
         <v>336</v>
       </c>
-      <c r="E30" t="s">
-        <v>337</v>
-      </c>
       <c r="F30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I30" t="s">
+        <v>342</v>
+      </c>
+      <c r="J30" t="s">
+        <v>340</v>
+      </c>
+      <c r="K30" t="s">
         <v>343</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
+        <v>344</v>
+      </c>
+      <c r="M30" t="s">
         <v>341</v>
       </c>
-      <c r="K30" t="s">
-        <v>344</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>345</v>
-      </c>
-      <c r="M30" t="s">
-        <v>342</v>
-      </c>
-      <c r="O30" t="s">
-        <v>346</v>
       </c>
       <c r="P30" t="e">
         <f>2^#REF!</f>

</xml_diff>

<commit_message>
Tx_Rx Mode working in DMA Mode
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_UartDesignImpl\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81AD52-11C9-4CF5-8A02-184D02DA2F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0055E5-4462-478E-904B-498319B4F725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="446">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1369,6 +1369,18 @@
   </si>
   <si>
     <t>VREFINT_CAL_5</t>
+  </si>
+  <si>
+    <t>GPIO_AF7_USART1</t>
+  </si>
+  <si>
+    <t>GPIO_AF7_USART3</t>
+  </si>
+  <si>
+    <t>GPIO_AF8_UART5</t>
+  </si>
+  <si>
+    <t>GPIO_AF14_UART4</t>
   </si>
 </sst>
 </file>
@@ -4107,13 +4119,18 @@
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}" name="FMKSRL_INFO" displayName="FMKSRL_INFO" ref="E2:H7" totalsRowShown="0">
-  <autoFilter ref="E2:H7" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}" name="FMKSRL_INFO" displayName="FMKSRL_INFO" ref="E2:M7" totalsRowShown="0">
+  <autoFilter ref="E2:M7" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{12502774-1323-464D-ABF1-A64EAE0742C0}" name="List USART/UART"/>
     <tableColumn id="2" xr3:uid="{73C1FD75-5549-419D-8E5F-A6563E10AE3C}" name="IRQN_Handler "/>
     <tableColumn id="3" xr3:uid="{51FF6EA1-88DA-48AF-B204-9E7E41DF7DE2}" name="Rx Buffer Size"/>
     <tableColumn id="4" xr3:uid="{0B3BF550-8B6E-4A05-8D50-A860E7703D9A}" name="Tx Buffer Size"/>
+    <tableColumn id="5" xr3:uid="{6D86083F-0334-4F94-BB1A-53D1074988B3}" name="Rx_GPIO_name"/>
+    <tableColumn id="6" xr3:uid="{386C4D1D-01F5-4796-8676-B3D0ACAF503C}" name="RxPin_name"/>
+    <tableColumn id="7" xr3:uid="{A5D26E27-EB27-44C5-9EC3-C28B26CCAA76}" name="Tx_Gpio_Name"/>
+    <tableColumn id="8" xr3:uid="{2F846358-5341-48BB-8F3B-6C6370021E51}" name="Tx_Pin_Name"/>
+    <tableColumn id="9" xr3:uid="{81B54DFD-A22D-46F2-8062-B9CA25246E06}" name="alternate function timer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6346,8 +6363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A6" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7591,7 +7608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
   <dimension ref="E2:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
@@ -8145,10 +8162,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85D06B3-E762-495B-BF06-A6CD7E704A4C}">
-  <dimension ref="E2:H7"/>
+  <dimension ref="E2:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8158,9 +8175,14 @@
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
         <v>429</v>
       </c>
@@ -8173,8 +8195,23 @@
       <c r="H2" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="3" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J2" t="s">
+        <v>301</v>
+      </c>
+      <c r="K2" t="s">
+        <v>302</v>
+      </c>
+      <c r="L2" t="s">
+        <v>303</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>78</v>
       </c>
@@ -8187,8 +8224,23 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>268</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>79</v>
       </c>
@@ -8201,16 +8253,46 @@
       <c r="H4">
         <v>256</v>
       </c>
-    </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>228</v>
       </c>
       <c r="F5" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>268</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>268</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>289</v>
       </c>
@@ -8223,8 +8305,23 @@
       <c r="H6">
         <v>256</v>
       </c>
-    </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>268</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>268</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>290</v>
       </c>
@@ -8237,8 +8334,24 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7" t="s">
+        <v>268</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>268</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" t="s">
+        <v>444</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Start Design Drive CL42T
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_Ecdr_Htim\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_DrvStepper\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CFF432-CDFF-40D2-9F11-B1B2B8B1ECC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08782A85-2B53-4E15-BD9B-94B0FB1FA8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -6366,8 +6366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7388,7 +7388,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 B7:B15 F7:F16 AA8:AA16 Q7:Q14 W7:W8 K7:K9" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
       <formula1>$AW$30:$AW$45</formula1>
     </dataValidation>
@@ -7420,7 +7420,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C3D18C3-7241-4088-8034-07AAE0EB53A9}">
           <x14:formula1>
             <xm:f>General_Info!$K$19:$K$30</xm:f>
@@ -7832,7 +7832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E18236-E25D-41B3-8B1E-0194276152B3}">
   <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finish Pwm Improve, Make some modif on FMKCPU_ConfigSpecific FMKCPU_ConfigSpecific, frequerncy calculation algorithm [to be tested]
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_DrvStepper\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_PwmImprove\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08782A85-2B53-4E15-BD9B-94B0FB1FA8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E06BA4-BD33-4877-8791-6B70AEE08AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -6366,7 +6366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -8381,8 +8381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860CCB6B-9BC8-4B28-B4AE-B22F38F81573}">
   <dimension ref="B1:P254"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="96" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8415,10 +8415,10 @@
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L5">
-        <v>63500</v>
+        <v>21332.3</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
@@ -8440,21 +8440,21 @@
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D8">
-        <v>200</v>
+        <v>6000</v>
       </c>
       <c r="E8">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <f>E8*C3/((D8)*(F8+1))</f>
-        <v>800000</v>
+        <f>E8*C3/((D8)*(F8+1))-1</f>
+        <v>21332.333333333332</v>
       </c>
       <c r="J8">
-        <f>(E8*1000000)/((L5+1))</f>
-        <v>2519.6453599155921</v>
+        <f>(E8*1000000)/((L5))</f>
+        <v>6000.2906390778307</v>
       </c>
       <c r="M8" t="s">
         <v>332</v>
@@ -8463,7 +8463,7 @@
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M9">
         <f>J14-ROUND(J14,0)</f>
-        <v>-0.40177320042204023</v>
+        <v>4.8439846304981771E-5</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
@@ -8472,28 +8472,34 @@
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f>E8/(L13+1)*D8</f>
+        <v>35.998312579097856</v>
+      </c>
       <c r="J13" t="s">
         <v>327</v>
       </c>
       <c r="L13">
-        <v>63997</v>
+        <f>L5+(L5/J15)*M9</f>
+        <v>21333.333333333332</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J14">
-        <f>E8*C3/(D8*(L5+1))</f>
-        <v>12.59822679957796</v>
+        <f>E8*C3/(D8*(L5))</f>
+        <v>1.000048439846305</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J15">
-        <v>9</v>
+        <f>TRUNC(J14)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D16">
         <f>E8*C3/D8</f>
-        <v>800000</v>
+        <v>21333.333333333332</v>
       </c>
       <c r="J16" t="s">
         <v>112</v>
@@ -8510,15 +8516,15 @@
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D18">
         <f>E8*C3/D16</f>
-        <v>200</v>
+        <v>6000</v>
       </c>
       <c r="J18">
-        <f>(E8*C3)/((L5)*(INT(J14)))</f>
-        <v>209.9737532808399</v>
+        <f>(E8*C3)/((L5)*(INT(J14)+1))</f>
+        <v>3000.1453195389154</v>
       </c>
       <c r="L18">
         <f>(E8*C3)/((J15)*(L13))</f>
-        <v>277.79079922149128</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Major change in FMKCPU.c create FMKTIM to deal with timer/ adv timer etc
add FMKMAC (dma mngmt) in FMKCPU
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_PwmImprove\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_DiagDesign\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E06BA4-BD33-4877-8791-6B70AEE08AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D5BF9E-500B-40A8-A132-9CE93DF0F2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
     <sheet name="FMK_IO" sheetId="2" r:id="rId2"/>
-    <sheet name="FMK_CPU" sheetId="3" r:id="rId3"/>
+    <sheet name="FMK_TIM" sheetId="3" r:id="rId3"/>
     <sheet name="FMK_CDA" sheetId="4" r:id="rId4"/>
     <sheet name="FMKMAC" sheetId="6" r:id="rId5"/>
     <sheet name="FMKCAN" sheetId="7" r:id="rId6"/>
@@ -4006,7 +4006,7 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKTIM_EvntTimer" displayName="FMKTIM_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B097540B-A2DD-432F-8D25-C369E6A041DD}" name="Colonne1"/>
@@ -4017,7 +4017,7 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}" name="FMKCPU_IRQNHandler" displayName="FMKCPU_IRQNHandler" ref="F4:G17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}" name="FMKTIM_IRQNHandler" displayName="FMKTIM_IRQNHandler" ref="F4:G17" totalsRowShown="0">
   <autoFilter ref="F4:G17" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C0EA827E-D0A1-4F96-9D94-60107C8F02D0}" name="List IRQN_Handler"/>
@@ -4524,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="N15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD49" sqref="AD49"/>
+    <sheetView topLeftCell="I15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7449,8 +7449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E52BA6-3E0A-4F7C-9391-164B38476F25}">
   <dimension ref="B3:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8381,7 +8381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860CCB6B-9BC8-4B28-B4AE-B22F38F81573}">
   <dimension ref="B1:P254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="96" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="96" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enable to use PWM with pulse numbet
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_DiagDesign\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D5BF9E-500B-40A8-A132-9CE93DF0F2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E1536A-CE8A-4FCE-8FAB-7BB30FA8FE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="448">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1384,6 +1384,9 @@
   </si>
   <si>
     <t>TIM8_CH1</t>
+  </si>
+  <si>
+    <t>GPIO_AF2_TIM1</t>
   </si>
 </sst>
 </file>
@@ -6366,8 +6369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6654,19 +6657,19 @@
         <v>92</v>
       </c>
       <c r="P9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="Q9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R9" t="s">
-        <v>296</v>
+        <v>447</v>
       </c>
       <c r="S9" t="s">
-        <v>265</v>
+        <v>4</v>
       </c>
       <c r="T9" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="Z9" t="s">
         <v>12</v>
@@ -7449,7 +7452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E52BA6-3E0A-4F7C-9391-164B38476F25}">
   <dimension ref="B3:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
End Design Logic Implementation, Bug to correct before testing logic
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_DiagDesign\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_designLogc\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E1536A-CE8A-4FCE-8FAB-7BB30FA8FE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FEC151-B6AC-4EA1-A2FD-12F7BAF43378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="439">
   <si>
     <t>Colonne1</t>
   </si>
@@ -384,30 +384,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Others SPI configuration</t>
-  </si>
-  <si>
-    <t>Bsp_Pin_Name</t>
-  </si>
-  <si>
-    <t>Others I2C  configuration</t>
-  </si>
-  <si>
-    <t>PB6</t>
-  </si>
-  <si>
-    <t>PB7</t>
-  </si>
-  <si>
-    <t>PC10</t>
-  </si>
-  <si>
-    <t>PC11</t>
-  </si>
-  <si>
-    <t>PC12</t>
-  </si>
-  <si>
     <t>PC15, PC14, PF0, PF1  are forbidden</t>
   </si>
   <si>
@@ -867,15 +843,6 @@
     <t>ADC_5</t>
   </si>
   <si>
-    <t>GPIO_AF1_TIM16</t>
-  </si>
-  <si>
-    <t>GPIO_AF1_TIM17</t>
-  </si>
-  <si>
-    <t>GPIO_AF9_TIM15</t>
-  </si>
-  <si>
     <t>TS_CAL2</t>
   </si>
   <si>
@@ -933,15 +900,6 @@
     <t>GPIO_AF2_TIM3</t>
   </si>
   <si>
-    <t>GPIO_AF2_TIM20</t>
-  </si>
-  <si>
-    <t>GPIO_AF6_TIM5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others USART configuration </t>
-  </si>
-  <si>
     <t>GPIO_AF9_FDCAN1</t>
   </si>
   <si>
@@ -1146,9 +1104,6 @@
     <t>TIM1_TRG_COM_TIM17_IRQHandler</t>
   </si>
   <si>
-    <t>TIM1_CC_IRQHandler</t>
-  </si>
-  <si>
     <t>TIM2_IRQHandler</t>
   </si>
   <si>
@@ -1387,6 +1342,24 @@
   </si>
   <si>
     <t>GPIO_AF2_TIM1</t>
+  </si>
+  <si>
+    <t>GPIO_AF4_TIM8</t>
+  </si>
+  <si>
+    <t>GPIO_AF6_TIM20</t>
+  </si>
+  <si>
+    <t>GPIO_AF2_TIM4</t>
+  </si>
+  <si>
+    <t>TIM8_UP_IRQHandler</t>
+  </si>
+  <si>
+    <t>EXTI2_IRQN</t>
+  </si>
+  <si>
+    <t>EXTI9_5_IRQN</t>
   </si>
 </sst>
 </file>
@@ -3818,8 +3791,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:B15" totalsRowShown="0">
-  <autoFilter ref="A6:B15" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:B14" totalsRowShown="0">
+  <autoFilter ref="A6:B14" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6C4BEFED-5E85-401A-AA66-51A07D13FEBC}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{E08F986F-8D6D-4DEB-A18F-F4FB9A36C956}" name="Pin_name"/>
@@ -3829,8 +3802,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="Z7:AA16" totalsRowShown="0">
-  <autoFilter ref="Z7:AA16" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="Z7:AA18" totalsRowShown="0">
+  <autoFilter ref="Z7:AA18" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{395BD36A-0840-48CF-8D8D-56878E366FC5}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{34DF2CF3-8826-4F9E-A09D-280EE0FEFFBB}" name="Pin_name"/>
@@ -3840,8 +3813,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="J6:N9" totalsRowShown="0">
-  <autoFilter ref="J6:N9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="J6:N10" totalsRowShown="0">
+  <autoFilter ref="J6:N10" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F1DD33F7-0EF3-4BDF-839A-2E3FA15D0FD7}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{1EC5875F-046C-4961-B678-CB3386C5E012}" name="Pin_name"/>
@@ -3866,8 +3839,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="P6:T14" totalsRowShown="0">
-  <autoFilter ref="P6:T14" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="P6:T18" totalsRowShown="0">
+  <autoFilter ref="P6:T18" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F2B685DB-87AE-429A-9E70-076DA856F9A2}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{30126296-E33C-4D56-9110-2D49FE159CF1}" name="Pin_name"/>
@@ -3880,8 +3853,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:H16" totalsRowShown="0">
-  <autoFilter ref="E6:H16" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:H11" totalsRowShown="0">
+  <autoFilter ref="E6:H11" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EDBDBF14-1FA4-44B8-A62D-BAA9F312652A}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{75AD9B1E-8F88-4CD9-86AB-C0D6BFDB44CD}" name="Pin_name"/>
@@ -3934,41 +3907,6 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}" name="Tableau20" displayName="Tableau20" ref="K74:L77" totalsRowShown="0">
-  <autoFilter ref="K74:L77" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{35492CF7-2D64-4A31-B52A-8DC201862D23}" name="GPIO_name"/>
-    <tableColumn id="2" xr3:uid="{55201EA4-78EC-451A-894D-4121BE7C2D46}" name="Pin_name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}" name="Tableau2022" displayName="Tableau2022" ref="O78:Q80" totalsRowShown="0">
-  <autoFilter ref="O78:Q80" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{231389D4-B645-4CB2-A30E-5CBE9EE6FEFC}" name="GPIO_name"/>
-    <tableColumn id="2" xr3:uid="{56336DBF-18EC-4309-B422-97BDC37985D4}" name="Pin_name"/>
-    <tableColumn id="3" xr3:uid="{1167559C-5083-4ABC-8F8C-8F11E7C7FAA7}" name="Bsp_Pin_Name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}" name="Tableau202223" displayName="Tableau202223" ref="S78:U81" totalsRowShown="0">
-  <autoFilter ref="S78:U81" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{30F87F4B-0EBB-4470-919C-8CEF7288D9C8}" name="GPIO_name"/>
-    <tableColumn id="2" xr3:uid="{DAB30C64-2E65-452D-A80D-3D932E8F35B6}" name="Pin_name"/>
-    <tableColumn id="3" xr3:uid="{5633DAA7-5910-4D39-A1CD-689650D5DAF3}" name="Bsp_Pin_Name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="FMKIO_CanCfg" displayName="FMKIO_CanCfg" ref="A25:F28" totalsRowShown="0">
   <autoFilter ref="A25:F28" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
   <tableColumns count="6">
@@ -3983,7 +3921,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}" name="FMKIO_SerialCfg" displayName="FMKIO_SerialCfg" ref="A34:F36" totalsRowShown="0">
   <autoFilter ref="A34:F36" xr:uid="{978057A4-13F6-44F3-B65B-2C409866E1DE}"/>
   <tableColumns count="6">
@@ -3998,9 +3936,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}" name="FMKIO_IRQNHandler" displayName="FMKIO_IRQNHandler" ref="L21:L28" totalsRowShown="0">
-  <autoFilter ref="L21:L28" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}"/>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}" name="FMKIO_IRQNHandler" displayName="FMKIO_IRQNHandler" ref="W29:W36" totalsRowShown="0">
+  <autoFilter ref="W29:W36" xr:uid="{DA1831B2-BC94-42A9-B299-31A3CE618396}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{435A2CB3-E527-4D4E-9A3C-7D2BA856E09C}" name="List IRQN_Handler"/>
   </tableColumns>
@@ -4008,7 +3946,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKTIM_EvntTimer" displayName="FMKTIM_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -4019,12 +3957,49 @@
 </table>
 </file>
 
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}" name="FMKTIM_IRQNHandler" displayName="FMKTIM_IRQNHandler" ref="F4:G17" totalsRowShown="0">
   <autoFilter ref="F4:G17" xr:uid="{CCB68487-82CB-434C-A0E4-701B1FDDACF5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C0EA827E-D0A1-4F96-9D94-60107C8F02D0}" name="List IRQN_Handler"/>
     <tableColumn id="2" xr3:uid="{B344E14A-A089-45F4-9C1B-D978E362DC5A}" name="Timer Associated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
+  <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{74AD6856-B046-40F9-89E8-C5AC0EB4C661}" name="calibration temperature "/>
+    <tableColumn id="2" xr3:uid="{D58B2B24-74EC-4445-9DDA-83A119877B67}" name="address in hexacecimal"/>
+    <tableColumn id="3" xr3:uid="{0793AAF2-321B-4695-AEBB-122FAB9D49F7}" name="Adc Vref"/>
+    <tableColumn id="4" xr3:uid="{F1198D75-5BAD-4CA5-814F-DDA2BB66E5F2}" name="Channel Vref"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V8" totalsRowShown="0">
+  <autoFilter ref="S3:V8" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0BCC2BC4-7FF0-4C14-809D-9D95A3225151}" name="Vref Calib"/>
+    <tableColumn id="2" xr3:uid="{0E78A6D4-DF9E-4966-A80E-64FE5BD9F1E2}" name="address  hexacecimal"/>
+    <tableColumn id="4" xr3:uid="{4C711A0D-EAF5-4229-B4D2-99254AE9F9BA}" name="Adc Vref"/>
+    <tableColumn id="5" xr3:uid="{0B4759AE-B188-4822-92BB-EEEB3203C895}" name="Channel Vref"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}" name="FMKCDA_IRQNHandler" displayName="FMKCDA_IRQNHandler" ref="E8:F12" totalsRowShown="0">
+  <autoFilter ref="E8:F12" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CD80BAAD-36DA-496C-9F7C-D80D4296914C}" name="List IRQN_Handler"/>
+    <tableColumn id="2" xr3:uid="{9F8B466B-BFC7-4900-8330-976222B1008D}" name="Adc, Dac associated"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4044,43 +4019,6 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L5" totalsRowShown="0">
-  <autoFilter ref="I3:L5" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{74AD6856-B046-40F9-89E8-C5AC0EB4C661}" name="calibration temperature "/>
-    <tableColumn id="2" xr3:uid="{D58B2B24-74EC-4445-9DDA-83A119877B67}" name="address in hexacecimal"/>
-    <tableColumn id="3" xr3:uid="{0793AAF2-321B-4695-AEBB-122FAB9D49F7}" name="Adc Vref"/>
-    <tableColumn id="4" xr3:uid="{F1198D75-5BAD-4CA5-814F-DDA2BB66E5F2}" name="Channel Vref"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V8" totalsRowShown="0">
-  <autoFilter ref="S3:V8" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0BCC2BC4-7FF0-4C14-809D-9D95A3225151}" name="Vref Calib"/>
-    <tableColumn id="2" xr3:uid="{0E78A6D4-DF9E-4966-A80E-64FE5BD9F1E2}" name="address  hexacecimal"/>
-    <tableColumn id="4" xr3:uid="{4C711A0D-EAF5-4229-B4D2-99254AE9F9BA}" name="Adc Vref"/>
-    <tableColumn id="5" xr3:uid="{0B4759AE-B188-4822-92BB-EEEB3203C895}" name="Channel Vref"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}" name="FMKCDA_IRQNHandler" displayName="FMKCDA_IRQNHandler" ref="E8:F12" totalsRowShown="0">
-  <autoFilter ref="E8:F12" xr:uid="{FAF38277-E25D-413A-A145-AFBC74566FF1}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CD80BAAD-36DA-496C-9F7C-D80D4296914C}" name="List IRQN_Handler"/>
-    <tableColumn id="2" xr3:uid="{9F8B466B-BFC7-4900-8330-976222B1008D}" name="Adc, Dac associated"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}" name="FMKMAC_Cfg" displayName="FMKMAC_Cfg" ref="B2:E12" totalsRowShown="0">
   <autoFilter ref="B2:E12" xr:uid="{333A4E38-7E7A-4098-B282-4F58DD308AC2}"/>
   <tableColumns count="4">
@@ -4093,7 +4031,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}" name="FMKMAC_IRQN" displayName="FMKMAC_IRQN" ref="J3:K18" totalsRowShown="0">
   <autoFilter ref="J3:K18" xr:uid="{8B613F4D-88F2-4091-AA3A-5550AB627653}"/>
   <tableColumns count="2">
@@ -4104,7 +4042,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{9E75F4B3-8C66-44CB-A927-82E8A09563A2}" name="FMKMAC_DMAMUX" displayName="FMKMAC_DMAMUX" ref="P3:P4" totalsRowShown="0">
   <autoFilter ref="P3:P4" xr:uid="{9E75F4B3-8C66-44CB-A927-82E8A09563A2}"/>
   <tableColumns count="1">
@@ -4114,7 +4052,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}" name="Tableau35" displayName="Tableau35" ref="B5:B11" totalsRowShown="0">
   <autoFilter ref="B5:B11" xr:uid="{3568793B-2270-4B9A-A9E5-55F929444AFF}"/>
   <tableColumns count="1">
@@ -4124,7 +4062,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}" name="FMKSRL_INFO" displayName="FMKSRL_INFO" ref="E2:M7" totalsRowShown="0">
   <autoFilter ref="E2:M7" xr:uid="{CF6032E9-4D15-4575-AD94-133BB9C2FD31}"/>
   <tableColumns count="9">
@@ -4527,8 +4465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView topLeftCell="I15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="H15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4559,16 +4497,16 @@
   <sheetData>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="F18" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -4583,27 +4521,27 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="N18" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="O18" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F19" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -4618,45 +4556,45 @@
         <v>4</v>
       </c>
       <c r="M19" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N19" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O19" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E20" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F20" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I20" t="s">
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="L20">
         <v>4</v>
       </c>
       <c r="M20" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N20" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O20" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="T20" t="s">
         <v>17</v>
@@ -4665,10 +4603,10 @@
         <v>18</v>
       </c>
       <c r="V20" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="W20" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="AB20" t="s">
         <v>22</v>
@@ -4677,21 +4615,21 @@
         <v>18</v>
       </c>
       <c r="AD20" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E21" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F21" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H21" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I21" t="s">
         <v>69</v>
@@ -4706,10 +4644,10 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O21" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="T21" t="s">
         <v>16</v>
@@ -4718,13 +4656,13 @@
         <v>18</v>
       </c>
       <c r="V21" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="W21" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="AB21" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="AC21">
         <v>8</v>
@@ -4735,66 +4673,66 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E22" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F22" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H22" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I22" t="s">
         <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="L22">
         <v>4</v>
       </c>
       <c r="M22" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="N22" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O22" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="T22" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="U22">
         <v>18</v>
       </c>
       <c r="V22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="W22" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="AB22" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="AC22">
         <v>8</v>
       </c>
       <c r="AD22" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E23" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F23" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
@@ -4803,42 +4741,42 @@
         <v>69</v>
       </c>
       <c r="K23" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="L23">
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="N23" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O23" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="T23" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="U23">
         <v>18</v>
       </c>
       <c r="V23" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="W23" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E24" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F24" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H24" t="s">
         <v>61</v>
@@ -4847,31 +4785,31 @@
         <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="N24" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="O24" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="T24" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="U24">
         <v>18</v>
       </c>
       <c r="V24" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="W24" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
@@ -4879,95 +4817,95 @@
         <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="F25" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H25" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I25" t="s">
         <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="N25" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="O25" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="T25" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="U25">
         <v>18</v>
       </c>
       <c r="V25" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="W25" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F26" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I26" t="s">
         <v>69</v>
       </c>
       <c r="K26" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="L26">
         <v>6</v>
       </c>
       <c r="M26" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="N26" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O26" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F27" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H27" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I27" t="s">
         <v>69</v>
@@ -4979,33 +4917,33 @@
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="N27" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="O27" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B28">
         <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E28" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F28" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H28" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="I28" t="s">
         <v>69</v>
@@ -5017,33 +4955,33 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="N28" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="O28" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B29">
         <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E29" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F29" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H29" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I29" t="s">
         <v>69</v>
@@ -5055,13 +4993,13 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="N29" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="O29" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -5069,10 +5007,10 @@
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F30" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -5081,19 +5019,19 @@
         <v>69</v>
       </c>
       <c r="K30" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="L30">
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N30" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="O30" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -5101,13 +5039,13 @@
         <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F31" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H31" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I31" t="s">
         <v>69</v>
@@ -5118,13 +5056,13 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F32" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H32" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I32" t="s">
         <v>69</v>
@@ -5132,16 +5070,16 @@
     </row>
     <row r="33" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E33" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="F33" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H33" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I33" t="s">
         <v>69</v>
@@ -5155,16 +5093,16 @@
     </row>
     <row r="34" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E34" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="F34" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H34" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I34" t="s">
         <v>69</v>
@@ -5178,16 +5116,16 @@
     </row>
     <row r="35" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E35" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F35" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H35" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I35" t="s">
         <v>69</v>
@@ -5201,16 +5139,16 @@
     </row>
     <row r="36" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E36" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F36" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H36" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I36" t="s">
         <v>69</v>
@@ -5230,16 +5168,16 @@
     </row>
     <row r="37" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E37" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F37" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H37" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I37" t="s">
         <v>69</v>
@@ -5259,22 +5197,22 @@
     </row>
     <row r="38" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E38" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F38" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H38" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I38" t="s">
         <v>69</v>
       </c>
       <c r="P38" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q38">
         <v>16</v>
@@ -5282,16 +5220,16 @@
     </row>
     <row r="39" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E39" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F39" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H39" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I39" t="s">
         <v>69</v>
@@ -5305,22 +5243,22 @@
     </row>
     <row r="40" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E40" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F40" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H40" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I40" t="s">
         <v>90</v>
       </c>
       <c r="P40" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="Q40">
         <v>11</v>
@@ -5331,16 +5269,16 @@
     </row>
     <row r="41" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E41" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="F41" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H41" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I41" t="s">
         <v>90</v>
@@ -5351,16 +5289,16 @@
     </row>
     <row r="42" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F42" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H42" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I42" t="s">
         <v>69</v>
@@ -5374,13 +5312,13 @@
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F43" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H43" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I43" t="s">
         <v>69</v>
@@ -5391,16 +5329,16 @@
     </row>
     <row r="44" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E44" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F44" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H44" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I44" t="s">
         <v>69</v>
@@ -5408,16 +5346,16 @@
     </row>
     <row r="45" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E45" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F45" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H45" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I45" t="s">
         <v>69</v>
@@ -5425,13 +5363,13 @@
     </row>
     <row r="46" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E46" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F46" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -5440,38 +5378,38 @@
         <v>69</v>
       </c>
       <c r="AF46" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E47" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F47" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H47" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I47" t="s">
         <v>69</v>
       </c>
       <c r="AF47" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E48" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F48" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H48" t="s">
         <v>64</v>
@@ -5480,27 +5418,27 @@
         <v>69</v>
       </c>
       <c r="AF48" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E49" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F49" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H49" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="I49" t="s">
         <v>69</v>
       </c>
       <c r="AF49" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="4:32" x14ac:dyDescent="0.3">
@@ -5508,13 +5446,13 @@
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F50" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H50" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I50" t="s">
         <v>69</v>
@@ -5525,13 +5463,13 @@
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F51" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H51" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I51" t="s">
         <v>69</v>
@@ -5539,22 +5477,22 @@
     </row>
     <row r="52" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E52" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F52" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H52" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I52" t="s">
         <v>69</v>
       </c>
       <c r="AF52" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="4:32" x14ac:dyDescent="0.3">
@@ -5562,30 +5500,30 @@
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F53" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H53" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="I53" t="s">
         <v>69</v>
       </c>
       <c r="AF53" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E54" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F54" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H54" t="s">
         <v>65</v>
@@ -5594,18 +5532,18 @@
         <v>69</v>
       </c>
       <c r="AF54" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E55" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F55" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H55" t="s">
         <v>66</v>
@@ -5614,18 +5552,18 @@
         <v>69</v>
       </c>
       <c r="AF55" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E56" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F56" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H56" t="s">
         <v>67</v>
@@ -5634,18 +5572,18 @@
         <v>69</v>
       </c>
       <c r="AF56" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E57" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F57" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H57" t="s">
         <v>68</v>
@@ -5654,47 +5592,47 @@
         <v>69</v>
       </c>
       <c r="AF57" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F58" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H58" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I58" t="s">
         <v>69</v>
       </c>
       <c r="AF58" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E59" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="F59" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H59" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I59" t="s">
         <v>69</v>
       </c>
       <c r="AF59" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="4:32" x14ac:dyDescent="0.3">
@@ -5702,73 +5640,73 @@
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F60" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H60" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I60" t="s">
         <v>69</v>
       </c>
       <c r="AF60" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="61" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E61" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F61" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H61" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I61" t="s">
         <v>69</v>
       </c>
       <c r="AF61" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E62" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F62" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H62" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="I62" t="s">
         <v>69</v>
       </c>
       <c r="AF62" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E63" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F63" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H63" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="I63" t="s">
         <v>69</v>
@@ -5779,13 +5717,13 @@
         <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F64" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H64" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I64" t="s">
         <v>69</v>
@@ -5796,13 +5734,13 @@
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F65" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H65" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I65" t="s">
         <v>69</v>
@@ -5813,13 +5751,13 @@
         <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F66" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H66" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I66" t="s">
         <v>69</v>
@@ -5827,16 +5765,16 @@
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E67" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F67" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H67" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I67" t="s">
         <v>69</v>
@@ -5847,13 +5785,13 @@
         <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F68" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H68" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I68" t="s">
         <v>69</v>
@@ -5861,16 +5799,16 @@
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E69" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F69" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H69" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I69" t="s">
         <v>69</v>
@@ -5881,13 +5819,13 @@
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F70" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H70" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I70" t="s">
         <v>69</v>
@@ -5898,13 +5836,13 @@
         <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F71" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H71" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I71" t="s">
         <v>69</v>
@@ -5915,13 +5853,13 @@
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F72" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H72" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="I72" t="s">
         <v>69</v>
@@ -5929,16 +5867,16 @@
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E73" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F73" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H73" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I73" t="s">
         <v>69</v>
@@ -5946,16 +5884,16 @@
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E74" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F74" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H74" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I74" t="s">
         <v>69</v>
@@ -5963,16 +5901,16 @@
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E75" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F75" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="H75" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I75" t="s">
         <v>69</v>
@@ -5980,7 +5918,7 @@
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H76" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I76" t="s">
         <v>69</v>
@@ -5988,7 +5926,7 @@
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H77" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I77" t="s">
         <v>69</v>
@@ -5996,7 +5934,7 @@
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H78" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I78" t="s">
         <v>69</v>
@@ -6004,7 +5942,7 @@
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H79" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I79" t="s">
         <v>69</v>
@@ -6012,7 +5950,7 @@
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H80" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I80" t="s">
         <v>69</v>
@@ -6020,7 +5958,7 @@
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I81" t="s">
         <v>69</v>
@@ -6028,7 +5966,7 @@
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I82" t="s">
         <v>69</v>
@@ -6036,7 +5974,7 @@
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I83" t="s">
         <v>69</v>
@@ -6044,7 +5982,7 @@
     </row>
     <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I84" t="s">
         <v>69</v>
@@ -6052,7 +5990,7 @@
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I85" t="s">
         <v>69</v>
@@ -6060,7 +5998,7 @@
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I86" t="s">
         <v>69</v>
@@ -6068,7 +6006,7 @@
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I87" t="s">
         <v>69</v>
@@ -6076,7 +6014,7 @@
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="I88" t="s">
         <v>69</v>
@@ -6084,7 +6022,7 @@
     </row>
     <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I89" t="s">
         <v>69</v>
@@ -6092,7 +6030,7 @@
     </row>
     <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I90" t="s">
         <v>69</v>
@@ -6100,7 +6038,7 @@
     </row>
     <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="I91" t="s">
         <v>69</v>
@@ -6108,7 +6046,7 @@
     </row>
     <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H92" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I92" t="s">
         <v>69</v>
@@ -6116,7 +6054,7 @@
     </row>
     <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H93" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I93" t="s">
         <v>69</v>
@@ -6124,7 +6062,7 @@
     </row>
     <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H94" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I94" t="s">
         <v>69</v>
@@ -6132,7 +6070,7 @@
     </row>
     <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H95" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I95" t="s">
         <v>69</v>
@@ -6140,7 +6078,7 @@
     </row>
     <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H96" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I96" t="s">
         <v>69</v>
@@ -6148,7 +6086,7 @@
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H97" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I97" t="s">
         <v>69</v>
@@ -6156,7 +6094,7 @@
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H98" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I98" t="s">
         <v>69</v>
@@ -6164,7 +6102,7 @@
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H99" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I99" t="s">
         <v>69</v>
@@ -6172,7 +6110,7 @@
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H100" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I100" t="s">
         <v>69</v>
@@ -6180,7 +6118,7 @@
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H101" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I101" t="s">
         <v>69</v>
@@ -6188,7 +6126,7 @@
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H102" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="I102" t="s">
         <v>69</v>
@@ -6196,7 +6134,7 @@
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H103" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I103" t="s">
         <v>69</v>
@@ -6204,7 +6142,7 @@
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H104" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="I104" t="s">
         <v>90</v>
@@ -6212,7 +6150,7 @@
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H105" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I105" t="s">
         <v>90</v>
@@ -6220,7 +6158,7 @@
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H106" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="I106" t="s">
         <v>90</v>
@@ -6228,7 +6166,7 @@
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H107" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="I107" t="s">
         <v>90</v>
@@ -6236,7 +6174,7 @@
     </row>
     <row r="108" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H108" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I108" t="s">
         <v>69</v>
@@ -6244,7 +6182,7 @@
     </row>
     <row r="109" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H109" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I109" t="s">
         <v>69</v>
@@ -6252,7 +6190,7 @@
     </row>
     <row r="110" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H110" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I110" t="s">
         <v>69</v>
@@ -6260,7 +6198,7 @@
     </row>
     <row r="111" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H111" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="I111" t="s">
         <v>69</v>
@@ -6268,7 +6206,7 @@
     </row>
     <row r="112" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H112" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I112" t="s">
         <v>69</v>
@@ -6276,7 +6214,7 @@
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H113" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I113" t="s">
         <v>69</v>
@@ -6284,7 +6222,7 @@
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H114" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I114" t="s">
         <v>69</v>
@@ -6292,7 +6230,7 @@
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H115" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I115" t="s">
         <v>69</v>
@@ -6300,7 +6238,7 @@
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H116" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="I116" t="s">
         <v>69</v>
@@ -6308,7 +6246,7 @@
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H117" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I117" t="s">
         <v>69</v>
@@ -6316,7 +6254,7 @@
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H118" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="I118" t="s">
         <v>69</v>
@@ -6324,7 +6262,7 @@
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H119" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="I119" t="s">
         <v>69</v>
@@ -6367,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
-  <dimension ref="A2:BA81"/>
+  <dimension ref="A2:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="Q3" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6392,7 +6330,8 @@
     <col min="19" max="19" width="23.33203125" customWidth="1"/>
     <col min="20" max="20" width="18.44140625" customWidth="1"/>
     <col min="21" max="21" width="23.109375" customWidth="1"/>
-    <col min="24" max="24" width="20" customWidth="1"/>
+    <col min="23" max="23" width="25.109375" customWidth="1"/>
+    <col min="24" max="24" width="34" customWidth="1"/>
     <col min="25" max="25" width="16.77734375" customWidth="1"/>
     <col min="26" max="26" width="20.77734375" customWidth="1"/>
     <col min="27" max="27" width="16.77734375" customWidth="1"/>
@@ -6404,7 +6343,7 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -6418,13 +6357,13 @@
         <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="P5" t="s">
         <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="V5" t="s">
         <v>55</v>
@@ -6494,61 +6433,61 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
       <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" t="s">
-        <v>267</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
       <c r="L7" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="M7" t="s">
-        <v>264</v>
+        <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
       </c>
       <c r="Q7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="R7" t="s">
-        <v>295</v>
+        <v>432</v>
       </c>
       <c r="S7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V7" t="s">
         <v>12</v>
       </c>
       <c r="W7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="X7" t="s">
-        <v>163</v>
+        <v>437</v>
       </c>
       <c r="Z7" t="s">
         <v>23</v>
@@ -6559,31 +6498,31 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
       <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>262</v>
+      </c>
+      <c r="H8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" t="s">
-        <v>267</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
       <c r="L8" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
@@ -6595,464 +6534,457 @@
         <v>13</v>
       </c>
       <c r="Q8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R8" t="s">
-        <v>295</v>
+        <v>432</v>
       </c>
       <c r="S8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="V8" t="s">
         <v>11</v>
       </c>
       <c r="W8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="X8" t="s">
-        <v>140</v>
+        <v>438</v>
       </c>
       <c r="Z8" t="s">
         <v>12</v>
       </c>
       <c r="AA8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>262</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9" t="s">
-        <v>267</v>
-      </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="P9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Q9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="R9" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="S9" t="s">
-        <v>4</v>
+        <v>257</v>
       </c>
       <c r="T9" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="Z9" t="s">
         <v>12</v>
       </c>
       <c r="AA9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" t="s">
+        <v>284</v>
+      </c>
+      <c r="M10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
+      <c r="Q10" t="s">
         <v>28</v>
       </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>103</v>
-      </c>
-      <c r="P10" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>39</v>
-      </c>
       <c r="R10" t="s">
-        <v>296</v>
+        <v>432</v>
       </c>
       <c r="S10" t="s">
-        <v>265</v>
+        <v>4</v>
       </c>
       <c r="T10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Z10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>262</v>
+      </c>
+      <c r="H11" t="s">
+        <v>109</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" t="s">
         <v>31</v>
       </c>
-      <c r="G11" t="s">
-        <v>270</v>
-      </c>
-      <c r="H11" t="s">
-        <v>97</v>
-      </c>
-      <c r="P11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>40</v>
-      </c>
       <c r="R11" t="s">
-        <v>296</v>
+        <v>433</v>
       </c>
       <c r="S11" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="T11" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="Z11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" t="s">
+        <v>433</v>
+      </c>
+      <c r="S12" t="s">
+        <v>256</v>
+      </c>
+      <c r="T12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>270</v>
-      </c>
-      <c r="H12" t="s">
-        <v>98</v>
-      </c>
-      <c r="P12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" t="s">
-        <v>296</v>
-      </c>
-      <c r="S12" t="s">
-        <v>265</v>
-      </c>
-      <c r="T12" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>13</v>
-      </c>
       <c r="AA12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>109</v>
-      </c>
       <c r="P13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R13" t="s">
-        <v>297</v>
+        <v>434</v>
       </c>
       <c r="S13" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="T13" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="Z13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AA13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" t="s">
+        <v>433</v>
+      </c>
+      <c r="S14" t="s">
+        <v>256</v>
+      </c>
+      <c r="T14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="Q15" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" t="s">
+        <v>435</v>
+      </c>
+      <c r="S15" t="s">
+        <v>253</v>
+      </c>
+      <c r="T15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" t="s">
-        <v>106</v>
-      </c>
-      <c r="P14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="Q16" t="s">
         <v>32</v>
       </c>
-      <c r="R14" t="s">
-        <v>297</v>
-      </c>
-      <c r="S14" t="s">
-        <v>266</v>
-      </c>
-      <c r="T14" t="s">
+      <c r="R16" t="s">
+        <v>435</v>
+      </c>
+      <c r="S16" t="s">
+        <v>253</v>
+      </c>
+      <c r="T16" t="s">
         <v>46</v>
       </c>
-      <c r="Z14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA14" t="s">
+      <c r="Z16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA15" t="s">
+      <c r="Q17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R17" t="s">
+        <v>435</v>
+      </c>
+      <c r="S17" t="s">
+        <v>253</v>
+      </c>
+      <c r="T17" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="L20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="L21" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="L22" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="L23" t="s">
-        <v>380</v>
+      <c r="R18" t="s">
+        <v>435</v>
+      </c>
+      <c r="S18" t="s">
+        <v>253</v>
+      </c>
+      <c r="T18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>427</v>
-      </c>
-      <c r="L24" t="s">
-        <v>381</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B25" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C25" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D25" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>307</v>
-      </c>
-      <c r="L25" t="s">
-        <v>382</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
         <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="F26" t="s">
-        <v>304</v>
-      </c>
-      <c r="L26" t="s">
-        <v>383</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="F27" t="s">
-        <v>306</v>
-      </c>
-      <c r="L27" t="s">
-        <v>384</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="F28" t="s">
-        <v>305</v>
-      </c>
-      <c r="L28" t="s">
-        <v>385</v>
+        <v>291</v>
+      </c>
+      <c r="W28" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="W29" t="s">
+        <v>356</v>
+      </c>
       <c r="AW29" t="s">
         <v>91</v>
       </c>
@@ -7061,6 +6993,9 @@
       </c>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="W30" t="s">
+        <v>364</v>
+      </c>
       <c r="AW30" t="s">
         <v>25</v>
       </c>
@@ -7072,6 +7007,9 @@
       </c>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="W31" t="s">
+        <v>365</v>
+      </c>
       <c r="AW31" t="s">
         <v>26</v>
       </c>
@@ -7083,6 +7021,9 @@
       </c>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="W32" t="s">
+        <v>366</v>
+      </c>
       <c r="AW32" t="s">
         <v>27</v>
       </c>
@@ -7095,7 +7036,10 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>360</v>
+        <v>346</v>
+      </c>
+      <c r="W33" t="s">
+        <v>367</v>
       </c>
       <c r="AW33" t="s">
         <v>28</v>
@@ -7109,22 +7053,25 @@
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B34" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C34" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D34" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>363</v>
+        <v>349</v>
+      </c>
+      <c r="W34" t="s">
+        <v>368</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -7150,10 +7097,13 @@
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
+      </c>
+      <c r="W35" t="s">
+        <v>369</v>
       </c>
       <c r="AW35" t="s">
         <v>30</v>
@@ -7176,10 +7126,13 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="F36" t="s">
-        <v>289</v>
+        <v>278</v>
+      </c>
+      <c r="W36" t="s">
+        <v>370</v>
       </c>
       <c r="AW36" t="s">
         <v>31</v>
@@ -7275,136 +7228,22 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="K73" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="K74" t="s">
-        <v>23</v>
-      </c>
-      <c r="L74" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="75" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="K75" t="s">
-        <v>11</v>
-      </c>
-      <c r="L75" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="K76" t="s">
-        <v>11</v>
-      </c>
-      <c r="L76" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="K77" t="s">
-        <v>11</v>
-      </c>
-      <c r="L77" t="s">
-        <v>32</v>
-      </c>
-      <c r="N77" t="s">
-        <v>115</v>
-      </c>
-      <c r="R77" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="78" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="O78" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>114</v>
-      </c>
-      <c r="S78" t="s">
-        <v>23</v>
-      </c>
-      <c r="T78" t="s">
-        <v>24</v>
-      </c>
-      <c r="U78" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="79" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="O79" t="s">
-        <v>12</v>
-      </c>
-      <c r="P79" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>116</v>
-      </c>
-      <c r="S79" t="s">
-        <v>13</v>
-      </c>
-      <c r="T79" t="s">
-        <v>35</v>
-      </c>
-      <c r="U79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="11:21" x14ac:dyDescent="0.3">
-      <c r="O80" t="s">
-        <v>12</v>
-      </c>
-      <c r="P80" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>117</v>
-      </c>
-      <c r="S80" t="s">
-        <v>13</v>
-      </c>
-      <c r="T80" t="s">
-        <v>36</v>
-      </c>
-      <c r="U80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="19:21" x14ac:dyDescent="0.3">
-      <c r="S81" t="s">
-        <v>13</v>
-      </c>
-      <c r="T81" t="s">
-        <v>38</v>
-      </c>
-      <c r="U81" t="s">
-        <v>120</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 B7:B15 F7:F16 AA8:AA16 Q7:Q14 W7:W8 K7:K9" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 K7:K10 Q7:Q14 F7:F11 B7:B14 W7:W8 AA8:AA18" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
       <formula1>$AW$30:$AW$45</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:T14 N7:N9" xr:uid="{727A5344-B28A-4866-9EC1-7C96029AF8B6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:T14 N7:N10" xr:uid="{727A5344-B28A-4866-9EC1-7C96029AF8B6}">
       <formula1>$AY$31:$AY$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H16" xr:uid="{FFFA1AF2-B35F-4BAA-AEF6-4A6121806F8D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11" xr:uid="{FFFA1AF2-B35F-4BAA-AEF6-4A6121806F8D}">
       <formula1>$BA$30:$BA$47</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="15">
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -7417,30 +7256,27 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
-    <tablePart r:id="rId14"/>
-    <tablePart r:id="rId15"/>
-    <tablePart r:id="rId16"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA00DA78-9682-47F8-B701-D35809CE3FB0}">
+          <x14:formula1>
+            <xm:f>General_Info!$P$34:$P$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>P7:P14 J7:J10 E7:E11 A7:A14 V7:V8 Z8:Z18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
+          <x14:formula1>
+            <xm:f>General_Info!$T$21:$T$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>G6:G11</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C3D18C3-7241-4088-8034-07AAE0EB53A9}">
           <x14:formula1>
             <xm:f>General_Info!$K$19:$K$30</xm:f>
           </x14:formula1>
           <xm:sqref>S7:S14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA00DA78-9682-47F8-B701-D35809CE3FB0}">
-          <x14:formula1>
-            <xm:f>General_Info!$P$34:$P$39</xm:f>
-          </x14:formula1>
-          <xm:sqref>J7:J9 A7:A15 E7:E16 Z8:Z16 P7:P14 V7:V8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
-          <x14:formula1>
-            <xm:f>General_Info!$T$21:$T$25</xm:f>
-          </x14:formula1>
-          <xm:sqref>G6:G16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7453,11 +7289,13 @@
   <dimension ref="B3:G17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
@@ -7467,7 +7305,7 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -7478,10 +7316,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="G4" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -7492,7 +7330,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -7506,7 +7344,7 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -7514,7 +7352,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -7522,7 +7360,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -7530,15 +7368,15 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="G9" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -7546,58 +7384,58 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="G11" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="G12" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="G13" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>374</v>
+        <v>436</v>
       </c>
       <c r="G14" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="G15" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="G16" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="G17" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -7635,44 +7473,44 @@
   <sheetData>
     <row r="2" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="K3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="S3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="T3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="U3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="V3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J4" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -7681,10 +7519,10 @@
         <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="T4" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
@@ -7695,22 +7533,22 @@
     </row>
     <row r="5" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="K5" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="L5" t="s">
         <v>98</v>
       </c>
       <c r="S5" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="T5" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="U5" t="s">
         <v>16</v>
@@ -7721,13 +7559,13 @@
     </row>
     <row r="6" spans="5:22" x14ac:dyDescent="0.3">
       <c r="S6" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="T6" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="U6" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="V6" t="s">
         <v>111</v>
@@ -7735,16 +7573,16 @@
     </row>
     <row r="7" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="S7" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="T7" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="U7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="V7" t="s">
         <v>111</v>
@@ -7752,19 +7590,19 @@
     </row>
     <row r="8" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="F8" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="S8" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="T8" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="U8" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="V8" t="s">
         <v>111</v>
@@ -7772,34 +7610,34 @@
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="F9" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="F10" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="F11" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="F12" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -7851,50 +7689,50 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="D2" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="E2" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="J2" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D3" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="K3" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="P3" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="C4" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -7903,24 +7741,24 @@
         <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="K4" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="L4" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="P4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="C5" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D5" t="s">
         <v>92</v>
@@ -7929,18 +7767,18 @@
         <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="K5" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C6" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7949,18 +7787,18 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="K6" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7969,58 +7807,58 @@
         <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="K7" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="C8" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D8" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="K8" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="C9" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D9" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="K9" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="C10" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -8029,18 +7867,18 @@
         <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="K10" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="C11" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -8049,18 +7887,18 @@
         <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="K11" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="C12" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="D12" t="s">
         <v>92</v>
@@ -8069,43 +7907,43 @@
         <v>69</v>
       </c>
       <c r="J12" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="K12" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="K13" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -8130,47 +7968,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -8205,28 +8043,28 @@
   <sheetData>
     <row r="2" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="F2" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="G2" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="H2" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="I2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="J2" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="K2" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="L2" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
@@ -8237,7 +8075,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -8246,19 +8084,19 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J3" t="s">
         <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="5:13" x14ac:dyDescent="0.3">
@@ -8266,7 +8104,7 @@
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="G4">
         <v>256</v>
@@ -8287,38 +8125,38 @@
         <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F5" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="I5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F6" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="G6">
         <v>256</v>
@@ -8327,27 +8165,27 @@
         <v>256</v>
       </c>
       <c r="I6" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J6" t="s">
         <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F7" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -8356,19 +8194,19 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L7" t="s">
         <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -8400,7 +8238,7 @@
   <sheetData>
     <row r="1" spans="3:14" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D1" s="6" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
@@ -8410,10 +8248,10 @@
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="N4" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -8426,19 +8264,19 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="E7" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="F7" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G7" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="J7" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -8460,7 +8298,7 @@
         <v>6000.2906390778307</v>
       </c>
       <c r="M8" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -8471,7 +8309,7 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -8480,7 +8318,7 @@
         <v>35.998312579097856</v>
       </c>
       <c r="J13" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="L13">
         <f>L5+(L5/J15)*M9</f>
@@ -8510,10 +8348,10 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="L17" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -8548,15 +8386,15 @@
     </row>
     <row r="27" spans="2:16" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D27" s="6" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="K28" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -8568,39 +8406,39 @@
         <v>0.5</v>
       </c>
       <c r="M29" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E30" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="F30" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G30" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="I30" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="J30" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="K30" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="L30" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="M30" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="O30" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="P30" t="e">
         <f>2^#REF!</f>

</xml_diff>

<commit_message>
End Logic, Logic has to be debug but APPSNS/ APPACT Configuration Working + Message Send OK
Warning in Serial Monitor, set Hex representation and not Text
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_designLogc\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FEC151-B6AC-4EA1-A2FD-12F7BAF43378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC6EC67-F4CB-4C2C-A8A8-7473ECD5F0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="440">
   <si>
     <t>Colonne1</t>
   </si>
@@ -1360,6 +1360,9 @@
   </si>
   <si>
     <t>EXTI9_5_IRQN</t>
+  </si>
+  <si>
+    <t>JTAG User -&gt; PA14/PA13</t>
   </si>
 </sst>
 </file>
@@ -6307,15 +6310,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q3" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" topLeftCell="S2" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="22.109375" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
@@ -6345,6 +6348,9 @@
       <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6844,7 +6850,7 @@
         <v>11</v>
       </c>
       <c r="AA16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
@@ -6864,10 +6870,10 @@
         <v>92</v>
       </c>
       <c r="Z17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AA17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
@@ -6887,10 +6893,10 @@
         <v>50</v>
       </c>
       <c r="Z18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AA18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Pulse Working well, Don't use Timer 1 channel 1 don't xorking in debug Mode
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32G474RE/STM32G474RE_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\f_debugCL42T\Doc\ConfigPrj\ExcelCfg\STM32G474RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837F6EA8-C6C7-4A7C-962B-E1A27BD99F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F3F433-34F5-4C18-84B3-6F13E4CA76C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="441">
   <si>
     <t>Colonne1</t>
   </si>
@@ -384,9 +384,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>PC15, PC14, PF0, PF1  are forbidden</t>
-  </si>
-  <si>
     <t>TS_CAL1</t>
   </si>
   <si>
@@ -1362,7 +1359,13 @@
     <t>EXTI9_5_IRQN</t>
   </si>
   <si>
-    <t>JTAG User -&gt; PA14/PA13</t>
+    <t>JTAG User -&gt; PA14/PA13, PA15, PC1, PC0</t>
+  </si>
+  <si>
+    <t>GPIO_AF6_TIM1</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -3805,8 +3808,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="Z7:AA18" totalsRowShown="0">
-  <autoFilter ref="Z7:AA18" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="Z7:AA16" totalsRowShown="0">
+  <autoFilter ref="Z7:AA16" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{395BD36A-0840-48CF-8D8D-56878E366FC5}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{34DF2CF3-8826-4F9E-A09D-280EE0FEFFBB}" name="Pin_name"/>
@@ -4468,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A18:AF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="H15" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -4500,16 +4503,16 @@
   <sheetData>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -4524,27 +4527,27 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
+        <v>269</v>
+      </c>
+      <c r="N18" t="s">
         <v>270</v>
       </c>
-      <c r="N18" t="s">
-        <v>271</v>
-      </c>
       <c r="O18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -4559,45 +4562,45 @@
         <v>4</v>
       </c>
       <c r="M19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I20" t="s">
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L20">
         <v>4</v>
       </c>
       <c r="M20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T20" t="s">
         <v>17</v>
@@ -4606,10 +4609,10 @@
         <v>18</v>
       </c>
       <c r="V20" t="s">
+        <v>275</v>
+      </c>
+      <c r="W20" t="s">
         <v>276</v>
-      </c>
-      <c r="W20" t="s">
-        <v>277</v>
       </c>
       <c r="AB20" t="s">
         <v>22</v>
@@ -4618,21 +4621,21 @@
         <v>18</v>
       </c>
       <c r="AD20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I21" t="s">
         <v>69</v>
@@ -4647,10 +4650,10 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T21" t="s">
         <v>16</v>
@@ -4659,13 +4662,13 @@
         <v>18</v>
       </c>
       <c r="V21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AB21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AC21">
         <v>8</v>
@@ -4676,66 +4679,66 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I22" t="s">
         <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L22">
         <v>4</v>
       </c>
       <c r="M22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U22">
         <v>18</v>
       </c>
       <c r="V22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AB22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AC22">
         <v>8</v>
       </c>
       <c r="AD22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
@@ -4744,42 +4747,42 @@
         <v>69</v>
       </c>
       <c r="K23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L23">
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U23">
         <v>18</v>
       </c>
       <c r="V23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H24" t="s">
         <v>61</v>
@@ -4788,31 +4791,31 @@
         <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U24">
         <v>18</v>
       </c>
       <c r="V24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
@@ -4820,95 +4823,95 @@
         <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I25" t="s">
         <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="T25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U25">
         <v>18</v>
       </c>
       <c r="V25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I26" t="s">
         <v>69</v>
       </c>
       <c r="K26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L26">
         <v>4</v>
       </c>
       <c r="M26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I27" t="s">
         <v>69</v>
@@ -4920,33 +4923,33 @@
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28">
         <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I28" t="s">
         <v>69</v>
@@ -4958,33 +4961,33 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B29">
         <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I29" t="s">
         <v>69</v>
@@ -4996,13 +4999,13 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -5010,10 +5013,10 @@
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -5022,19 +5025,19 @@
         <v>69</v>
       </c>
       <c r="K30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L30">
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -5042,13 +5045,13 @@
         <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I31" t="s">
         <v>69</v>
@@ -5059,13 +5062,13 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" t="s">
         <v>69</v>
@@ -5073,16 +5076,16 @@
     </row>
     <row r="33" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I33" t="s">
         <v>69</v>
@@ -5096,16 +5099,16 @@
     </row>
     <row r="34" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I34" t="s">
         <v>69</v>
@@ -5119,16 +5122,16 @@
     </row>
     <row r="35" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I35" t="s">
         <v>69</v>
@@ -5142,16 +5145,16 @@
     </row>
     <row r="36" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F36" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I36" t="s">
         <v>69</v>
@@ -5171,16 +5174,16 @@
     </row>
     <row r="37" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I37" t="s">
         <v>69</v>
@@ -5200,22 +5203,22 @@
     </row>
     <row r="38" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F38" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I38" t="s">
         <v>69</v>
       </c>
       <c r="P38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q38">
         <v>16</v>
@@ -5223,16 +5226,16 @@
     </row>
     <row r="39" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F39" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I39" t="s">
         <v>69</v>
@@ -5246,22 +5249,22 @@
     </row>
     <row r="40" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I40" t="s">
         <v>90</v>
       </c>
       <c r="P40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q40">
         <v>11</v>
@@ -5272,16 +5275,16 @@
     </row>
     <row r="41" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F41" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I41" t="s">
         <v>90</v>
@@ -5292,16 +5295,16 @@
     </row>
     <row r="42" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I42" t="s">
         <v>69</v>
@@ -5315,13 +5318,13 @@
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F43" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I43" t="s">
         <v>69</v>
@@ -5332,16 +5335,16 @@
     </row>
     <row r="44" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I44" t="s">
         <v>69</v>
@@ -5349,16 +5352,16 @@
     </row>
     <row r="45" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F45" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I45" t="s">
         <v>69</v>
@@ -5366,13 +5369,13 @@
     </row>
     <row r="46" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -5381,38 +5384,38 @@
         <v>69</v>
       </c>
       <c r="AF46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I47" t="s">
         <v>69</v>
       </c>
       <c r="AF47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H48" t="s">
         <v>64</v>
@@ -5421,27 +5424,27 @@
         <v>69</v>
       </c>
       <c r="AF48" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F49" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I49" t="s">
         <v>69</v>
       </c>
       <c r="AF49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="4:32" x14ac:dyDescent="0.3">
@@ -5449,13 +5452,13 @@
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F50" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I50" t="s">
         <v>69</v>
@@ -5466,13 +5469,13 @@
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F51" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I51" t="s">
         <v>69</v>
@@ -5480,22 +5483,22 @@
     </row>
     <row r="52" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E52" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F52" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I52" t="s">
         <v>69</v>
       </c>
       <c r="AF52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="4:32" x14ac:dyDescent="0.3">
@@ -5503,30 +5506,30 @@
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F53" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I53" t="s">
         <v>69</v>
       </c>
       <c r="AF53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="54" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F54" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H54" t="s">
         <v>65</v>
@@ -5535,18 +5538,18 @@
         <v>69</v>
       </c>
       <c r="AF54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="55" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F55" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H55" t="s">
         <v>66</v>
@@ -5555,18 +5558,18 @@
         <v>69</v>
       </c>
       <c r="AF55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F56" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H56" t="s">
         <v>67</v>
@@ -5575,18 +5578,18 @@
         <v>69</v>
       </c>
       <c r="AF56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F57" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H57" t="s">
         <v>68</v>
@@ -5595,47 +5598,47 @@
         <v>69</v>
       </c>
       <c r="AF57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E58" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F58" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I58" t="s">
         <v>69</v>
       </c>
       <c r="AF58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E59" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F59" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H59" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I59" t="s">
         <v>69</v>
       </c>
       <c r="AF59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="4:32" x14ac:dyDescent="0.3">
@@ -5643,73 +5646,73 @@
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F60" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I60" t="s">
         <v>69</v>
       </c>
       <c r="AF60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F61" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I61" t="s">
         <v>69</v>
       </c>
       <c r="AF61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E62" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F62" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I62" t="s">
         <v>69</v>
       </c>
       <c r="AF62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F63" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I63" t="s">
         <v>69</v>
@@ -5720,13 +5723,13 @@
         <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I64" t="s">
         <v>69</v>
@@ -5737,13 +5740,13 @@
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F65" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I65" t="s">
         <v>69</v>
@@ -5754,13 +5757,13 @@
         <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F66" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I66" t="s">
         <v>69</v>
@@ -5768,16 +5771,16 @@
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E67" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F67" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I67" t="s">
         <v>69</v>
@@ -5788,13 +5791,13 @@
         <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F68" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I68" t="s">
         <v>69</v>
@@ -5802,16 +5805,16 @@
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F69" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I69" t="s">
         <v>69</v>
@@ -5822,13 +5825,13 @@
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F70" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I70" t="s">
         <v>69</v>
@@ -5839,13 +5842,13 @@
         <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F71" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H71" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I71" t="s">
         <v>69</v>
@@ -5856,13 +5859,13 @@
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F72" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I72" t="s">
         <v>69</v>
@@ -5870,16 +5873,16 @@
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F73" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I73" t="s">
         <v>69</v>
@@ -5887,16 +5890,16 @@
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F74" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I74" t="s">
         <v>69</v>
@@ -5904,16 +5907,16 @@
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E75" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F75" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H75" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I75" t="s">
         <v>69</v>
@@ -5921,7 +5924,7 @@
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I76" t="s">
         <v>69</v>
@@ -5929,7 +5932,7 @@
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I77" t="s">
         <v>69</v>
@@ -5937,7 +5940,7 @@
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I78" t="s">
         <v>69</v>
@@ -5945,7 +5948,7 @@
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H79" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I79" t="s">
         <v>69</v>
@@ -5953,7 +5956,7 @@
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I80" t="s">
         <v>69</v>
@@ -5961,7 +5964,7 @@
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I81" t="s">
         <v>69</v>
@@ -5969,7 +5972,7 @@
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I82" t="s">
         <v>69</v>
@@ -5977,7 +5980,7 @@
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I83" t="s">
         <v>69</v>
@@ -5985,7 +5988,7 @@
     </row>
     <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I84" t="s">
         <v>69</v>
@@ -5993,7 +5996,7 @@
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I85" t="s">
         <v>69</v>
@@ -6001,7 +6004,7 @@
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I86" t="s">
         <v>69</v>
@@ -6009,7 +6012,7 @@
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I87" t="s">
         <v>69</v>
@@ -6017,7 +6020,7 @@
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I88" t="s">
         <v>69</v>
@@ -6025,7 +6028,7 @@
     </row>
     <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I89" t="s">
         <v>69</v>
@@ -6033,7 +6036,7 @@
     </row>
     <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I90" t="s">
         <v>69</v>
@@ -6041,7 +6044,7 @@
     </row>
     <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I91" t="s">
         <v>69</v>
@@ -6049,7 +6052,7 @@
     </row>
     <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H92" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I92" t="s">
         <v>69</v>
@@ -6057,7 +6060,7 @@
     </row>
     <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H93" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I93" t="s">
         <v>69</v>
@@ -6065,7 +6068,7 @@
     </row>
     <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I94" t="s">
         <v>69</v>
@@ -6073,7 +6076,7 @@
     </row>
     <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H95" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I95" t="s">
         <v>69</v>
@@ -6081,7 +6084,7 @@
     </row>
     <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H96" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I96" t="s">
         <v>69</v>
@@ -6089,7 +6092,7 @@
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H97" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I97" t="s">
         <v>69</v>
@@ -6097,7 +6100,7 @@
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H98" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I98" t="s">
         <v>69</v>
@@ -6105,7 +6108,7 @@
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I99" t="s">
         <v>69</v>
@@ -6113,7 +6116,7 @@
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H100" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I100" t="s">
         <v>69</v>
@@ -6121,7 +6124,7 @@
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H101" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I101" t="s">
         <v>69</v>
@@ -6129,7 +6132,7 @@
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H102" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I102" t="s">
         <v>69</v>
@@ -6137,7 +6140,7 @@
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H103" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I103" t="s">
         <v>69</v>
@@ -6145,7 +6148,7 @@
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H104" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I104" t="s">
         <v>90</v>
@@ -6153,7 +6156,7 @@
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I105" t="s">
         <v>90</v>
@@ -6161,7 +6164,7 @@
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H106" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I106" t="s">
         <v>90</v>
@@ -6169,7 +6172,7 @@
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H107" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I107" t="s">
         <v>90</v>
@@ -6177,7 +6180,7 @@
     </row>
     <row r="108" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I108" t="s">
         <v>69</v>
@@ -6185,7 +6188,7 @@
     </row>
     <row r="109" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H109" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I109" t="s">
         <v>69</v>
@@ -6193,7 +6196,7 @@
     </row>
     <row r="110" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I110" t="s">
         <v>69</v>
@@ -6201,7 +6204,7 @@
     </row>
     <row r="111" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I111" t="s">
         <v>69</v>
@@ -6209,7 +6212,7 @@
     </row>
     <row r="112" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H112" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I112" t="s">
         <v>69</v>
@@ -6217,7 +6220,7 @@
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H113" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I113" t="s">
         <v>69</v>
@@ -6225,7 +6228,7 @@
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H114" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I114" t="s">
         <v>69</v>
@@ -6233,7 +6236,7 @@
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H115" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I115" t="s">
         <v>69</v>
@@ -6241,7 +6244,7 @@
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H116" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I116" t="s">
         <v>69</v>
@@ -6249,7 +6252,7 @@
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H117" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I117" t="s">
         <v>69</v>
@@ -6257,7 +6260,7 @@
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I118" t="s">
         <v>69</v>
@@ -6265,7 +6268,7 @@
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H119" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I119" t="s">
         <v>69</v>
@@ -6310,8 +6313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A2:BA57"/>
   <sheetViews>
-    <sheetView topLeftCell="S2" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6346,10 +6349,10 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>440</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -6363,13 +6366,13 @@
         <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P5" t="s">
         <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="V5" t="s">
         <v>55</v>
@@ -6451,7 +6454,7 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H7" t="s">
         <v>111</v>
@@ -6463,7 +6466,7 @@
         <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M7" t="s">
         <v>5</v>
@@ -6472,19 +6475,19 @@
         <v>92</v>
       </c>
       <c r="P7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="R7" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="S7" t="s">
         <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="V7" t="s">
         <v>12</v>
@@ -6493,7 +6496,7 @@
         <v>27</v>
       </c>
       <c r="X7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Z7" t="s">
         <v>23</v>
@@ -6516,7 +6519,7 @@
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H8" t="s">
         <v>107</v>
@@ -6528,7 +6531,7 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
@@ -6537,28 +6540,28 @@
         <v>50</v>
       </c>
       <c r="P8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="R8" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="S8" t="s">
         <v>4</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="V8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="W8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="X8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Z8" t="s">
         <v>12</v>
@@ -6581,7 +6584,7 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H9" t="s">
         <v>97</v>
@@ -6593,7 +6596,7 @@
         <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
@@ -6608,10 +6611,10 @@
         <v>27</v>
       </c>
       <c r="R9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T9" t="s">
         <v>46</v>
@@ -6637,7 +6640,7 @@
         <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H10" t="s">
         <v>98</v>
@@ -6649,7 +6652,7 @@
         <v>29</v>
       </c>
       <c r="L10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M10" t="s">
         <v>5</v>
@@ -6664,7 +6667,7 @@
         <v>28</v>
       </c>
       <c r="R10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="S10" t="s">
         <v>4</v>
@@ -6693,7 +6696,7 @@
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H11" t="s">
         <v>109</v>
@@ -6705,10 +6708,10 @@
         <v>31</v>
       </c>
       <c r="R11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T11" t="s">
         <v>45</v>
@@ -6734,10 +6737,10 @@
         <v>32</v>
       </c>
       <c r="R12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T12" t="s">
         <v>46</v>
@@ -6763,10 +6766,10 @@
         <v>33</v>
       </c>
       <c r="R13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T13" t="s">
         <v>92</v>
@@ -6775,7 +6778,7 @@
         <v>11</v>
       </c>
       <c r="AA13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
@@ -6792,10 +6795,10 @@
         <v>34</v>
       </c>
       <c r="R14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T14" t="s">
         <v>50</v>
@@ -6815,10 +6818,10 @@
         <v>31</v>
       </c>
       <c r="R15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T15" t="s">
         <v>45</v>
@@ -6838,19 +6841,19 @@
         <v>32</v>
       </c>
       <c r="R16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T16" t="s">
         <v>46</v>
       </c>
       <c r="Z16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AA16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
@@ -6861,19 +6864,13 @@
         <v>33</v>
       </c>
       <c r="R17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T17" t="s">
         <v>92</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
@@ -6884,44 +6881,38 @@
         <v>34</v>
       </c>
       <c r="R18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T18" t="s">
         <v>50</v>
       </c>
-      <c r="Z18" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" t="s">
         <v>286</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>287</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>288</v>
-      </c>
-      <c r="D25" t="s">
-        <v>289</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.3">
@@ -6938,58 +6929,58 @@
         <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
       <c r="W29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AW29" t="s">
         <v>91</v>
@@ -7000,7 +6991,7 @@
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.3">
       <c r="W30" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AW30" t="s">
         <v>25</v>
@@ -7014,7 +7005,7 @@
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.3">
       <c r="W31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AW31" t="s">
         <v>26</v>
@@ -7028,7 +7019,7 @@
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.3">
       <c r="W32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AW32" t="s">
         <v>27</v>
@@ -7042,10 +7033,10 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="W33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AW33" t="s">
         <v>28</v>
@@ -7059,25 +7050,25 @@
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B34" t="s">
         <v>286</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>287</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>288</v>
-      </c>
-      <c r="D34" t="s">
-        <v>289</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W34" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AW34" t="s">
         <v>29</v>
@@ -7103,13 +7094,13 @@
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
       </c>
       <c r="W35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AW35" t="s">
         <v>30</v>
@@ -7132,13 +7123,13 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="W36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AW36" t="s">
         <v>31</v>
@@ -7237,7 +7228,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 K7:K10 Q7:Q14 F7:F11 B7:B14 W7:W8 AA8:AA18" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW46 K7:K10 Q7:Q14 F7:F11 B7:B14 W7:W8 AA8:AA16" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
       <formula1>$AW$30:$AW$45</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:T14 N7:N10" xr:uid="{727A5344-B28A-4866-9EC1-7C96029AF8B6}">
@@ -7270,7 +7261,7 @@
           <x14:formula1>
             <xm:f>General_Info!$P$34:$P$39</xm:f>
           </x14:formula1>
-          <xm:sqref>P7:P14 J7:J10 E7:E11 A7:A14 V7:V8 Z8:Z18</xm:sqref>
+          <xm:sqref>P7:P14 J7:J10 E7:E11 A7:A14 V7:V8 Z8:Z16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C428027-B16D-4B04-9CB2-8290577ED0FB}">
           <x14:formula1>
@@ -7311,7 +7302,7 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -7322,10 +7313,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -7336,7 +7327,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -7350,7 +7341,7 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -7358,7 +7349,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -7366,7 +7357,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -7374,15 +7365,15 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -7390,58 +7381,58 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -7479,44 +7470,44 @@
   <sheetData>
     <row r="2" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S3" t="s">
+        <v>116</v>
+      </c>
+      <c r="T3" t="s">
         <v>121</v>
       </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
+        <v>118</v>
+      </c>
+      <c r="V3" t="s">
         <v>119</v>
-      </c>
-      <c r="L3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S3" t="s">
-        <v>117</v>
-      </c>
-      <c r="T3" t="s">
-        <v>122</v>
-      </c>
-      <c r="U3" t="s">
-        <v>119</v>
-      </c>
-      <c r="V3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -7525,10 +7516,10 @@
         <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U4" t="s">
         <v>16</v>
@@ -7539,22 +7530,22 @@
     </row>
     <row r="5" spans="5:22" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L5" t="s">
         <v>98</v>
       </c>
       <c r="S5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U5" t="s">
         <v>16</v>
@@ -7565,13 +7556,13 @@
     </row>
     <row r="6" spans="5:22" x14ac:dyDescent="0.3">
       <c r="S6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="V6" t="s">
         <v>111</v>
@@ -7579,16 +7570,16 @@
     </row>
     <row r="7" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V7" t="s">
         <v>111</v>
@@ -7596,19 +7587,19 @@
     </row>
     <row r="8" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="V8" t="s">
         <v>111</v>
@@ -7616,34 +7607,34 @@
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -7695,50 +7686,50 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
         <v>335</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>336</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>337</v>
       </c>
-      <c r="E2" t="s">
-        <v>338</v>
-      </c>
       <c r="J2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" t="s">
         <v>332</v>
       </c>
-      <c r="C3" t="s">
-        <v>333</v>
-      </c>
       <c r="D3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="P3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -7747,24 +7738,24 @@
         <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="P4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D5" t="s">
         <v>92</v>
@@ -7773,18 +7764,18 @@
         <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -7793,18 +7784,18 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -7813,58 +7804,58 @@
         <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" t="s">
         <v>342</v>
-      </c>
-      <c r="C8" t="s">
-        <v>333</v>
-      </c>
-      <c r="D8" t="s">
-        <v>343</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" t="s">
         <v>344</v>
-      </c>
-      <c r="C9" t="s">
-        <v>333</v>
-      </c>
-      <c r="D9" t="s">
-        <v>345</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -7873,18 +7864,18 @@
         <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -7893,18 +7884,18 @@
         <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D12" t="s">
         <v>92</v>
@@ -7913,43 +7904,43 @@
         <v>69</v>
       </c>
       <c r="J12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -7974,47 +7965,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -8049,28 +8040,28 @@
   <sheetData>
     <row r="2" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H2" t="s">
         <v>420</v>
       </c>
-      <c r="H2" t="s">
-        <v>421</v>
-      </c>
       <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J2" t="s">
         <v>286</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>287</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>288</v>
-      </c>
-      <c r="L2" t="s">
-        <v>289</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
@@ -8081,7 +8072,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -8090,19 +8081,19 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J3" t="s">
         <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="5:13" x14ac:dyDescent="0.3">
@@ -8110,7 +8101,7 @@
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G4">
         <v>256</v>
@@ -8131,38 +8122,38 @@
         <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G6">
         <v>256</v>
@@ -8171,27 +8162,27 @@
         <v>256</v>
       </c>
       <c r="I6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J6" t="s">
         <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -8200,19 +8191,19 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L7" t="s">
         <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -8244,7 +8235,7 @@
   <sheetData>
     <row r="1" spans="3:14" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D1" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
@@ -8254,10 +8245,10 @@
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -8270,19 +8261,19 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J7" t="s">
         <v>310</v>
-      </c>
-      <c r="E7" t="s">
-        <v>309</v>
-      </c>
-      <c r="F7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G7" t="s">
-        <v>308</v>
-      </c>
-      <c r="J7" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -8304,7 +8295,7 @@
         <v>6000.2906390778307</v>
       </c>
       <c r="M8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -8315,7 +8306,7 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -8324,7 +8315,7 @@
         <v>35.998312579097856</v>
       </c>
       <c r="J13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L13">
         <f>L5+(L5/J15)*M9</f>
@@ -8354,10 +8345,10 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -8392,15 +8383,15 @@
     </row>
     <row r="27" spans="2:16" ht="93.6" x14ac:dyDescent="1.75">
       <c r="D27" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -8412,39 +8403,39 @@
         <v>0.5</v>
       </c>
       <c r="M29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
+        <v>320</v>
+      </c>
+      <c r="E30" t="s">
         <v>321</v>
       </c>
-      <c r="E30" t="s">
-        <v>322</v>
-      </c>
       <c r="F30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I30" t="s">
+        <v>327</v>
+      </c>
+      <c r="J30" t="s">
+        <v>325</v>
+      </c>
+      <c r="K30" t="s">
         <v>328</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
+        <v>329</v>
+      </c>
+      <c r="M30" t="s">
         <v>326</v>
       </c>
-      <c r="K30" t="s">
-        <v>329</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>330</v>
-      </c>
-      <c r="M30" t="s">
-        <v>327</v>
-      </c>
-      <c r="O30" t="s">
-        <v>331</v>
       </c>
       <c r="P30" t="e">
         <f>2^#REF!</f>

</xml_diff>